<commit_message>
Adds card and mage descriptions to the data.
</commit_message>
<xml_diff>
--- a/lib/seeds/Aeon's End Database.xlsx
+++ b/lib/seeds/Aeon's End Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="282">
   <si>
     <t>Name</t>
   </si>
@@ -33,222 +33,337 @@
     <t>Image Name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Ability</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Adelheim</t>
+  </si>
+  <si>
+    <t>Adelheim.jpg</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during the nemesis draw phase: 
+When a nemesis attack or power card is drawn but before it is resolved, you may discard it. It has no effect.</t>
+  </si>
+  <si>
+    <t>Brama</t>
+  </si>
+  <si>
+    <t>Brama.jpg</t>
+  </si>
+  <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Any player gains 4 life.</t>
+  </si>
+  <si>
+    <t>Dezmodia</t>
+  </si>
+  <si>
+    <t>Dezmodia.jpg</t>
+  </si>
+  <si>
+    <t>Amethyst Shard</t>
+  </si>
+  <si>
+    <t>Cost: 6 Charges.
+Activate during your main phase:
+Any player destroys an opened I or II breach and returns any spells to their hand. That player gains a Sigil breach and places it where the destroyed breach was. Then, that player may prep a spell from their hand to a breach.</t>
+  </si>
+  <si>
+    <t>Garu</t>
+  </si>
+  <si>
+    <t>Garu.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Discard up to 4 of your prepped spells.
+Deal 2 damage plus 4 additional damage for each spell you discarded divided however you choose to the nemesis or any number of minions</t>
+  </si>
+  <si>
+    <t>Gex</t>
+  </si>
+  <si>
+    <t>Buried Light</t>
+  </si>
+  <si>
+    <t>Gex.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Destroy up to two cards in your discard pile that cost 0 Aether.
+Any ally draws one card and gains 2 life.</t>
+  </si>
+  <si>
+    <t>Jian</t>
+  </si>
+  <si>
+    <t>Jian.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 4 Charges.
+Activate during your main phase:
+Cast any player's prepped spell without discarding it.
+Then cast that prepped spell again.</t>
+  </si>
+  <si>
     <t>Amplify Vision</t>
   </si>
   <si>
+    <t>Kadir</t>
+  </si>
+  <si>
+    <t>Kadir.jpg</t>
+  </si>
+  <si>
+    <t>Oblivion Shard</t>
+  </si>
+  <si>
     <t>Spell</t>
   </si>
   <si>
+    <t>Cost: 5 Charges.
+Activate during any player's main phase:
+That player may return up to three spells in their discard pile to their hand. That player may prep up to two spells to each of their opened breaches this turn.</t>
+  </si>
+  <si>
     <t>Market</t>
   </si>
   <si>
+    <t>Lash</t>
+  </si>
+  <si>
     <t>AmplifyVision.jpg</t>
   </si>
   <si>
-    <t>Mage</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Adelheim</t>
-  </si>
-  <si>
-    <t>Crystal</t>
+    <t>Lash.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 6 Charges.
+Activate during any player's main phase:
+Shuffle any player's turn order card into the turn order deck. That player suffers 1 damage.</t>
+  </si>
+  <si>
+    <t>Mazahaedron</t>
+  </si>
+  <si>
+    <t>Mazahaedron.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 4 Charges.
+Activate during your main phase:
+You may gain a gem that costs 4 Aether or less from any supply pile.
+Gravehold gains 4 life.</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Mist (Dagger Captain)</t>
+  </si>
+  <si>
+    <t>Mist.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Any ally draws 4 cards.</t>
+  </si>
+  <si>
+    <t>Mist (Voidwalker)</t>
+  </si>
+  <si>
+    <t>MistWE.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 6 Charges.
+Activate during your main phase:
+Cast up to three different spells prepped by any number of players. For each spell cast this way, place that spell into any ally's hand.</t>
   </si>
   <si>
     <t>Arcane Nexus</t>
   </si>
   <si>
-    <t>Spark</t>
-  </si>
-  <si>
-    <t>Adelheim.jpg</t>
-  </si>
-  <si>
-    <t>Brama</t>
-  </si>
-  <si>
-    <t>Amethyst Shard</t>
-  </si>
-  <si>
-    <t>Brama.jpg</t>
-  </si>
-  <si>
-    <t>Dezmodia</t>
-  </si>
-  <si>
-    <t>Dezmodia.jpg</t>
-  </si>
-  <si>
-    <t>Garu</t>
-  </si>
-  <si>
-    <t>Garu.jpg</t>
-  </si>
-  <si>
-    <t>Gex</t>
+    <t>Nym</t>
+  </si>
+  <si>
+    <t>Nym.jpg</t>
+  </si>
+  <si>
+    <t>Shattered Geode</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Discard the top card of the nemesis deck.
+If you discarded an attack card, discard an additional card.</t>
   </si>
   <si>
     <t>ArcaneNexus.jpg</t>
   </si>
   <si>
-    <t>Gex.jpg</t>
-  </si>
-  <si>
-    <t>Buried Light</t>
+    <t>Phaedraxa</t>
   </si>
   <si>
     <t>Aurora</t>
   </si>
   <si>
-    <t>Jian</t>
-  </si>
-  <si>
-    <t>Jian.jpg</t>
+    <t>Phaedraxa.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate immediately after a turn order card is drawn:
+Prevent any damage that the players or Gravehold would suffer during that turn.</t>
   </si>
   <si>
     <t>Aurora.jpg</t>
   </si>
   <si>
-    <t>Kadir</t>
+    <t>Quilius</t>
   </si>
   <si>
     <t>Banishing Topaz</t>
   </si>
   <si>
-    <t>Kadir.jpg</t>
-  </si>
-  <si>
-    <t>Lash</t>
-  </si>
-  <si>
-    <t>Lash.jpg</t>
+    <t>Quilius.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Deal 2 damage for each Trophy token you have.</t>
   </si>
   <si>
     <t>Gem</t>
   </si>
   <si>
-    <t>Mazahaedron</t>
-  </si>
-  <si>
-    <t>Oblivion Shard</t>
-  </si>
-  <si>
-    <t>Mazahaedron.jpg</t>
+    <t>Reeve</t>
+  </si>
+  <si>
+    <t>Reeve.jpg</t>
   </si>
   <si>
     <t>BanishingTopaz.jpg</t>
   </si>
   <si>
-    <t>Mist (Dagger Captain)</t>
+    <t>Cost: 4 Charges.
+Activate during your main phase:
+Deal 5 damage to a minion.
+Deal 3 damage to a different minion.</t>
   </si>
   <si>
     <t>Blasting Staff</t>
   </si>
   <si>
-    <t>Mist.jpg</t>
-  </si>
-  <si>
-    <t>Mist (Voidwalker)</t>
+    <t>Ulgimor</t>
+  </si>
+  <si>
+    <t>Ulgimor.jpg</t>
   </si>
   <si>
     <t>Relic</t>
   </si>
   <si>
-    <t>MistWE.jpg</t>
+    <t>Moonstone Shard</t>
+  </si>
+  <si>
+    <t>Cost: 6 Charges.
+Activate during your main phase:
+Gain 6 life.
+If you are exhausted, any ally gains 5 life instead.</t>
   </si>
   <si>
     <t>BlastingStaff.jpg</t>
   </si>
   <si>
-    <t>Nym</t>
-  </si>
-  <si>
-    <t>Nym.jpg</t>
+    <t>Xaxos</t>
   </si>
   <si>
     <t>Bloodstone Jewel</t>
   </si>
   <si>
-    <t>Torch</t>
-  </si>
-  <si>
-    <t>Phaedraxa</t>
-  </si>
-  <si>
-    <t>Phaedraxa.jpg</t>
-  </si>
-  <si>
-    <t>Quilius</t>
+    <t>Xaxos.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during any player's main phase:
+Allies collectively gain 4 charges.
+Reveal the turn order deck and return the revealed cards in any order.</t>
   </si>
   <si>
     <t>BloodstoneJewel.jpg</t>
   </si>
   <si>
-    <t>Quilius.jpg</t>
+    <t>Yan Magda</t>
   </si>
   <si>
     <t>Bottled Vortex</t>
   </si>
   <si>
-    <t>Reeve</t>
-  </si>
-  <si>
-    <t>Reeve.jpg</t>
+    <t>YanMagda.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
   </si>
   <si>
     <t>BottledVortex.jpg</t>
   </si>
   <si>
-    <t>Ulgimor</t>
-  </si>
-  <si>
-    <t>Ulgimor.jpg</t>
-  </si>
-  <si>
-    <t>Shattered Geode</t>
+    <t>Emerald Shard</t>
+  </si>
+  <si>
+    <t>Z'hana</t>
   </si>
   <si>
     <t>Breach Ore</t>
   </si>
   <si>
-    <t>Xaxos</t>
-  </si>
-  <si>
-    <t>Xaxos.jpg</t>
+    <t>Zhana.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Gravehold gains 7 life.</t>
   </si>
   <si>
     <t>BreachOre.jpg</t>
   </si>
   <si>
-    <t>Yan Magda</t>
-  </si>
-  <si>
-    <t>YanMagda.jpg</t>
-  </si>
-  <si>
     <t>Burning Opal</t>
   </si>
   <si>
-    <t>Z'hana</t>
-  </si>
-  <si>
-    <t>Zhana.jpg</t>
-  </si>
-  <si>
     <t>BurningOpal.jpg</t>
   </si>
   <si>
-    <t>Moonstone Shard</t>
-  </si>
-  <si>
     <t>Cairn Compass</t>
   </si>
   <si>
+    <t>Quartz Shard</t>
+  </si>
+  <si>
     <t>CairnCompass.jpg</t>
   </si>
   <si>
@@ -261,7 +376,7 @@
     <t>Celestial Spire</t>
   </si>
   <si>
-    <t>Emerald Shard</t>
+    <t>Worldheart Shard</t>
   </si>
   <si>
     <t>CelestialSpire.jpg</t>
@@ -276,7 +391,7 @@
     <t>Clouded Sapphire</t>
   </si>
   <si>
-    <t>Quartz Shard</t>
+    <t>Garnet Shard</t>
   </si>
   <si>
     <t>CloudedSapphire.jpg</t>
@@ -285,9 +400,6 @@
     <t>Combustion</t>
   </si>
   <si>
-    <t>Worldheart Shard</t>
-  </si>
-  <si>
     <t>Combustion.jpg</t>
   </si>
   <si>
@@ -300,9 +412,6 @@
     <t>Conjure The Lost</t>
   </si>
   <si>
-    <t>Garnet Shard</t>
-  </si>
-  <si>
     <t>ConjureTheLost.jpg</t>
   </si>
   <si>
@@ -315,177 +424,177 @@
     <t>Convection Field</t>
   </si>
   <si>
+    <t>ConvectionField.jpg</t>
+  </si>
+  <si>
+    <t>Crystallize</t>
+  </si>
+  <si>
+    <t>Crystallize.jpg</t>
+  </si>
+  <si>
+    <t>Dark Fire</t>
+  </si>
+  <si>
+    <t>DarkFire.jpg</t>
+  </si>
+  <si>
+    <t>Devouring Shadow</t>
+  </si>
+  <si>
+    <t>DevouringShadow.jpg</t>
+  </si>
+  <si>
+    <t>Diamond Cluster</t>
+  </si>
+  <si>
+    <t>DiamondCluster.jpg</t>
+  </si>
+  <si>
+    <t>Disintegrating Scythe</t>
+  </si>
+  <si>
+    <t>DisintegratingScythe.jpg</t>
+  </si>
+  <si>
+    <t>Dread Diamond</t>
+  </si>
+  <si>
+    <t>DreadDiamond.jpg</t>
+  </si>
+  <si>
+    <t>Equilibrium</t>
+  </si>
+  <si>
+    <t>Equilibrium.jpg</t>
+  </si>
+  <si>
+    <t>Erratic Ingot</t>
+  </si>
+  <si>
+    <t>ErraticIngot.jpg</t>
+  </si>
+  <si>
+    <t>Essence Theft</t>
+  </si>
+  <si>
+    <t>EssenceTheft.jpg</t>
+  </si>
+  <si>
+    <t>Feral Lightning</t>
+  </si>
+  <si>
     <t>Amethyst Paragon</t>
   </si>
   <si>
-    <t>ConvectionField.jpg</t>
-  </si>
-  <si>
-    <t>Crystallize</t>
-  </si>
-  <si>
-    <t>Crystallize.jpg</t>
-  </si>
-  <si>
-    <t>Dark Fire</t>
+    <t>FeralLightning.jpg</t>
+  </si>
+  <si>
+    <t>Fiend Catcher</t>
+  </si>
+  <si>
+    <t>FiendCatcher.jpg</t>
   </si>
   <si>
     <t>Cinder</t>
   </si>
   <si>
-    <t>DarkFire.jpg</t>
-  </si>
-  <si>
-    <t>Devouring Shadow</t>
-  </si>
-  <si>
-    <t>DevouringShadow.jpg</t>
-  </si>
-  <si>
-    <t>Diamond Cluster</t>
+    <t>Fiery Torrent</t>
+  </si>
+  <si>
+    <t>FieryTorrent.jpg</t>
+  </si>
+  <si>
+    <t>Flexing Dagger</t>
   </si>
   <si>
     <t>Tourmaline Shard</t>
   </si>
   <si>
-    <t>DiamondCluster.jpg</t>
-  </si>
-  <si>
-    <t>Disintegrating Scythe</t>
-  </si>
-  <si>
-    <t>DisintegratingScythe.jpg</t>
-  </si>
-  <si>
-    <t>Dread Diamond</t>
+    <t>FlexingDagger.jpg</t>
+  </si>
+  <si>
+    <t>Focusing Orb</t>
+  </si>
+  <si>
+    <t>FocusingOrb.jpg</t>
+  </si>
+  <si>
+    <t>Frozen Magmite</t>
+  </si>
+  <si>
+    <t>FrozenMagmite.jpg</t>
   </si>
   <si>
     <t>Extinguish</t>
   </si>
   <si>
-    <t>DreadDiamond.jpg</t>
-  </si>
-  <si>
-    <t>Equilibrium</t>
-  </si>
-  <si>
-    <t>Equilibrium.jpg</t>
-  </si>
-  <si>
-    <t>Erratic Ingot</t>
-  </si>
-  <si>
-    <t>ErraticIngot.jpg</t>
-  </si>
-  <si>
-    <t>Essence Theft</t>
+    <t>Ignite</t>
+  </si>
+  <si>
+    <t>Ignite.jpg</t>
+  </si>
+  <si>
+    <t>Jade</t>
   </si>
   <si>
     <t>Obsidian Shard</t>
   </si>
   <si>
-    <t>EssenceTheft.jpg</t>
-  </si>
-  <si>
-    <t>Feral Lightning</t>
-  </si>
-  <si>
-    <t>FeralLightning.jpg</t>
-  </si>
-  <si>
-    <t>Fiend Catcher</t>
+    <t>Jade.jpg</t>
+  </si>
+  <si>
+    <t>Jagged Lightning</t>
+  </si>
+  <si>
+    <t>JaggedLightning.jpg</t>
+  </si>
+  <si>
+    <t>Kindle</t>
   </si>
   <si>
     <t>Coal Shard</t>
   </si>
   <si>
-    <t>FiendCatcher.jpg</t>
-  </si>
-  <si>
-    <t>Fiery Torrent</t>
-  </si>
-  <si>
-    <t>FieryTorrent.jpg</t>
-  </si>
-  <si>
-    <t>Flexing Dagger</t>
+    <t>Kindle.jpg</t>
+  </si>
+  <si>
+    <t>Lava Tendril</t>
+  </si>
+  <si>
+    <t>LavaTendril.jpg</t>
   </si>
   <si>
     <t>Flare</t>
   </si>
   <si>
-    <t>FlexingDagger.jpg</t>
-  </si>
-  <si>
-    <t>Focusing Orb</t>
-  </si>
-  <si>
-    <t>FocusingOrb.jpg</t>
-  </si>
-  <si>
-    <t>Frozen Magmite</t>
+    <t>Mage's Talisman</t>
+  </si>
+  <si>
+    <t>MagesTalisman.jpg</t>
+  </si>
+  <si>
+    <t>Mage's Totem</t>
+  </si>
+  <si>
+    <t>MagesTotem.jpg</t>
   </si>
   <si>
     <t>Illuminate</t>
   </si>
   <si>
-    <t>FrozenMagmite.jpg</t>
-  </si>
-  <si>
-    <t>Ignite</t>
-  </si>
-  <si>
-    <t>Ignite.jpg</t>
-  </si>
-  <si>
-    <t>Jade</t>
+    <t>Monstrous Inferno</t>
+  </si>
+  <si>
+    <t>MonstrousInferno.jpg</t>
+  </si>
+  <si>
+    <t>Nova Forge</t>
   </si>
   <si>
     <t>Eternal Ember</t>
   </si>
   <si>
-    <t>Jade.jpg</t>
-  </si>
-  <si>
-    <t>Jagged Lightning</t>
-  </si>
-  <si>
-    <t>JaggedLightning.jpg</t>
-  </si>
-  <si>
-    <t>Kindle</t>
-  </si>
-  <si>
-    <t>Kindle.jpg</t>
-  </si>
-  <si>
-    <t>Lava Tendril</t>
-  </si>
-  <si>
-    <t>LavaTendril.jpg</t>
-  </si>
-  <si>
-    <t>Mage's Talisman</t>
-  </si>
-  <si>
-    <t>MagesTalisman.jpg</t>
-  </si>
-  <si>
-    <t>Mage's Totem</t>
-  </si>
-  <si>
-    <t>MagesTotem.jpg</t>
-  </si>
-  <si>
-    <t>Monstrous Inferno</t>
-  </si>
-  <si>
-    <t>MonstrousInferno.jpg</t>
-  </si>
-  <si>
-    <t>Nova Forge</t>
-  </si>
-  <si>
     <t>NovaForge.jpg</t>
   </si>
   <si>
@@ -516,45 +625,102 @@
     <t>Pyrotechnic Surge</t>
   </si>
   <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
     <t>PyrotechnicSurge.jpg</t>
   </si>
   <si>
+    <t>Carapace Queen</t>
+  </si>
+  <si>
     <t>Reduce To Ash</t>
   </si>
   <si>
+    <t>CarapaceQueen.jpg</t>
+  </si>
+  <si>
+    <t>Crooked Mask</t>
+  </si>
+  <si>
     <t>ReduceToAsh.jpg</t>
   </si>
   <si>
+    <t>CrookedMask.jpg</t>
+  </si>
+  <si>
     <t>Scoria Slag</t>
   </si>
   <si>
     <t>ScoriaSlag.jpg</t>
   </si>
   <si>
+    <t>Gate Witch</t>
+  </si>
+  <si>
     <t>Searing Ruby</t>
   </si>
   <si>
+    <t>GateWitch.jpg</t>
+  </si>
+  <si>
+    <t>Hollow Crown</t>
+  </si>
+  <si>
     <t>SearingRuby.jpg</t>
   </si>
   <si>
+    <t>HollowCrown.jpg</t>
+  </si>
+  <si>
     <t>Sifter's Pearl</t>
   </si>
   <si>
+    <t>Horde Crone</t>
+  </si>
+  <si>
+    <t>HordeCrone.jpg</t>
+  </si>
+  <si>
     <t>SiftersPearl.jpg</t>
   </si>
   <si>
+    <t>Magus Of Cloaks</t>
+  </si>
+  <si>
     <t>Spectral Echo</t>
   </si>
   <si>
+    <t>MagusOfCloaks.jpg</t>
+  </si>
+  <si>
+    <t>Prince Of Gluttons</t>
+  </si>
+  <si>
     <t>SpectralEcho.jpg</t>
   </si>
   <si>
+    <t>PrinceOfGluttons.jpg</t>
+  </si>
+  <si>
+    <t>RageBorne</t>
+  </si>
+  <si>
     <t>Thoughtform Familiar</t>
   </si>
   <si>
+    <t>RageBorne.jpg</t>
+  </si>
+  <si>
+    <t>Umbra Titan</t>
+  </si>
+  <si>
     <t>ThoughtformFamiliar.jpg</t>
   </si>
   <si>
+    <t>UmbraTitan.jpg</t>
+  </si>
+  <si>
     <t>Transmogrifier</t>
   </si>
   <si>
@@ -600,72 +766,35 @@
     <t>Wildfire Whip</t>
   </si>
   <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
     <t>WildfireWhip.jpg</t>
   </si>
   <si>
-    <t>Carapace Queen</t>
-  </si>
-  <si>
     <t>Unique</t>
   </si>
   <si>
-    <t>CarapaceQueen.jpg</t>
-  </si>
-  <si>
-    <t>Crooked Mask</t>
-  </si>
-  <si>
-    <t>CrookedMask.jpg</t>
-  </si>
-  <si>
-    <t>Gate Witch</t>
-  </si>
-  <si>
-    <t>GateWitch.jpg</t>
-  </si>
-  <si>
-    <t>Hollow Crown</t>
-  </si>
-  <si>
-    <t>HollowCrown.jpg</t>
-  </si>
-  <si>
-    <t>Horde Crone</t>
-  </si>
-  <si>
-    <t>HordeCrone.jpg</t>
-  </si>
-  <si>
-    <t>Magus Of Cloaks</t>
-  </si>
-  <si>
-    <t>MagusOfCloaks.jpg</t>
-  </si>
-  <si>
-    <t>Prince Of Gluttons</t>
-  </si>
-  <si>
-    <t>PrinceOfGluttons.jpg</t>
-  </si>
-  <si>
-    <t>RageBorne</t>
-  </si>
-  <si>
-    <t>RageBorne.jpg</t>
-  </si>
-  <si>
-    <t>Umbra Titan</t>
-  </si>
-  <si>
-    <t>UmbraTitan.jpg</t>
+    <t>Gain 1 Aether. 
+Any ally may prep a spell in hand to their opened or closed breach(es).</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether. 
+Any ally may draw a card and then discard a card in hand.</t>
+  </si>
+  <si>
+    <t>Cast: Deal 1 damage. Gain 1 Aether.</t>
+  </si>
+  <si>
+    <t>Cast: Deal 1 damage.
+OR
+Cast: Gain 2 Aether.</t>
   </si>
   <si>
     <t>Miriam</t>
   </si>
   <si>
+    <t>If you have 2 life or less, destroy this.
+Otherwise, gain 3 Aether, gain 1 charge, and suffer 2 damage.</t>
+  </si>
+  <si>
     <t>James</t>
   </si>
   <si>
@@ -675,37 +804,96 @@
     <t>Homura</t>
   </si>
   <si>
+    <t>Gain 1 Aether 
+OR 
+Any player gains 1 life.</t>
+  </si>
+  <si>
+    <t>Cast: Deal 1 damage.
+OR
+Cast: Cast one of your prepped spells without discarding it.</t>
+  </si>
+  <si>
+    <t>Cast: Deal 1 damage.
+If this damage causes a minion from the nemesis deck to be discarded, Quilius gains a Trophy token.</t>
+  </si>
+  <si>
+    <t>Cast: Reveal the top card of the turn order deck, and then place it back on top of the turn order deck. If you revealed a player turn order card, deal 3 damage. Otherwise deal 1 damage.</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether.
+OR
+Cast any player's prepped spell.</t>
+  </si>
+  <si>
+    <t>While prepped, when you focus or open one of your breaches during your turn, deal 1 damage.
+Cast: Deal 1 damage.</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether.
+Gain an additional 1 Aether that can only be used to gain a gem.</t>
+  </si>
+  <si>
+    <t>Gain 2 Aether that cannot be used to gain a relic or spell.</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether.
+You may suffer 1 damage. If you do, gain an additional 2 Aether.</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether.
+Reveal the top card of the turn order deck. You may place that card on the bottom or the top of the turn order deck. If you revealed a player turn order card, gain an additional 1 Aether.</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether.
+You may place the top card of any ally's discard pile into your hand.</t>
+  </si>
+  <si>
+    <t>Cast: Deal 1 damage.
+OR
+Cast: Focus any player's breach.</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether.
+Any ally may suffer 1 damage. If they do, they destroy a card in hand.</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Mage 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Mage 2</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>Gain 1 Aether.
+OR
+Gain 2 Aether that can only be used to gain a card. Place the next card you gain this turn on top of any ally's discard pile.</t>
+  </si>
+  <si>
+    <t>Nemesis</t>
+  </si>
+  <si>
+    <t>Market Card 1</t>
+  </si>
+  <si>
     <t>Common</t>
   </si>
   <si>
+    <t>Market Card 2</t>
+  </si>
+  <si>
     <t>Crystal.png</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Player 1</t>
-  </si>
-  <si>
-    <t>Mage 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
-  </si>
-  <si>
-    <t>Mage 2</t>
-  </si>
-  <si>
-    <t>Won</t>
-  </si>
-  <si>
-    <t>Nemesis</t>
-  </si>
-  <si>
-    <t>Market Card 1</t>
-  </si>
-  <si>
-    <t>Market Card 2</t>
   </si>
   <si>
     <t>Market Card 3</t>
@@ -853,1357 +1041,1417 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1">
         <v>7.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1">
         <v>6.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1">
         <v>3.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1">
         <v>4.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B10" s="1">
         <v>5.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="B11" s="1">
         <v>4.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="B12" s="1">
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B13" s="1">
         <v>5.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="B14" s="1">
         <v>6.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="B15" s="1">
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="B16" s="1">
         <v>5.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="B17" s="1">
         <v>3.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="B18" s="1">
         <v>6.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B19" s="1">
         <v>7.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="B20" s="1">
         <v>5.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="B21" s="1">
         <v>8.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B22" s="1">
         <v>5.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B23" s="1">
         <v>6.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B24" s="1">
         <v>4.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="B25" s="1">
         <v>7.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B26" s="1">
         <v>3.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="B27" s="1">
         <v>7.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="B28" s="1">
         <v>5.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B29" s="1">
         <v>5.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B31" s="1">
         <v>3.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B32" s="1">
         <v>5.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="B33" s="1">
         <v>2.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="B34" s="1">
         <v>4.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B35" s="1">
         <v>3.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="B36" s="1">
         <v>4.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="B37" s="1">
         <v>2.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B38" s="1">
         <v>4.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="B39" s="1">
         <v>4.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="B40" s="1">
         <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="B41" s="1">
         <v>5.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B42" s="1">
         <v>2.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="B43" s="1">
         <v>8.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="B44" s="1">
         <v>6.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="B45" s="1">
         <v>5.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="B46" s="1">
         <v>3.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="B47" s="1">
         <v>6.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="B48" s="1">
         <v>4.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="B49" s="1">
         <v>4.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="B50" s="1">
         <v>7.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="B51" s="1">
         <v>4.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="B52" s="1">
         <v>4.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="B53" s="1">
         <v>3.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="B54" s="1">
         <v>3.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="B55" s="1">
         <v>3.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="B56" s="1">
         <v>4.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="B57" s="1">
         <v>3.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="B58" s="1">
         <v>3.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>184</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="B59" s="1">
         <v>4.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="B60" s="1">
         <v>4.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="B61" s="1">
         <v>3.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="B62" s="1">
         <v>6.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>192</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="B63" s="1">
         <v>6.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="B64" s="1">
         <v>0.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B65" s="1">
         <v>0.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" s="1">
         <v>0.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="B67" s="1">
         <v>0.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="B68" s="1">
         <v>0.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B69" s="1">
         <v>0.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="B70" s="1">
         <v>0.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="B71" s="1">
         <v>0.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="B72" s="1">
         <v>0.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B73" s="1">
         <v>0.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="B74" s="1">
         <v>0.0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B75" s="1">
         <v>0.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B76" s="1">
         <v>0.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="B77" s="1">
         <v>0.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B78" s="1">
         <v>0.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B79" s="1">
         <v>0.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B80" s="1">
         <v>0.0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="B81" s="1">
         <v>0.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B82" s="1">
         <v>0.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>197</v>
+        <v>235</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B83" s="1">
         <v>0.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>219</v>
+        <v>267</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>220</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B84" s="1">
         <v>0.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>219</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2231,28 +2479,40 @@
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2263,13 +2523,19 @@
       <c r="B5" t="s">
         <v>23</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -2279,109 +2545,151 @@
       <c r="B7" t="s">
         <v>30</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>66</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>82</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>87</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>93</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2401,23 +2709,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>7.0</v>
@@ -2427,10 +2735,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -2440,10 +2748,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
@@ -2452,10 +2760,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>7.0</v>
@@ -2464,10 +2772,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -2476,10 +2784,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -2488,10 +2796,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>6.0</v>
@@ -2500,10 +2808,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -2512,10 +2820,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1">
         <v>1.0</v>
@@ -2527,7 +2835,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>6.0</v>
@@ -2540,7 +2848,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
         <v>3.0</v>
@@ -2552,7 +2860,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
@@ -2561,10 +2869,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>7.0</v>
@@ -2573,10 +2881,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
         <v>2.0</v>
@@ -2585,10 +2893,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -2600,7 +2908,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1">
         <v>5.0</v>
@@ -2612,7 +2920,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>4.0</v>
@@ -2624,7 +2932,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1">
         <v>1.0</v>
@@ -2633,10 +2941,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1">
         <v>6.0</v>
@@ -2645,10 +2953,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1">
         <v>3.0</v>
@@ -2657,10 +2965,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1">
         <v>1.0</v>
@@ -2669,10 +2977,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
         <v>6.0</v>
@@ -2681,10 +2989,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" s="1">
         <v>3.0</v>
@@ -2693,10 +3001,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -2705,10 +3013,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1">
         <v>6.0</v>
@@ -2717,10 +3025,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1">
         <v>3.0</v>
@@ -2729,10 +3037,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C28" s="1">
         <v>1.0</v>
@@ -2741,10 +3049,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" s="1">
         <v>6.0</v>
@@ -2753,10 +3061,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1">
         <v>3.0</v>
@@ -2764,10 +3072,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C31" s="1">
         <v>1.0</v>
@@ -2775,10 +3083,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="1">
         <v>6.0</v>
@@ -2786,10 +3094,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1">
         <v>3.0</v>
@@ -2797,10 +3105,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="C34" s="1">
         <v>1.0</v>
@@ -2808,10 +3116,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1">
         <v>7.0</v>
@@ -2819,10 +3127,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36" s="1">
         <v>2.0</v>
@@ -2830,10 +3138,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="C37" s="1">
         <v>1.0</v>
@@ -2841,10 +3149,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C38" s="1">
         <v>7.0</v>
@@ -2852,10 +3160,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C39" s="1">
         <v>2.0</v>
@@ -2863,10 +3171,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="C40" s="1">
         <v>1.0</v>
@@ -2874,10 +3182,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" s="1">
         <v>6.0</v>
@@ -2885,10 +3193,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C42" s="1">
         <v>2.0</v>
@@ -2896,10 +3204,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="C43" s="1">
         <v>2.0</v>
@@ -2907,10 +3215,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1">
         <v>5.0</v>
@@ -2918,10 +3226,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C45" s="1">
         <v>4.0</v>
@@ -2929,10 +3237,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="C46" s="1">
         <v>1.0</v>
@@ -2940,10 +3248,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47" s="1">
         <v>5.0</v>
@@ -2951,10 +3259,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C48" s="1">
         <v>4.0</v>
@@ -2962,10 +3270,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="C49" s="1">
         <v>1.0</v>
@@ -2973,10 +3281,10 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C50" s="1">
         <v>8.0</v>
@@ -2984,10 +3292,10 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C51" s="1">
         <v>1.0</v>
@@ -2995,10 +3303,10 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="C52" s="1">
         <v>1.0</v>
@@ -3006,10 +3314,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C53" s="1">
         <v>8.0</v>
@@ -3017,10 +3325,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C54" s="1">
         <v>1.0</v>
@@ -3028,10 +3336,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="C55" s="1">
         <v>1.0</v>
@@ -3039,10 +3347,10 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56" s="1">
         <v>8.0</v>
@@ -3050,10 +3358,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C57" s="1">
         <v>1.0</v>
@@ -3061,10 +3369,10 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="C58" s="1">
         <v>1.0</v>
@@ -3094,7 +3402,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -3102,57 +3410,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1">
         <v>3.0</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B3" s="1">
         <v>5.0</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B4" s="1">
         <v>7.0</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="1">
         <v>6.0</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7">
@@ -3163,40 +3471,40 @@
         <v>7.0</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B8" s="1">
         <v>5.0</v>
       </c>
       <c r="C8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B9" s="1">
         <v>2.0</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B10" s="1">
         <v>3.0</v>
       </c>
       <c r="C10" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3218,22 +3526,22 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3253,73 +3561,73 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>259</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>223</v>
+        <v>260</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>224</v>
+        <v>261</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>226</v>
+        <v>263</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>229</v>
+        <v>268</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>230</v>
+        <v>270</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>231</v>
+        <v>271</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>233</v>
+        <v>273</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>234</v>
+        <v>274</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -3328,51 +3636,51 @@
         <v>10.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -3381,51 +3689,51 @@
         <v>10.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
@@ -3434,51 +3742,51 @@
         <v>8.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -3487,51 +3795,51 @@
         <v>10.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -3540,34 +3848,34 @@
         <v>8.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds the nameless expansion to the database. Run db:reset.
</commit_message>
<xml_diff>
--- a/lib/seeds/Aeon's End Database.xlsx
+++ b/lib/seeds/Aeon's End Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -68,12 +68,12 @@
     <t>Brama.jpg</t>
   </si>
   <si>
-    <t>Spark</t>
-  </si>
-  <si>
     <t>Cost: 5 Charges.
 Activate during your main phase:
 Any player gains 4 life.</t>
+  </si>
+  <si>
+    <t>Spark</t>
   </si>
   <si>
     <t>Dezmodia</t>
@@ -102,10 +102,10 @@
 Deal 2 damage plus 4 additional damage for each spell you discarded divided however you choose to the nemesis or any number of minions</t>
   </si>
   <si>
+    <t>Buried Light</t>
+  </si>
+  <si>
     <t>Gex</t>
-  </si>
-  <si>
-    <t>Buried Light</t>
   </si>
   <si>
     <t>Gex.jpg</t>
@@ -129,9 +129,6 @@
 Then cast that prepped spell again.</t>
   </si>
   <si>
-    <t>Amplify Vision</t>
-  </si>
-  <si>
     <t>Kadir</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
   </si>
   <si>
     <t>Oblivion Shard</t>
-  </si>
-  <si>
-    <t>Spell</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -149,13 +143,7 @@
 That player may return up to three spells in their discard pile to their hand. That player may prep up to two spells to each of their opened breaches this turn.</t>
   </si>
   <si>
-    <t>Market</t>
-  </si>
-  <si>
     <t>Lash</t>
-  </si>
-  <si>
-    <t>AmplifyVision.jpg</t>
   </si>
   <si>
     <t>Lash.jpg</t>
@@ -164,6 +152,20 @@
     <t>Cost: 6 Charges.
 Activate during any player's main phase:
 Shuffle any player's turn order card into the turn order deck. That player suffers 1 damage.</t>
+  </si>
+  <si>
+    <t>Malastar</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Malastar.jpg</t>
+  </si>
+  <si>
+    <t>6 Charges.
+Activate during your main phase:
+Gain a spell from any supply pile. You may prep that spell to any player's opened breach.</t>
   </si>
   <si>
     <t>Mazahaedron</t>
@@ -178,9 +180,6 @@
 Gravehold gains 4 life.</t>
   </si>
   <si>
-    <t>Torch</t>
-  </si>
-  <si>
     <t>Mist (Dagger Captain)</t>
   </si>
   <si>
@@ -192,6 +191,9 @@
 Any ally draws 4 cards.</t>
   </si>
   <si>
+    <t>Shattered Geode</t>
+  </si>
+  <si>
     <t>Mist (Voidwalker)</t>
   </si>
   <si>
@@ -203,16 +205,10 @@
 Cast up to three different spells prepped by any number of players. For each spell cast this way, place that spell into any ally's hand.</t>
   </si>
   <si>
-    <t>Arcane Nexus</t>
-  </si>
-  <si>
     <t>Nym</t>
   </si>
   <si>
     <t>Nym.jpg</t>
-  </si>
-  <si>
-    <t>Shattered Geode</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -221,13 +217,10 @@
 If you discarded an attack card, discard an additional card.</t>
   </si>
   <si>
-    <t>ArcaneNexus.jpg</t>
+    <t>Moonstone Shard</t>
   </si>
   <si>
     <t>Phaedraxa</t>
-  </si>
-  <si>
-    <t>Aurora</t>
   </si>
   <si>
     <t>Phaedraxa.jpg</t>
@@ -238,13 +231,7 @@
 Prevent any damage that the players or Gravehold would suffer during that turn.</t>
   </si>
   <si>
-    <t>Aurora.jpg</t>
-  </si>
-  <si>
     <t>Quilius</t>
-  </si>
-  <si>
-    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Quilius.jpg</t>
@@ -255,16 +242,13 @@
 Deal 2 damage for each Trophy token you have.</t>
   </si>
   <si>
-    <t>Gem</t>
-  </si>
-  <si>
     <t>Reeve</t>
   </si>
   <si>
+    <t>Emerald Shard</t>
+  </si>
+  <si>
     <t>Reeve.jpg</t>
-  </si>
-  <si>
-    <t>BanishingTopaz.jpg</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -273,19 +257,10 @@
 Deal 3 damage to a different minion.</t>
   </si>
   <si>
-    <t>Blasting Staff</t>
-  </si>
-  <si>
     <t>Ulgimor</t>
   </si>
   <si>
     <t>Ulgimor.jpg</t>
-  </si>
-  <si>
-    <t>Relic</t>
-  </si>
-  <si>
-    <t>Moonstone Shard</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -294,13 +269,10 @@
 If you are exhausted, any ally gains 5 life instead.</t>
   </si>
   <si>
-    <t>BlastingStaff.jpg</t>
-  </si>
-  <si>
     <t>Xaxos</t>
   </si>
   <si>
-    <t>Bloodstone Jewel</t>
+    <t>Quartz Shard</t>
   </si>
   <si>
     <t>Xaxos.jpg</t>
@@ -312,13 +284,7 @@
 Reveal the turn order deck and return the revealed cards in any order.</t>
   </si>
   <si>
-    <t>BloodstoneJewel.jpg</t>
-  </si>
-  <si>
     <t>Yan Magda</t>
-  </si>
-  <si>
-    <t>Bottled Vortex</t>
   </si>
   <si>
     <t>YanMagda.jpg</t>
@@ -329,16 +295,7 @@
 Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
   </si>
   <si>
-    <t>BottledVortex.jpg</t>
-  </si>
-  <si>
-    <t>Emerald Shard</t>
-  </si>
-  <si>
     <t>Z'hana</t>
-  </si>
-  <si>
-    <t>Breach Ore</t>
   </si>
   <si>
     <t>Zhana.jpg</t>
@@ -349,6 +306,105 @@
 Gravehold gains 7 life.</t>
   </si>
   <si>
+    <t>Immolate</t>
+  </si>
+  <si>
+    <t>Worldheart Shard</t>
+  </si>
+  <si>
+    <t>Garnet Shard</t>
+  </si>
+  <si>
+    <t>Amethyst Paragon</t>
+  </si>
+  <si>
+    <t>Cinder</t>
+  </si>
+  <si>
+    <t>Tourmaline Shard</t>
+  </si>
+  <si>
+    <t>Extinguish</t>
+  </si>
+  <si>
+    <t>Obsidian Shard</t>
+  </si>
+  <si>
+    <t>Coal Shard</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>Illuminate</t>
+  </si>
+  <si>
+    <t>Eternal Ember</t>
+  </si>
+  <si>
+    <t>Amplify Vision</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>AmplifyVision.jpg</t>
+  </si>
+  <si>
+    <t>Arcane Nexus</t>
+  </si>
+  <si>
+    <t>ArcaneNexus.jpg</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>Aurora.jpg</t>
+  </si>
+  <si>
+    <t>Banishing Topaz</t>
+  </si>
+  <si>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>BanishingTopaz.jpg</t>
+  </si>
+  <si>
+    <t>Blasting Staff</t>
+  </si>
+  <si>
+    <t>Relic</t>
+  </si>
+  <si>
+    <t>BlastingStaff.jpg</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Blaze.jpg</t>
+  </si>
+  <si>
+    <t>Bloodstone Jewel</t>
+  </si>
+  <si>
+    <t>BloodstoneJewel.jpg</t>
+  </si>
+  <si>
+    <t>Bottled Vortex</t>
+  </si>
+  <si>
+    <t>BottledVortex.jpg</t>
+  </si>
+  <si>
+    <t>Breach Ore</t>
+  </si>
+  <si>
     <t>BreachOre.jpg</t>
   </si>
   <si>
@@ -361,9 +417,6 @@
     <t>Cairn Compass</t>
   </si>
   <si>
-    <t>Quartz Shard</t>
-  </si>
-  <si>
     <t>CairnCompass.jpg</t>
   </si>
   <si>
@@ -376,9 +429,6 @@
     <t>Celestial Spire</t>
   </si>
   <si>
-    <t>Worldheart Shard</t>
-  </si>
-  <si>
     <t>CelestialSpire.jpg</t>
   </si>
   <si>
@@ -391,15 +441,24 @@
     <t>Clouded Sapphire</t>
   </si>
   <si>
-    <t>Garnet Shard</t>
+    <t>Miriam</t>
   </si>
   <si>
     <t>CloudedSapphire.jpg</t>
   </si>
   <si>
+    <t>James</t>
+  </si>
+  <si>
     <t>Combustion</t>
   </si>
   <si>
+    <t>Kermit</t>
+  </si>
+  <si>
+    <t>Homura</t>
+  </si>
+  <si>
     <t>Combustion.jpg</t>
   </si>
   <si>
@@ -412,63 +471,132 @@
     <t>Conjure The Lost</t>
   </si>
   <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
     <t>ConjureTheLost.jpg</t>
   </si>
   <si>
     <t>Consuming Void</t>
   </si>
   <si>
+    <t>Blight Lord</t>
+  </si>
+  <si>
     <t>ConsumingVoid.jpg</t>
   </si>
   <si>
     <t>Convection Field</t>
   </si>
   <si>
+    <t>BlightLord.jpg</t>
+  </si>
+  <si>
     <t>ConvectionField.jpg</t>
   </si>
   <si>
     <t>Crystallize</t>
   </si>
   <si>
+    <t>Carapace Queen</t>
+  </si>
+  <si>
+    <t>CarapaceQueen.jpg</t>
+  </si>
+  <si>
+    <t>Crooked Mask</t>
+  </si>
+  <si>
     <t>Crystallize.jpg</t>
   </si>
   <si>
     <t>Dark Fire</t>
   </si>
   <si>
+    <t>CrookedMask.jpg</t>
+  </si>
+  <si>
+    <t>Gate Witch</t>
+  </si>
+  <si>
     <t>DarkFire.jpg</t>
   </si>
   <si>
+    <t>GateWitch.jpg</t>
+  </si>
+  <si>
     <t>Devouring Shadow</t>
   </si>
   <si>
+    <t>Hollow Crown</t>
+  </si>
+  <si>
+    <t>HollowCrown.jpg</t>
+  </si>
+  <si>
     <t>DevouringShadow.jpg</t>
   </si>
   <si>
+    <t>Horde Crone</t>
+  </si>
+  <si>
     <t>Diamond Cluster</t>
   </si>
   <si>
+    <t>HordeCrone.jpg</t>
+  </si>
+  <si>
+    <t>Magus Of Cloaks</t>
+  </si>
+  <si>
     <t>DiamondCluster.jpg</t>
   </si>
   <si>
+    <t>MagusOfCloaks.jpg</t>
+  </si>
+  <si>
     <t>Disintegrating Scythe</t>
   </si>
   <si>
+    <t>Prince Of Gluttons</t>
+  </si>
+  <si>
+    <t>PrinceOfGluttons.jpg</t>
+  </si>
+  <si>
     <t>DisintegratingScythe.jpg</t>
   </si>
   <si>
+    <t>RageBorne</t>
+  </si>
+  <si>
     <t>Dread Diamond</t>
   </si>
   <si>
+    <t>RageBorne.jpg</t>
+  </si>
+  <si>
+    <t>Umbra Titan</t>
+  </si>
+  <si>
     <t>DreadDiamond.jpg</t>
   </si>
   <si>
+    <t>UmbraTitan.jpg</t>
+  </si>
+  <si>
     <t>Equilibrium</t>
   </si>
   <si>
+    <t>Wayward One</t>
+  </si>
+  <si>
     <t>Equilibrium.jpg</t>
   </si>
   <si>
+    <t>WaywardOne.jpg</t>
+  </si>
+  <si>
     <t>Erratic Ingot</t>
   </si>
   <si>
@@ -484,9 +612,6 @@
     <t>Feral Lightning</t>
   </si>
   <si>
-    <t>Amethyst Paragon</t>
-  </si>
-  <si>
     <t>FeralLightning.jpg</t>
   </si>
   <si>
@@ -496,9 +621,6 @@
     <t>FiendCatcher.jpg</t>
   </si>
   <si>
-    <t>Cinder</t>
-  </si>
-  <si>
     <t>Fiery Torrent</t>
   </si>
   <si>
@@ -508,9 +630,6 @@
     <t>Flexing Dagger</t>
   </si>
   <si>
-    <t>Tourmaline Shard</t>
-  </si>
-  <si>
     <t>FlexingDagger.jpg</t>
   </si>
   <si>
@@ -526,9 +645,6 @@
     <t>FrozenMagmite.jpg</t>
   </si>
   <si>
-    <t>Extinguish</t>
-  </si>
-  <si>
     <t>Ignite</t>
   </si>
   <si>
@@ -538,9 +654,6 @@
     <t>Jade</t>
   </si>
   <si>
-    <t>Obsidian Shard</t>
-  </si>
-  <si>
     <t>Jade.jpg</t>
   </si>
   <si>
@@ -553,9 +666,6 @@
     <t>Kindle</t>
   </si>
   <si>
-    <t>Coal Shard</t>
-  </si>
-  <si>
     <t>Kindle.jpg</t>
   </si>
   <si>
@@ -565,7 +675,10 @@
     <t>LavaTendril.jpg</t>
   </si>
   <si>
-    <t>Flare</t>
+    <t>Leeching Agate</t>
+  </si>
+  <si>
+    <t>LeechingAgate.jpg</t>
   </si>
   <si>
     <t>Mage's Talisman</t>
@@ -580,21 +693,21 @@
     <t>MagesTotem.jpg</t>
   </si>
   <si>
-    <t>Illuminate</t>
-  </si>
-  <si>
     <t>Monstrous Inferno</t>
   </si>
   <si>
     <t>MonstrousInferno.jpg</t>
   </si>
   <si>
+    <t>Molten Hammer</t>
+  </si>
+  <si>
+    <t>MoltenHammer.jpg</t>
+  </si>
+  <si>
     <t>Nova Forge</t>
   </si>
   <si>
-    <t>Eternal Ember</t>
-  </si>
-  <si>
     <t>NovaForge.jpg</t>
   </si>
   <si>
@@ -625,28 +738,25 @@
     <t>Pyrotechnic Surge</t>
   </si>
   <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
     <t>PyrotechnicSurge.jpg</t>
   </si>
   <si>
-    <t>Carapace Queen</t>
+    <t>Radiance</t>
+  </si>
+  <si>
+    <t>Radiance.jpg</t>
   </si>
   <si>
     <t>Reduce To Ash</t>
   </si>
   <si>
-    <t>CarapaceQueen.jpg</t>
-  </si>
-  <si>
-    <t>Crooked Mask</t>
-  </si>
-  <si>
     <t>ReduceToAsh.jpg</t>
   </si>
   <si>
-    <t>CrookedMask.jpg</t>
+    <t>Sage's Brand</t>
+  </si>
+  <si>
+    <t>SagesBrand.jpg</t>
   </si>
   <si>
     <t>Scoria Slag</t>
@@ -655,85 +765,91 @@
     <t>ScoriaSlag.jpg</t>
   </si>
   <si>
-    <t>Gate Witch</t>
+    <t>Scrying Bolt</t>
+  </si>
+  <si>
+    <t>ScryingBolt.jpg</t>
   </si>
   <si>
     <t>Searing Ruby</t>
   </si>
   <si>
-    <t>GateWitch.jpg</t>
-  </si>
-  <si>
-    <t>Hollow Crown</t>
-  </si>
-  <si>
     <t>SearingRuby.jpg</t>
   </si>
   <si>
-    <t>HollowCrown.jpg</t>
-  </si>
-  <si>
     <t>Sifter's Pearl</t>
   </si>
   <si>
-    <t>Horde Crone</t>
-  </si>
-  <si>
-    <t>HordeCrone.jpg</t>
-  </si>
-  <si>
     <t>SiftersPearl.jpg</t>
   </si>
   <si>
-    <t>Magus Of Cloaks</t>
-  </si>
-  <si>
     <t>Spectral Echo</t>
   </si>
   <si>
-    <t>MagusOfCloaks.jpg</t>
-  </si>
-  <si>
-    <t>Prince Of Gluttons</t>
-  </si>
-  <si>
     <t>SpectralEcho.jpg</t>
   </si>
   <si>
-    <t>PrinceOfGluttons.jpg</t>
-  </si>
-  <si>
-    <t>RageBorne</t>
+    <t>Temporal Helix</t>
+  </si>
+  <si>
+    <t>TemporalHelix.jpg</t>
   </si>
   <si>
     <t>Thoughtform Familiar</t>
   </si>
   <si>
-    <t>RageBorne.jpg</t>
-  </si>
-  <si>
-    <t>Umbra Titan</t>
-  </si>
-  <si>
     <t>ThoughtformFamiliar.jpg</t>
   </si>
   <si>
-    <t>UmbraTitan.jpg</t>
+    <t>Date</t>
   </si>
   <si>
     <t>Transmogrifier</t>
   </si>
   <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Mage 1</t>
+  </si>
+  <si>
     <t>Transmogrifier.jpg</t>
   </si>
   <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Mage 2</t>
+  </si>
+  <si>
     <t>Unstable Prism</t>
   </si>
   <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>Nemesis</t>
+  </si>
+  <si>
     <t>UnstablePrism.jpg</t>
   </si>
   <si>
+    <t>Market Card 1</t>
+  </si>
+  <si>
+    <t>Market Card 2</t>
+  </si>
+  <si>
     <t>V'riswood Amber</t>
+  </si>
+  <si>
+    <t>Market Card 3</t>
+  </si>
+  <si>
+    <t>Market Card 4</t>
+  </si>
+  <si>
+    <t>Market Card 5</t>
   </si>
   <si>
     <t>VriswoodAmber.jpg</t>
@@ -788,20 +904,8 @@
 Cast: Gain 2 Aether.</t>
   </si>
   <si>
-    <t>Miriam</t>
-  </si>
-  <si>
     <t>If you have 2 life or less, destroy this.
 Otherwise, gain 3 Aether, gain 1 charge, and suffer 2 damage.</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Kermit</t>
-  </si>
-  <si>
-    <t>Homura</t>
   </si>
   <si>
     <t>Gain 1 Aether 
@@ -814,8 +918,23 @@
 Cast: Cast one of your prepped spells without discarding it.</t>
   </si>
   <si>
+    <t>Market Card 6</t>
+  </si>
+  <si>
+    <t>Market Card 7</t>
+  </si>
+  <si>
+    <t>Market Card 8</t>
+  </si>
+  <si>
+    <t>Market Card 9</t>
+  </si>
+  <si>
     <t>Cast: Deal 1 damage.
 If this damage causes a minion from the nemesis deck to be discarded, Quilius gains a Trophy token.</t>
+  </si>
+  <si>
+    <t>2017/11/12 5:30PM PST</t>
   </si>
   <si>
     <t>Cast: Reveal the top card of the turn order deck, and then place it back on top of the turn order deck. If you revealed a player turn order card, deal 3 damage. Otherwise deal 1 damage.</t>
@@ -830,6 +949,13 @@
 Cast: Deal 1 damage.</t>
   </si>
   <si>
+    <t>While prepped, when you suffer damage cain 1 charge.
+Cast: Deal 1 damage.</t>
+  </si>
+  <si>
+    <t>2017/11/12 7:00PM PST</t>
+  </si>
+  <si>
     <t>Gain 1 Aether.
 Gain an additional 1 Aether that can only be used to gain a gem.</t>
   </si>
@@ -837,6 +963,9 @@
     <t>Gain 2 Aether that cannot be used to gain a relic or spell.</t>
   </si>
   <si>
+    <t>2017/11/12 9:00PM PST</t>
+  </si>
+  <si>
     <t>Gain 1 Aether.
 You may suffer 1 damage. If you do, gain an additional 2 Aether.</t>
   </si>
@@ -847,6 +976,9 @@
   <si>
     <t>Gain 1 Aether.
 You may place the top card of any ally's discard pile into your hand.</t>
+  </si>
+  <si>
+    <t>2017/11/10 7:00PM PST</t>
   </si>
   <si>
     <t>Cast: Deal 1 damage.
@@ -858,78 +990,18 @@
 Any ally may suffer 1 damage. If they do, they destroy a card in hand.</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Player 1</t>
-  </si>
-  <si>
-    <t>Mage 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
-  </si>
-  <si>
-    <t>Mage 2</t>
-  </si>
-  <si>
-    <t>Won</t>
-  </si>
-  <si>
     <t>Gain 1 Aether.
 OR
 Gain 2 Aether that can only be used to gain a card. Place the next card you gain this turn on top of any ally's discard pile.</t>
   </si>
   <si>
-    <t>Nemesis</t>
-  </si>
-  <si>
-    <t>Market Card 1</t>
+    <t>2017/11/10 9:00PM PST</t>
   </si>
   <si>
     <t>Common</t>
   </si>
   <si>
-    <t>Market Card 2</t>
-  </si>
-  <si>
     <t>Crystal.png</t>
-  </si>
-  <si>
-    <t>Market Card 3</t>
-  </si>
-  <si>
-    <t>Market Card 4</t>
-  </si>
-  <si>
-    <t>Market Card 5</t>
-  </si>
-  <si>
-    <t>Market Card 6</t>
-  </si>
-  <si>
-    <t>Market Card 7</t>
-  </si>
-  <si>
-    <t>Market Card 8</t>
-  </si>
-  <si>
-    <t>Market Card 9</t>
-  </si>
-  <si>
-    <t>2017/11/12 5:30PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/12 7:00PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/12 9:00PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/10 7:00PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/10 9:00PM PST</t>
   </si>
 </sst>
 </file>
@@ -1047,1411 +1119,1548 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1">
         <v>7.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B8" s="1">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B10" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B11" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1">
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B13" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B15" s="1">
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B16" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B17" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B18" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="B19" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B21" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B22" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="B23" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="B24" s="1">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="B25" s="1">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="B27" s="1">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="B28" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="B29" s="1">
         <v>5.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="B31" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="B32" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="B33" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="B34" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="B35" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="B36" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="B37" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="B38" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="B39" s="1">
         <v>4.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="B40" s="1">
         <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="B41" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B42" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>171</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" s="1"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="B43" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="B44" s="1">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="B45" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="B46" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>181</v>
+        <v>94</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="B47" s="1">
         <v>6.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="B48" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="B49" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="B50" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="B51" s="1">
         <v>4.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="B52" s="1">
         <v>4.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="B53" s="1">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>206</v>
+        <v>94</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="B54" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="B55" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>217</v>
+        <v>94</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="B56" s="1">
         <v>4.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B57" s="1">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>222</v>
+        <v>94</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="B58" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="B59" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="B60" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B61" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>230</v>
+        <v>94</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="B62" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="B63" s="1">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>252</v>
       </c>
       <c r="B64" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>236</v>
+        <v>94</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>20</v>
+        <v>258</v>
       </c>
       <c r="B65" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>237</v>
+        <v>94</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="B66" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>238</v>
+        <v>94</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>144</v>
+        <v>265</v>
       </c>
       <c r="B67" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>239</v>
+        <v>94</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>163</v>
+        <v>267</v>
       </c>
       <c r="B68" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>241</v>
+        <v>94</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>269</v>
       </c>
       <c r="B69" s="1">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>245</v>
+        <v>94</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>176</v>
+        <v>271</v>
       </c>
       <c r="B70" s="1">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>246</v>
+        <v>94</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="B71" s="1">
         <v>0.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>167</v>
+        <v>20</v>
       </c>
       <c r="B72" s="1">
         <v>0.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="B73" s="1">
         <v>0.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>172</v>
+        <v>84</v>
       </c>
       <c r="B74" s="1">
         <v>0.0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B75" s="1">
         <v>0.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B76" s="1">
         <v>0.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="B77" s="1">
         <v>0.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B78" s="1">
         <v>0.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B79" s="1">
         <v>0.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B80" s="1">
         <v>0.0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="B81" s="1">
         <v>0.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1">
         <v>0.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B83" s="1">
         <v>0.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B84" s="1">
         <v>0.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2502,7 +2711,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -2529,7 +2738,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -2551,145 +2760,156 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2738,7 +2958,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -2775,7 +2995,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -2787,7 +3007,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -2811,7 +3031,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -2823,7 +3043,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>1.0</v>
@@ -2848,7 +3068,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1">
         <v>3.0</v>
@@ -2860,7 +3080,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
@@ -2869,7 +3089,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -2881,10 +3101,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <v>2.0</v>
@@ -2893,10 +3113,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -2920,7 +3140,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1">
         <v>4.0</v>
@@ -2932,7 +3152,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1">
         <v>1.0</v>
@@ -2941,7 +3161,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>12</v>
@@ -2953,10 +3173,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1">
         <v>3.0</v>
@@ -2965,10 +3185,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1">
         <v>1.0</v>
@@ -2977,7 +3197,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>12</v>
@@ -2989,10 +3209,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1">
         <v>3.0</v>
@@ -3001,10 +3221,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -3013,34 +3233,34 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="1">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1">
         <v>1.0</v>
@@ -3049,7 +3269,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>12</v>
@@ -3061,29 +3281,31 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1">
         <v>3.0</v>
       </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="C31" s="1">
         <v>1.0</v>
       </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>12</v>
@@ -3091,13 +3313,14 @@
       <c r="C32" s="1">
         <v>6.0</v>
       </c>
+      <c r="E32" s="1"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1">
         <v>3.0</v>
@@ -3105,10 +3328,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1">
         <v>1.0</v>
@@ -3116,32 +3339,32 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C36" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1">
         <v>1.0</v>
@@ -3149,7 +3372,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>12</v>
@@ -3160,10 +3383,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1">
         <v>2.0</v>
@@ -3171,10 +3394,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="C40" s="1">
         <v>1.0</v>
@@ -3182,21 +3405,21 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1">
         <v>2.0</v>
@@ -3204,51 +3427,51 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="C43" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>12</v>
@@ -3259,10 +3482,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C48" s="1">
         <v>4.0</v>
@@ -3270,10 +3493,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>163</v>
+        <v>87</v>
       </c>
       <c r="C49" s="1">
         <v>1.0</v>
@@ -3281,32 +3504,32 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C51" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="C52" s="1">
         <v>1.0</v>
@@ -3314,7 +3537,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>12</v>
@@ -3325,10 +3548,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C54" s="1">
         <v>1.0</v>
@@ -3336,10 +3559,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="C55" s="1">
         <v>1.0</v>
@@ -3347,7 +3570,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>12</v>
@@ -3358,10 +3581,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C57" s="1">
         <v>1.0</v>
@@ -3369,12 +3592,45 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C58" s="1">
+      <c r="C61" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -3402,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -3410,101 +3666,123 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
+        <v>4.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>144</v>
       </c>
       <c r="B3" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B7" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="B8" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>216</v>
+        <v>167</v>
       </c>
       <c r="B10" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="1">
         <v>3.0</v>
       </c>
-      <c r="C10" t="s">
-        <v>218</v>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3526,22 +3804,22 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>242</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>243</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>244</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3561,70 +3839,70 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -3636,48 +3914,48 @@
         <v>10.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -3689,48 +3967,48 @@
         <v>10.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -3742,51 +4020,51 @@
         <v>8.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -3795,51 +4073,51 @@
         <v>10.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>231</v>
+        <v>269</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -3848,34 +4126,34 @@
         <v>8.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>231</v>
+        <v>269</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds the nameless expansion to the database. (#31)
Run db:reset.
</commit_message>
<xml_diff>
--- a/lib/seeds/Aeon's End Database.xlsx
+++ b/lib/seeds/Aeon's End Database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -68,12 +68,12 @@
     <t>Brama.jpg</t>
   </si>
   <si>
-    <t>Spark</t>
-  </si>
-  <si>
     <t>Cost: 5 Charges.
 Activate during your main phase:
 Any player gains 4 life.</t>
+  </si>
+  <si>
+    <t>Spark</t>
   </si>
   <si>
     <t>Dezmodia</t>
@@ -102,10 +102,10 @@
 Deal 2 damage plus 4 additional damage for each spell you discarded divided however you choose to the nemesis or any number of minions</t>
   </si>
   <si>
+    <t>Buried Light</t>
+  </si>
+  <si>
     <t>Gex</t>
-  </si>
-  <si>
-    <t>Buried Light</t>
   </si>
   <si>
     <t>Gex.jpg</t>
@@ -129,9 +129,6 @@
 Then cast that prepped spell again.</t>
   </si>
   <si>
-    <t>Amplify Vision</t>
-  </si>
-  <si>
     <t>Kadir</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
   </si>
   <si>
     <t>Oblivion Shard</t>
-  </si>
-  <si>
-    <t>Spell</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -149,13 +143,7 @@
 That player may return up to three spells in their discard pile to their hand. That player may prep up to two spells to each of their opened breaches this turn.</t>
   </si>
   <si>
-    <t>Market</t>
-  </si>
-  <si>
     <t>Lash</t>
-  </si>
-  <si>
-    <t>AmplifyVision.jpg</t>
   </si>
   <si>
     <t>Lash.jpg</t>
@@ -164,6 +152,20 @@
     <t>Cost: 6 Charges.
 Activate during any player's main phase:
 Shuffle any player's turn order card into the turn order deck. That player suffers 1 damage.</t>
+  </si>
+  <si>
+    <t>Malastar</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Malastar.jpg</t>
+  </si>
+  <si>
+    <t>6 Charges.
+Activate during your main phase:
+Gain a spell from any supply pile. You may prep that spell to any player's opened breach.</t>
   </si>
   <si>
     <t>Mazahaedron</t>
@@ -178,9 +180,6 @@
 Gravehold gains 4 life.</t>
   </si>
   <si>
-    <t>Torch</t>
-  </si>
-  <si>
     <t>Mist (Dagger Captain)</t>
   </si>
   <si>
@@ -192,6 +191,9 @@
 Any ally draws 4 cards.</t>
   </si>
   <si>
+    <t>Shattered Geode</t>
+  </si>
+  <si>
     <t>Mist (Voidwalker)</t>
   </si>
   <si>
@@ -203,16 +205,10 @@
 Cast up to three different spells prepped by any number of players. For each spell cast this way, place that spell into any ally's hand.</t>
   </si>
   <si>
-    <t>Arcane Nexus</t>
-  </si>
-  <si>
     <t>Nym</t>
   </si>
   <si>
     <t>Nym.jpg</t>
-  </si>
-  <si>
-    <t>Shattered Geode</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -221,13 +217,10 @@
 If you discarded an attack card, discard an additional card.</t>
   </si>
   <si>
-    <t>ArcaneNexus.jpg</t>
+    <t>Moonstone Shard</t>
   </si>
   <si>
     <t>Phaedraxa</t>
-  </si>
-  <si>
-    <t>Aurora</t>
   </si>
   <si>
     <t>Phaedraxa.jpg</t>
@@ -238,13 +231,7 @@
 Prevent any damage that the players or Gravehold would suffer during that turn.</t>
   </si>
   <si>
-    <t>Aurora.jpg</t>
-  </si>
-  <si>
     <t>Quilius</t>
-  </si>
-  <si>
-    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Quilius.jpg</t>
@@ -255,16 +242,13 @@
 Deal 2 damage for each Trophy token you have.</t>
   </si>
   <si>
-    <t>Gem</t>
-  </si>
-  <si>
     <t>Reeve</t>
   </si>
   <si>
+    <t>Emerald Shard</t>
+  </si>
+  <si>
     <t>Reeve.jpg</t>
-  </si>
-  <si>
-    <t>BanishingTopaz.jpg</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -273,19 +257,10 @@
 Deal 3 damage to a different minion.</t>
   </si>
   <si>
-    <t>Blasting Staff</t>
-  </si>
-  <si>
     <t>Ulgimor</t>
   </si>
   <si>
     <t>Ulgimor.jpg</t>
-  </si>
-  <si>
-    <t>Relic</t>
-  </si>
-  <si>
-    <t>Moonstone Shard</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -294,13 +269,10 @@
 If you are exhausted, any ally gains 5 life instead.</t>
   </si>
   <si>
-    <t>BlastingStaff.jpg</t>
-  </si>
-  <si>
     <t>Xaxos</t>
   </si>
   <si>
-    <t>Bloodstone Jewel</t>
+    <t>Quartz Shard</t>
   </si>
   <si>
     <t>Xaxos.jpg</t>
@@ -312,13 +284,7 @@
 Reveal the turn order deck and return the revealed cards in any order.</t>
   </si>
   <si>
-    <t>BloodstoneJewel.jpg</t>
-  </si>
-  <si>
     <t>Yan Magda</t>
-  </si>
-  <si>
-    <t>Bottled Vortex</t>
   </si>
   <si>
     <t>YanMagda.jpg</t>
@@ -329,16 +295,7 @@
 Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
   </si>
   <si>
-    <t>BottledVortex.jpg</t>
-  </si>
-  <si>
-    <t>Emerald Shard</t>
-  </si>
-  <si>
     <t>Z'hana</t>
-  </si>
-  <si>
-    <t>Breach Ore</t>
   </si>
   <si>
     <t>Zhana.jpg</t>
@@ -349,6 +306,105 @@
 Gravehold gains 7 life.</t>
   </si>
   <si>
+    <t>Immolate</t>
+  </si>
+  <si>
+    <t>Worldheart Shard</t>
+  </si>
+  <si>
+    <t>Garnet Shard</t>
+  </si>
+  <si>
+    <t>Amethyst Paragon</t>
+  </si>
+  <si>
+    <t>Cinder</t>
+  </si>
+  <si>
+    <t>Tourmaline Shard</t>
+  </si>
+  <si>
+    <t>Extinguish</t>
+  </si>
+  <si>
+    <t>Obsidian Shard</t>
+  </si>
+  <si>
+    <t>Coal Shard</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>Illuminate</t>
+  </si>
+  <si>
+    <t>Eternal Ember</t>
+  </si>
+  <si>
+    <t>Amplify Vision</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>AmplifyVision.jpg</t>
+  </si>
+  <si>
+    <t>Arcane Nexus</t>
+  </si>
+  <si>
+    <t>ArcaneNexus.jpg</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>Aurora.jpg</t>
+  </si>
+  <si>
+    <t>Banishing Topaz</t>
+  </si>
+  <si>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>BanishingTopaz.jpg</t>
+  </si>
+  <si>
+    <t>Blasting Staff</t>
+  </si>
+  <si>
+    <t>Relic</t>
+  </si>
+  <si>
+    <t>BlastingStaff.jpg</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Blaze.jpg</t>
+  </si>
+  <si>
+    <t>Bloodstone Jewel</t>
+  </si>
+  <si>
+    <t>BloodstoneJewel.jpg</t>
+  </si>
+  <si>
+    <t>Bottled Vortex</t>
+  </si>
+  <si>
+    <t>BottledVortex.jpg</t>
+  </si>
+  <si>
+    <t>Breach Ore</t>
+  </si>
+  <si>
     <t>BreachOre.jpg</t>
   </si>
   <si>
@@ -361,9 +417,6 @@
     <t>Cairn Compass</t>
   </si>
   <si>
-    <t>Quartz Shard</t>
-  </si>
-  <si>
     <t>CairnCompass.jpg</t>
   </si>
   <si>
@@ -376,9 +429,6 @@
     <t>Celestial Spire</t>
   </si>
   <si>
-    <t>Worldheart Shard</t>
-  </si>
-  <si>
     <t>CelestialSpire.jpg</t>
   </si>
   <si>
@@ -391,15 +441,24 @@
     <t>Clouded Sapphire</t>
   </si>
   <si>
-    <t>Garnet Shard</t>
+    <t>Miriam</t>
   </si>
   <si>
     <t>CloudedSapphire.jpg</t>
   </si>
   <si>
+    <t>James</t>
+  </si>
+  <si>
     <t>Combustion</t>
   </si>
   <si>
+    <t>Kermit</t>
+  </si>
+  <si>
+    <t>Homura</t>
+  </si>
+  <si>
     <t>Combustion.jpg</t>
   </si>
   <si>
@@ -412,63 +471,132 @@
     <t>Conjure The Lost</t>
   </si>
   <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
     <t>ConjureTheLost.jpg</t>
   </si>
   <si>
     <t>Consuming Void</t>
   </si>
   <si>
+    <t>Blight Lord</t>
+  </si>
+  <si>
     <t>ConsumingVoid.jpg</t>
   </si>
   <si>
     <t>Convection Field</t>
   </si>
   <si>
+    <t>BlightLord.jpg</t>
+  </si>
+  <si>
     <t>ConvectionField.jpg</t>
   </si>
   <si>
     <t>Crystallize</t>
   </si>
   <si>
+    <t>Carapace Queen</t>
+  </si>
+  <si>
+    <t>CarapaceQueen.jpg</t>
+  </si>
+  <si>
+    <t>Crooked Mask</t>
+  </si>
+  <si>
     <t>Crystallize.jpg</t>
   </si>
   <si>
     <t>Dark Fire</t>
   </si>
   <si>
+    <t>CrookedMask.jpg</t>
+  </si>
+  <si>
+    <t>Gate Witch</t>
+  </si>
+  <si>
     <t>DarkFire.jpg</t>
   </si>
   <si>
+    <t>GateWitch.jpg</t>
+  </si>
+  <si>
     <t>Devouring Shadow</t>
   </si>
   <si>
+    <t>Hollow Crown</t>
+  </si>
+  <si>
+    <t>HollowCrown.jpg</t>
+  </si>
+  <si>
     <t>DevouringShadow.jpg</t>
   </si>
   <si>
+    <t>Horde Crone</t>
+  </si>
+  <si>
     <t>Diamond Cluster</t>
   </si>
   <si>
+    <t>HordeCrone.jpg</t>
+  </si>
+  <si>
+    <t>Magus Of Cloaks</t>
+  </si>
+  <si>
     <t>DiamondCluster.jpg</t>
   </si>
   <si>
+    <t>MagusOfCloaks.jpg</t>
+  </si>
+  <si>
     <t>Disintegrating Scythe</t>
   </si>
   <si>
+    <t>Prince Of Gluttons</t>
+  </si>
+  <si>
+    <t>PrinceOfGluttons.jpg</t>
+  </si>
+  <si>
     <t>DisintegratingScythe.jpg</t>
   </si>
   <si>
+    <t>RageBorne</t>
+  </si>
+  <si>
     <t>Dread Diamond</t>
   </si>
   <si>
+    <t>RageBorne.jpg</t>
+  </si>
+  <si>
+    <t>Umbra Titan</t>
+  </si>
+  <si>
     <t>DreadDiamond.jpg</t>
   </si>
   <si>
+    <t>UmbraTitan.jpg</t>
+  </si>
+  <si>
     <t>Equilibrium</t>
   </si>
   <si>
+    <t>Wayward One</t>
+  </si>
+  <si>
     <t>Equilibrium.jpg</t>
   </si>
   <si>
+    <t>WaywardOne.jpg</t>
+  </si>
+  <si>
     <t>Erratic Ingot</t>
   </si>
   <si>
@@ -484,9 +612,6 @@
     <t>Feral Lightning</t>
   </si>
   <si>
-    <t>Amethyst Paragon</t>
-  </si>
-  <si>
     <t>FeralLightning.jpg</t>
   </si>
   <si>
@@ -496,9 +621,6 @@
     <t>FiendCatcher.jpg</t>
   </si>
   <si>
-    <t>Cinder</t>
-  </si>
-  <si>
     <t>Fiery Torrent</t>
   </si>
   <si>
@@ -508,9 +630,6 @@
     <t>Flexing Dagger</t>
   </si>
   <si>
-    <t>Tourmaline Shard</t>
-  </si>
-  <si>
     <t>FlexingDagger.jpg</t>
   </si>
   <si>
@@ -526,9 +645,6 @@
     <t>FrozenMagmite.jpg</t>
   </si>
   <si>
-    <t>Extinguish</t>
-  </si>
-  <si>
     <t>Ignite</t>
   </si>
   <si>
@@ -538,9 +654,6 @@
     <t>Jade</t>
   </si>
   <si>
-    <t>Obsidian Shard</t>
-  </si>
-  <si>
     <t>Jade.jpg</t>
   </si>
   <si>
@@ -553,9 +666,6 @@
     <t>Kindle</t>
   </si>
   <si>
-    <t>Coal Shard</t>
-  </si>
-  <si>
     <t>Kindle.jpg</t>
   </si>
   <si>
@@ -565,7 +675,10 @@
     <t>LavaTendril.jpg</t>
   </si>
   <si>
-    <t>Flare</t>
+    <t>Leeching Agate</t>
+  </si>
+  <si>
+    <t>LeechingAgate.jpg</t>
   </si>
   <si>
     <t>Mage's Talisman</t>
@@ -580,21 +693,21 @@
     <t>MagesTotem.jpg</t>
   </si>
   <si>
-    <t>Illuminate</t>
-  </si>
-  <si>
     <t>Monstrous Inferno</t>
   </si>
   <si>
     <t>MonstrousInferno.jpg</t>
   </si>
   <si>
+    <t>Molten Hammer</t>
+  </si>
+  <si>
+    <t>MoltenHammer.jpg</t>
+  </si>
+  <si>
     <t>Nova Forge</t>
   </si>
   <si>
-    <t>Eternal Ember</t>
-  </si>
-  <si>
     <t>NovaForge.jpg</t>
   </si>
   <si>
@@ -625,28 +738,25 @@
     <t>Pyrotechnic Surge</t>
   </si>
   <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
     <t>PyrotechnicSurge.jpg</t>
   </si>
   <si>
-    <t>Carapace Queen</t>
+    <t>Radiance</t>
+  </si>
+  <si>
+    <t>Radiance.jpg</t>
   </si>
   <si>
     <t>Reduce To Ash</t>
   </si>
   <si>
-    <t>CarapaceQueen.jpg</t>
-  </si>
-  <si>
-    <t>Crooked Mask</t>
-  </si>
-  <si>
     <t>ReduceToAsh.jpg</t>
   </si>
   <si>
-    <t>CrookedMask.jpg</t>
+    <t>Sage's Brand</t>
+  </si>
+  <si>
+    <t>SagesBrand.jpg</t>
   </si>
   <si>
     <t>Scoria Slag</t>
@@ -655,85 +765,91 @@
     <t>ScoriaSlag.jpg</t>
   </si>
   <si>
-    <t>Gate Witch</t>
+    <t>Scrying Bolt</t>
+  </si>
+  <si>
+    <t>ScryingBolt.jpg</t>
   </si>
   <si>
     <t>Searing Ruby</t>
   </si>
   <si>
-    <t>GateWitch.jpg</t>
-  </si>
-  <si>
-    <t>Hollow Crown</t>
-  </si>
-  <si>
     <t>SearingRuby.jpg</t>
   </si>
   <si>
-    <t>HollowCrown.jpg</t>
-  </si>
-  <si>
     <t>Sifter's Pearl</t>
   </si>
   <si>
-    <t>Horde Crone</t>
-  </si>
-  <si>
-    <t>HordeCrone.jpg</t>
-  </si>
-  <si>
     <t>SiftersPearl.jpg</t>
   </si>
   <si>
-    <t>Magus Of Cloaks</t>
-  </si>
-  <si>
     <t>Spectral Echo</t>
   </si>
   <si>
-    <t>MagusOfCloaks.jpg</t>
-  </si>
-  <si>
-    <t>Prince Of Gluttons</t>
-  </si>
-  <si>
     <t>SpectralEcho.jpg</t>
   </si>
   <si>
-    <t>PrinceOfGluttons.jpg</t>
-  </si>
-  <si>
-    <t>RageBorne</t>
+    <t>Temporal Helix</t>
+  </si>
+  <si>
+    <t>TemporalHelix.jpg</t>
   </si>
   <si>
     <t>Thoughtform Familiar</t>
   </si>
   <si>
-    <t>RageBorne.jpg</t>
-  </si>
-  <si>
-    <t>Umbra Titan</t>
-  </si>
-  <si>
     <t>ThoughtformFamiliar.jpg</t>
   </si>
   <si>
-    <t>UmbraTitan.jpg</t>
+    <t>Date</t>
   </si>
   <si>
     <t>Transmogrifier</t>
   </si>
   <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Mage 1</t>
+  </si>
+  <si>
     <t>Transmogrifier.jpg</t>
   </si>
   <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Mage 2</t>
+  </si>
+  <si>
     <t>Unstable Prism</t>
   </si>
   <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>Nemesis</t>
+  </si>
+  <si>
     <t>UnstablePrism.jpg</t>
   </si>
   <si>
+    <t>Market Card 1</t>
+  </si>
+  <si>
+    <t>Market Card 2</t>
+  </si>
+  <si>
     <t>V'riswood Amber</t>
+  </si>
+  <si>
+    <t>Market Card 3</t>
+  </si>
+  <si>
+    <t>Market Card 4</t>
+  </si>
+  <si>
+    <t>Market Card 5</t>
   </si>
   <si>
     <t>VriswoodAmber.jpg</t>
@@ -788,20 +904,8 @@
 Cast: Gain 2 Aether.</t>
   </si>
   <si>
-    <t>Miriam</t>
-  </si>
-  <si>
     <t>If you have 2 life or less, destroy this.
 Otherwise, gain 3 Aether, gain 1 charge, and suffer 2 damage.</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Kermit</t>
-  </si>
-  <si>
-    <t>Homura</t>
   </si>
   <si>
     <t>Gain 1 Aether 
@@ -814,8 +918,23 @@
 Cast: Cast one of your prepped spells without discarding it.</t>
   </si>
   <si>
+    <t>Market Card 6</t>
+  </si>
+  <si>
+    <t>Market Card 7</t>
+  </si>
+  <si>
+    <t>Market Card 8</t>
+  </si>
+  <si>
+    <t>Market Card 9</t>
+  </si>
+  <si>
     <t>Cast: Deal 1 damage.
 If this damage causes a minion from the nemesis deck to be discarded, Quilius gains a Trophy token.</t>
+  </si>
+  <si>
+    <t>2017/11/12 5:30PM PST</t>
   </si>
   <si>
     <t>Cast: Reveal the top card of the turn order deck, and then place it back on top of the turn order deck. If you revealed a player turn order card, deal 3 damage. Otherwise deal 1 damage.</t>
@@ -830,6 +949,13 @@
 Cast: Deal 1 damage.</t>
   </si>
   <si>
+    <t>While prepped, when you suffer damage cain 1 charge.
+Cast: Deal 1 damage.</t>
+  </si>
+  <si>
+    <t>2017/11/12 7:00PM PST</t>
+  </si>
+  <si>
     <t>Gain 1 Aether.
 Gain an additional 1 Aether that can only be used to gain a gem.</t>
   </si>
@@ -837,6 +963,9 @@
     <t>Gain 2 Aether that cannot be used to gain a relic or spell.</t>
   </si>
   <si>
+    <t>2017/11/12 9:00PM PST</t>
+  </si>
+  <si>
     <t>Gain 1 Aether.
 You may suffer 1 damage. If you do, gain an additional 2 Aether.</t>
   </si>
@@ -847,6 +976,9 @@
   <si>
     <t>Gain 1 Aether.
 You may place the top card of any ally's discard pile into your hand.</t>
+  </si>
+  <si>
+    <t>2017/11/10 7:00PM PST</t>
   </si>
   <si>
     <t>Cast: Deal 1 damage.
@@ -858,78 +990,18 @@
 Any ally may suffer 1 damage. If they do, they destroy a card in hand.</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Player 1</t>
-  </si>
-  <si>
-    <t>Mage 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
-  </si>
-  <si>
-    <t>Mage 2</t>
-  </si>
-  <si>
-    <t>Won</t>
-  </si>
-  <si>
     <t>Gain 1 Aether.
 OR
 Gain 2 Aether that can only be used to gain a card. Place the next card you gain this turn on top of any ally's discard pile.</t>
   </si>
   <si>
-    <t>Nemesis</t>
-  </si>
-  <si>
-    <t>Market Card 1</t>
+    <t>2017/11/10 9:00PM PST</t>
   </si>
   <si>
     <t>Common</t>
   </si>
   <si>
-    <t>Market Card 2</t>
-  </si>
-  <si>
     <t>Crystal.png</t>
-  </si>
-  <si>
-    <t>Market Card 3</t>
-  </si>
-  <si>
-    <t>Market Card 4</t>
-  </si>
-  <si>
-    <t>Market Card 5</t>
-  </si>
-  <si>
-    <t>Market Card 6</t>
-  </si>
-  <si>
-    <t>Market Card 7</t>
-  </si>
-  <si>
-    <t>Market Card 8</t>
-  </si>
-  <si>
-    <t>Market Card 9</t>
-  </si>
-  <si>
-    <t>2017/11/12 5:30PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/12 7:00PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/12 9:00PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/10 7:00PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/10 9:00PM PST</t>
   </si>
 </sst>
 </file>
@@ -1047,1411 +1119,1548 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1">
         <v>7.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B8" s="1">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B10" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B11" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1">
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B13" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B15" s="1">
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B16" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B17" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B18" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="B19" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B21" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B22" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="B23" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="B24" s="1">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="B25" s="1">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="B27" s="1">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="B28" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="B29" s="1">
         <v>5.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="B31" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="B32" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="B33" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="B34" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="B35" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="B36" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="B37" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="B38" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="B39" s="1">
         <v>4.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="B40" s="1">
         <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="B41" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B42" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>171</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" s="1"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="B43" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="B44" s="1">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="B45" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="B46" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>181</v>
+        <v>94</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="B47" s="1">
         <v>6.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
       <c r="B48" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="B49" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="B50" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="B51" s="1">
         <v>4.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="B52" s="1">
         <v>4.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="B53" s="1">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>206</v>
+        <v>94</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="B54" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="B55" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>217</v>
+        <v>94</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="B56" s="1">
         <v>4.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B57" s="1">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>222</v>
+        <v>94</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="B58" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="B59" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="B60" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B61" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>230</v>
+        <v>94</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="B62" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="B63" s="1">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>252</v>
       </c>
       <c r="B64" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>236</v>
+        <v>94</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>20</v>
+        <v>258</v>
       </c>
       <c r="B65" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>237</v>
+        <v>94</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="B66" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>238</v>
+        <v>94</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>144</v>
+        <v>265</v>
       </c>
       <c r="B67" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>239</v>
+        <v>94</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>163</v>
+        <v>267</v>
       </c>
       <c r="B68" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>241</v>
+        <v>94</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>269</v>
       </c>
       <c r="B69" s="1">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>245</v>
+        <v>94</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>176</v>
+        <v>271</v>
       </c>
       <c r="B70" s="1">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>246</v>
+        <v>94</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="B71" s="1">
         <v>0.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>167</v>
+        <v>20</v>
       </c>
       <c r="B72" s="1">
         <v>0.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="B73" s="1">
         <v>0.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>172</v>
+        <v>84</v>
       </c>
       <c r="B74" s="1">
         <v>0.0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B75" s="1">
         <v>0.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B76" s="1">
         <v>0.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="B77" s="1">
         <v>0.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B78" s="1">
         <v>0.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B79" s="1">
         <v>0.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B80" s="1">
         <v>0.0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>256</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="B81" s="1">
         <v>0.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1">
         <v>0.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B83" s="1">
         <v>0.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B84" s="1">
         <v>0.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2502,7 +2711,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -2529,7 +2738,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -2551,145 +2760,156 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2738,7 +2958,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -2775,7 +2995,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -2787,7 +3007,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -2811,7 +3031,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -2823,7 +3043,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>1.0</v>
@@ -2848,7 +3068,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1">
         <v>3.0</v>
@@ -2860,7 +3080,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
@@ -2869,7 +3089,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -2881,10 +3101,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <v>2.0</v>
@@ -2893,10 +3113,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -2920,7 +3140,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1">
         <v>4.0</v>
@@ -2932,7 +3152,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1">
         <v>1.0</v>
@@ -2941,7 +3161,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>12</v>
@@ -2953,10 +3173,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1">
         <v>3.0</v>
@@ -2965,10 +3185,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1">
         <v>1.0</v>
@@ -2977,7 +3197,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>12</v>
@@ -2989,10 +3209,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1">
         <v>3.0</v>
@@ -3001,10 +3221,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -3013,34 +3233,34 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="1">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1">
         <v>1.0</v>
@@ -3049,7 +3269,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>12</v>
@@ -3061,29 +3281,31 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1">
         <v>3.0</v>
       </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="C31" s="1">
         <v>1.0</v>
       </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>12</v>
@@ -3091,13 +3313,14 @@
       <c r="C32" s="1">
         <v>6.0</v>
       </c>
+      <c r="E32" s="1"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1">
         <v>3.0</v>
@@ -3105,10 +3328,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1">
         <v>1.0</v>
@@ -3116,32 +3339,32 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C36" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1">
         <v>1.0</v>
@@ -3149,7 +3372,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>12</v>
@@ -3160,10 +3383,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1">
         <v>2.0</v>
@@ -3171,10 +3394,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="C40" s="1">
         <v>1.0</v>
@@ -3182,21 +3405,21 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1">
         <v>2.0</v>
@@ -3204,51 +3427,51 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="C43" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>12</v>
@@ -3259,10 +3482,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C48" s="1">
         <v>4.0</v>
@@ -3270,10 +3493,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>163</v>
+        <v>87</v>
       </c>
       <c r="C49" s="1">
         <v>1.0</v>
@@ -3281,32 +3504,32 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C51" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="C52" s="1">
         <v>1.0</v>
@@ -3314,7 +3537,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>12</v>
@@ -3325,10 +3548,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C54" s="1">
         <v>1.0</v>
@@ -3336,10 +3559,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="C55" s="1">
         <v>1.0</v>
@@ -3347,7 +3570,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>12</v>
@@ -3358,10 +3581,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C57" s="1">
         <v>1.0</v>
@@ -3369,12 +3592,45 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C58" s="1">
+      <c r="C61" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -3402,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -3410,101 +3666,123 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
+        <v>4.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>144</v>
       </c>
       <c r="B3" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="B4" s="1">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B7" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="B8" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>216</v>
+        <v>167</v>
       </c>
       <c r="B10" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="1">
         <v>3.0</v>
       </c>
-      <c r="C10" t="s">
-        <v>218</v>
+      <c r="C11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3526,22 +3804,22 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>242</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>243</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>244</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3561,70 +3839,70 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -3636,48 +3914,48 @@
         <v>10.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -3689,48 +3967,48 @@
         <v>10.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -3742,51 +4020,51 @@
         <v>8.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -3795,51 +4073,51 @@
         <v>10.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>231</v>
+        <v>269</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>240</v>
+        <v>129</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -3848,34 +4126,34 @@
         <v>8.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>231</v>
+        <v>269</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix spacing of the mage ability. Run rake db:reset.
</commit_message>
<xml_diff>
--- a/lib/seeds/Aeon's End Database.xlsx
+++ b/lib/seeds/Aeon's End Database.xlsx
@@ -16,45 +16,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Adelheim</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>Image Name</t>
+  </si>
+  <si>
+    <t>Ability</t>
+  </si>
+  <si>
+    <t>Amethyst Shard</t>
+  </si>
+  <si>
     <t>Cost</t>
   </si>
   <si>
+    <t>Adelheim.jpg</t>
+  </si>
+  <si>
+    <t>Brama</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
     <t>Category</t>
   </si>
   <si>
-    <t>Image Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Mage</t>
-  </si>
-  <si>
-    <t>Ability</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Adelheim</t>
-  </si>
-  <si>
-    <t>Adelheim.jpg</t>
-  </si>
-  <si>
-    <t>Crystal</t>
+    <t>Amplify Vision</t>
+  </si>
+  <si>
+    <t>Buried Light</t>
+  </si>
+  <si>
+    <t>Dezmodia</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -62,13 +80,10 @@
 When a nemesis attack or power card is drawn but before it is resolved, you may discard it. It has no effect.</t>
   </si>
   <si>
-    <t>Brama</t>
-  </si>
-  <si>
     <t>Brama.jpg</t>
   </si>
   <si>
-    <t>Spark</t>
+    <t>Spell</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -76,13 +91,13 @@
 Any player gains 4 life.</t>
   </si>
   <si>
-    <t>Dezmodia</t>
+    <t>Market</t>
   </si>
   <si>
     <t>Dezmodia.jpg</t>
   </si>
   <si>
-    <t>Amethyst Shard</t>
+    <t>AmplifyVision.jpg</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -94,6 +109,9 @@
   </si>
   <si>
     <t>Garu.jpg</t>
+  </si>
+  <si>
+    <t>Oblivion Shard</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -102,10 +120,10 @@
 Deal 2 damage plus 4 additional damage for each spell you discarded divided however you choose to the nemesis or any number of minions</t>
   </si>
   <si>
+    <t>Torch</t>
+  </si>
+  <si>
     <t>Gex</t>
-  </si>
-  <si>
-    <t>Buried Light</t>
   </si>
   <si>
     <t>Gex.jpg</t>
@@ -129,19 +147,13 @@
 Then cast that prepped spell again.</t>
   </si>
   <si>
-    <t>Amplify Vision</t>
+    <t>Shattered Geode</t>
   </si>
   <si>
     <t>Kadir</t>
   </si>
   <si>
     <t>Kadir.jpg</t>
-  </si>
-  <si>
-    <t>Oblivion Shard</t>
-  </si>
-  <si>
-    <t>Spell</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -149,16 +161,13 @@
 That player may return up to three spells in their discard pile to their hand. That player may prep up to two spells to each of their opened breaches this turn.</t>
   </si>
   <si>
-    <t>Market</t>
-  </si>
-  <si>
     <t>Lash</t>
   </si>
   <si>
-    <t>AmplifyVision.jpg</t>
-  </si>
-  <si>
     <t>Lash.jpg</t>
+  </si>
+  <si>
+    <t>Arcane Nexus</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -166,10 +175,36 @@
 Shuffle any player's turn order card into the turn order deck. That player suffers 1 damage.</t>
   </si>
   <si>
+    <t>Malastar</t>
+  </si>
+  <si>
+    <t>Moonstone Shard</t>
+  </si>
+  <si>
+    <t>ArcaneNexus.jpg</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>Malastar.jpg</t>
+  </si>
+  <si>
+    <t>6 Charges.
+Activate during your main phase:
+Gain a spell from any supply pile. You may prep that spell to any player's opened breach.</t>
+  </si>
+  <si>
+    <t>Aurora.jpg</t>
+  </si>
+  <si>
     <t>Mazahaedron</t>
   </si>
   <si>
     <t>Mazahaedron.jpg</t>
+  </si>
+  <si>
+    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -178,13 +213,19 @@
 Gravehold gains 4 life.</t>
   </si>
   <si>
-    <t>Torch</t>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>Emerald Shard</t>
   </si>
   <si>
     <t>Mist (Dagger Captain)</t>
   </si>
   <si>
     <t>Mist.jpg</t>
+  </si>
+  <si>
+    <t>BanishingTopaz.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -195,6 +236,9 @@
     <t>Mist (Voidwalker)</t>
   </si>
   <si>
+    <t>Blasting Staff</t>
+  </si>
+  <si>
     <t>MistWE.jpg</t>
   </si>
   <si>
@@ -203,7 +247,7 @@
 Cast up to three different spells prepped by any number of players. For each spell cast this way, place that spell into any ally's hand.</t>
   </si>
   <si>
-    <t>Arcane Nexus</t>
+    <t>Relic</t>
   </si>
   <si>
     <t>Nym</t>
@@ -212,7 +256,7 @@
     <t>Nym.jpg</t>
   </si>
   <si>
-    <t>Shattered Geode</t>
+    <t>BlastingStaff.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -221,16 +265,16 @@
 If you discarded an attack card, discard an additional card.</t>
   </si>
   <si>
-    <t>ArcaneNexus.jpg</t>
-  </si>
-  <si>
     <t>Phaedraxa</t>
   </si>
   <si>
-    <t>Aurora</t>
+    <t>Blaze</t>
   </si>
   <si>
     <t>Phaedraxa.jpg</t>
+  </si>
+  <si>
+    <t>Quartz Shard</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -238,16 +282,13 @@
 Prevent any damage that the players or Gravehold would suffer during that turn.</t>
   </si>
   <si>
-    <t>Aurora.jpg</t>
-  </si>
-  <si>
     <t>Quilius</t>
   </si>
   <si>
-    <t>Banishing Topaz</t>
-  </si>
-  <si>
     <t>Quilius.jpg</t>
+  </si>
+  <si>
+    <t>Blaze.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -255,16 +296,13 @@
 Deal 2 damage for each Trophy token you have.</t>
   </si>
   <si>
-    <t>Gem</t>
-  </si>
-  <si>
     <t>Reeve</t>
   </si>
   <si>
     <t>Reeve.jpg</t>
   </si>
   <si>
-    <t>BanishingTopaz.jpg</t>
+    <t>Bloodstone Jewel</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -273,19 +311,13 @@
 Deal 3 damage to a different minion.</t>
   </si>
   <si>
-    <t>Blasting Staff</t>
-  </si>
-  <si>
     <t>Ulgimor</t>
   </si>
   <si>
     <t>Ulgimor.jpg</t>
   </si>
   <si>
-    <t>Relic</t>
-  </si>
-  <si>
-    <t>Moonstone Shard</t>
+    <t>BloodstoneJewel.jpg</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -294,13 +326,13 @@
 If you are exhausted, any ally gains 5 life instead.</t>
   </si>
   <si>
-    <t>BlastingStaff.jpg</t>
+    <t>Immolate</t>
   </si>
   <si>
     <t>Xaxos</t>
   </si>
   <si>
-    <t>Bloodstone Jewel</t>
+    <t>Bottled Vortex</t>
   </si>
   <si>
     <t>Xaxos.jpg</t>
@@ -312,16 +344,13 @@
 Reveal the turn order deck and return the revealed cards in any order.</t>
   </si>
   <si>
-    <t>BloodstoneJewel.jpg</t>
-  </si>
-  <si>
     <t>Yan Magda</t>
   </si>
   <si>
-    <t>Bottled Vortex</t>
-  </si>
-  <si>
     <t>YanMagda.jpg</t>
+  </si>
+  <si>
+    <t>BottledVortex.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -329,12 +358,6 @@
 Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
   </si>
   <si>
-    <t>BottledVortex.jpg</t>
-  </si>
-  <si>
-    <t>Emerald Shard</t>
-  </si>
-  <si>
     <t>Z'hana</t>
   </si>
   <si>
@@ -355,15 +378,15 @@
     <t>Burning Opal</t>
   </si>
   <si>
+    <t>Worldheart Shard</t>
+  </si>
+  <si>
     <t>BurningOpal.jpg</t>
   </si>
   <si>
     <t>Cairn Compass</t>
   </si>
   <si>
-    <t>Quartz Shard</t>
-  </si>
-  <si>
     <t>CairnCompass.jpg</t>
   </si>
   <si>
@@ -376,7 +399,7 @@
     <t>Celestial Spire</t>
   </si>
   <si>
-    <t>Worldheart Shard</t>
+    <t>Garnet Shard</t>
   </si>
   <si>
     <t>CelestialSpire.jpg</t>
@@ -388,18 +411,21 @@
     <t>ChaosArc.jpg</t>
   </si>
   <si>
+    <t>Amethyst Paragon</t>
+  </si>
+  <si>
     <t>Clouded Sapphire</t>
   </si>
   <si>
-    <t>Garnet Shard</t>
-  </si>
-  <si>
     <t>CloudedSapphire.jpg</t>
   </si>
   <si>
     <t>Combustion</t>
   </si>
   <si>
+    <t>Cinder</t>
+  </si>
+  <si>
     <t>Combustion.jpg</t>
   </si>
   <si>
@@ -412,6 +438,9 @@
     <t>Conjure The Lost</t>
   </si>
   <si>
+    <t>Tourmaline Shard</t>
+  </si>
+  <si>
     <t>ConjureTheLost.jpg</t>
   </si>
   <si>
@@ -427,6 +456,9 @@
     <t>ConvectionField.jpg</t>
   </si>
   <si>
+    <t>Extinguish</t>
+  </si>
+  <si>
     <t>Crystallize</t>
   </si>
   <si>
@@ -436,6 +468,9 @@
     <t>Dark Fire</t>
   </si>
   <si>
+    <t>Obsidian Shard</t>
+  </si>
+  <si>
     <t>DarkFire.jpg</t>
   </si>
   <si>
@@ -448,6 +483,9 @@
     <t>Diamond Cluster</t>
   </si>
   <si>
+    <t>Coal Shard</t>
+  </si>
+  <si>
     <t>DiamondCluster.jpg</t>
   </si>
   <si>
@@ -457,6 +495,9 @@
     <t>DisintegratingScythe.jpg</t>
   </si>
   <si>
+    <t>Flare</t>
+  </si>
+  <si>
     <t>Dread Diamond</t>
   </si>
   <si>
@@ -466,6 +507,9 @@
     <t>Equilibrium</t>
   </si>
   <si>
+    <t>Illuminate</t>
+  </si>
+  <si>
     <t>Equilibrium.jpg</t>
   </si>
   <si>
@@ -478,15 +522,15 @@
     <t>Essence Theft</t>
   </si>
   <si>
+    <t>Eternal Ember</t>
+  </si>
+  <si>
     <t>EssenceTheft.jpg</t>
   </si>
   <si>
     <t>Feral Lightning</t>
   </si>
   <si>
-    <t>Amethyst Paragon</t>
-  </si>
-  <si>
     <t>FeralLightning.jpg</t>
   </si>
   <si>
@@ -496,9 +540,6 @@
     <t>FiendCatcher.jpg</t>
   </si>
   <si>
-    <t>Cinder</t>
-  </si>
-  <si>
     <t>Fiery Torrent</t>
   </si>
   <si>
@@ -508,9 +549,6 @@
     <t>Flexing Dagger</t>
   </si>
   <si>
-    <t>Tourmaline Shard</t>
-  </si>
-  <si>
     <t>FlexingDagger.jpg</t>
   </si>
   <si>
@@ -526,9 +564,6 @@
     <t>FrozenMagmite.jpg</t>
   </si>
   <si>
-    <t>Extinguish</t>
-  </si>
-  <si>
     <t>Ignite</t>
   </si>
   <si>
@@ -538,9 +573,6 @@
     <t>Jade</t>
   </si>
   <si>
-    <t>Obsidian Shard</t>
-  </si>
-  <si>
     <t>Jade.jpg</t>
   </si>
   <si>
@@ -553,9 +585,6 @@
     <t>Kindle</t>
   </si>
   <si>
-    <t>Coal Shard</t>
-  </si>
-  <si>
     <t>Kindle.jpg</t>
   </si>
   <si>
@@ -565,7 +594,10 @@
     <t>LavaTendril.jpg</t>
   </si>
   <si>
-    <t>Flare</t>
+    <t>Leeching Agate</t>
+  </si>
+  <si>
+    <t>LeechingAgate.jpg</t>
   </si>
   <si>
     <t>Mage's Talisman</t>
@@ -580,24 +612,42 @@
     <t>MagesTotem.jpg</t>
   </si>
   <si>
-    <t>Illuminate</t>
-  </si>
-  <si>
     <t>Monstrous Inferno</t>
   </si>
   <si>
     <t>MonstrousInferno.jpg</t>
   </si>
   <si>
+    <t>Molten Hammer</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>MoltenHammer.jpg</t>
+  </si>
+  <si>
+    <t>Blight Lord</t>
+  </si>
+  <si>
     <t>Nova Forge</t>
   </si>
   <si>
-    <t>Eternal Ember</t>
+    <t>BlightLord.jpg</t>
   </si>
   <si>
     <t>NovaForge.jpg</t>
   </si>
   <si>
+    <t>Carapace Queen</t>
+  </si>
+  <si>
+    <t>CarapaceQueen.jpg</t>
+  </si>
+  <si>
+    <t>Crooked Mask</t>
+  </si>
+  <si>
     <t>Oblivion Swell</t>
   </si>
   <si>
@@ -616,111 +666,129 @@
     <t>PlanarInsight.jpg</t>
   </si>
   <si>
+    <t>CrookedMask.jpg</t>
+  </si>
+  <si>
     <t>Primordial Fetish</t>
   </si>
   <si>
     <t>PrimordialFetish.jpg</t>
   </si>
   <si>
+    <t>Gate Witch</t>
+  </si>
+  <si>
     <t>Pyrotechnic Surge</t>
   </si>
   <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
     <t>PyrotechnicSurge.jpg</t>
   </si>
   <si>
-    <t>Carapace Queen</t>
+    <t>GateWitch.jpg</t>
+  </si>
+  <si>
+    <t>Radiance</t>
+  </si>
+  <si>
+    <t>Hollow Crown</t>
+  </si>
+  <si>
+    <t>Radiance.jpg</t>
   </si>
   <si>
     <t>Reduce To Ash</t>
   </si>
   <si>
-    <t>CarapaceQueen.jpg</t>
-  </si>
-  <si>
-    <t>Crooked Mask</t>
+    <t>HollowCrown.jpg</t>
   </si>
   <si>
     <t>ReduceToAsh.jpg</t>
   </si>
   <si>
-    <t>CrookedMask.jpg</t>
+    <t>Horde Crone</t>
+  </si>
+  <si>
+    <t>Sage's Brand</t>
+  </si>
+  <si>
+    <t>SagesBrand.jpg</t>
+  </si>
+  <si>
+    <t>HordeCrone.jpg</t>
   </si>
   <si>
     <t>Scoria Slag</t>
   </si>
   <si>
+    <t>Magus Of Cloaks</t>
+  </si>
+  <si>
     <t>ScoriaSlag.jpg</t>
   </si>
   <si>
-    <t>Gate Witch</t>
+    <t>MagusOfCloaks.jpg</t>
+  </si>
+  <si>
+    <t>Scrying Bolt</t>
+  </si>
+  <si>
+    <t>Prince Of Gluttons</t>
+  </si>
+  <si>
+    <t>PrinceOfGluttons.jpg</t>
+  </si>
+  <si>
+    <t>ScryingBolt.jpg</t>
+  </si>
+  <si>
+    <t>RageBorne</t>
   </si>
   <si>
     <t>Searing Ruby</t>
   </si>
   <si>
-    <t>GateWitch.jpg</t>
-  </si>
-  <si>
-    <t>Hollow Crown</t>
+    <t>RageBorne.jpg</t>
+  </si>
+  <si>
+    <t>Umbra Titan</t>
+  </si>
+  <si>
+    <t>UmbraTitan.jpg</t>
   </si>
   <si>
     <t>SearingRuby.jpg</t>
   </si>
   <si>
-    <t>HollowCrown.jpg</t>
-  </si>
-  <si>
     <t>Sifter's Pearl</t>
   </si>
   <si>
-    <t>Horde Crone</t>
-  </si>
-  <si>
-    <t>HordeCrone.jpg</t>
+    <t>Wayward One</t>
+  </si>
+  <si>
+    <t>WaywardOne.jpg</t>
   </si>
   <si>
     <t>SiftersPearl.jpg</t>
   </si>
   <si>
-    <t>Magus Of Cloaks</t>
-  </si>
-  <si>
     <t>Spectral Echo</t>
   </si>
   <si>
-    <t>MagusOfCloaks.jpg</t>
-  </si>
-  <si>
-    <t>Prince Of Gluttons</t>
-  </si>
-  <si>
     <t>SpectralEcho.jpg</t>
   </si>
   <si>
-    <t>PrinceOfGluttons.jpg</t>
-  </si>
-  <si>
-    <t>RageBorne</t>
+    <t>Temporal Helix</t>
+  </si>
+  <si>
+    <t>TemporalHelix.jpg</t>
   </si>
   <si>
     <t>Thoughtform Familiar</t>
   </si>
   <si>
-    <t>RageBorne.jpg</t>
-  </si>
-  <si>
-    <t>Umbra Titan</t>
-  </si>
-  <si>
     <t>ThoughtformFamiliar.jpg</t>
   </si>
   <si>
-    <t>UmbraTitan.jpg</t>
-  </si>
-  <si>
     <t>Transmogrifier</t>
   </si>
   <si>
@@ -751,13 +819,25 @@
     <t>VoidBond.jpg</t>
   </si>
   <si>
+    <t>Miriam</t>
+  </si>
+  <si>
     <t>Volcanic Glass</t>
   </si>
   <si>
+    <t>James</t>
+  </si>
+  <si>
     <t>VolcanicGlass.jpg</t>
   </si>
   <si>
+    <t>Kermit</t>
+  </si>
+  <si>
     <t>Vortex Gauntlet</t>
+  </si>
+  <si>
+    <t>Homura</t>
   </si>
   <si>
     <t>VortexGauntlet.jpg</t>
@@ -788,24 +868,12 @@
 Cast: Gain 2 Aether.</t>
   </si>
   <si>
-    <t>Miriam</t>
-  </si>
-  <si>
     <t>If you have 2 life or less, destroy this.
 Otherwise, gain 3 Aether, gain 1 charge, and suffer 2 damage.</t>
   </si>
   <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Kermit</t>
-  </si>
-  <si>
-    <t>Homura</t>
-  </si>
-  <si>
     <t>Gain 1 Aether 
-OR 
+OR
 Any player gains 1 life.</t>
   </si>
   <si>
@@ -830,6 +898,10 @@
 Cast: Deal 1 damage.</t>
   </si>
   <si>
+    <t>While prepped, when you suffer damage cain 1 charge.
+Cast: Deal 1 damage.</t>
+  </si>
+  <si>
     <t>Gain 1 Aether.
 Gain an additional 1 Aether that can only be used to gain a gem.</t>
   </si>
@@ -858,42 +930,42 @@
 Any ally may suffer 1 damage. If they do, they destroy a card in hand.</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Player 1</t>
-  </si>
-  <si>
-    <t>Mage 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
-  </si>
-  <si>
-    <t>Mage 2</t>
-  </si>
-  <si>
-    <t>Won</t>
-  </si>
-  <si>
     <t>Gain 1 Aether.
 OR
 Gain 2 Aether that can only be used to gain a card. Place the next card you gain this turn on top of any ally's discard pile.</t>
   </si>
   <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Crystal.png</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Mage 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Mage 2</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
     <t>Nemesis</t>
   </si>
   <si>
     <t>Market Card 1</t>
   </si>
   <si>
-    <t>Common</t>
-  </si>
-  <si>
     <t>Market Card 2</t>
-  </si>
-  <si>
-    <t>Crystal.png</t>
   </si>
   <si>
     <t>Market Card 3</t>
@@ -1030,921 +1102,922 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1">
         <v>7.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>84</v>
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B10" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1">
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B13" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B14" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1">
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B16" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B18" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B19" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B20" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B21" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B22" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B24" s="1">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B25" s="1">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B26" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B27" s="1">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B28" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B29" s="1">
         <v>5.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B31" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B32" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B33" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B35" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B36" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B37" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B38" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B39" s="1">
         <v>4.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B40" s="1">
         <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B41" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B42" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>171</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F42" s="1"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B43" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B44" s="1">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B45" s="1">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B46" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>181</v>
+        <v>23</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B47" s="1">
         <v>6.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B48" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B49" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B51" s="1">
         <v>4.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B52" s="1">
         <v>4.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B53" s="1">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>206</v>
+        <v>23</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B54" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55">
@@ -1952,33 +2025,33 @@
         <v>214</v>
       </c>
       <c r="B55" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>217</v>
+        <v>23</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B56" s="1">
         <v>4.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57">
@@ -1986,472 +2059,608 @@
         <v>221</v>
       </c>
       <c r="B57" s="1">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>222</v>
+        <v>23</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B58" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B59" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B60" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="B61" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>230</v>
+        <v>23</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B62" s="1">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B63" s="1">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>243</v>
       </c>
       <c r="B64" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>236</v>
+        <v>23</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>20</v>
+        <v>245</v>
       </c>
       <c r="B65" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>237</v>
+        <v>23</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>26</v>
+        <v>247</v>
       </c>
       <c r="B66" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>238</v>
+        <v>23</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>144</v>
+        <v>249</v>
       </c>
       <c r="B67" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>239</v>
+        <v>23</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>163</v>
+        <v>252</v>
       </c>
       <c r="B68" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>241</v>
+        <v>23</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>256</v>
       </c>
       <c r="B69" s="1">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>245</v>
+        <v>23</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
       <c r="B70" s="1">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>246</v>
+        <v>23</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="B71" s="1">
         <v>0.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="B72" s="1">
         <v>0.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="B73" s="1">
         <v>0.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="B74" s="1">
         <v>0.0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="B75" s="1">
         <v>0.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B76" s="1">
         <v>0.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B77" s="1">
         <v>0.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="B78" s="1">
         <v>0.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>56</v>
+        <v>143</v>
       </c>
       <c r="B79" s="1">
         <v>0.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B80" s="1">
         <v>0.0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B81" s="1">
         <v>0.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B82" s="1">
         <v>0.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B83" s="1">
         <v>0.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B84" s="1">
         <v>0.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2477,32 +2686,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -2510,186 +2719,197 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2709,23 +2929,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>7.0</v>
@@ -2735,10 +2955,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -2748,10 +2968,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
@@ -2760,10 +2980,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>7.0</v>
@@ -2772,10 +2992,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -2784,10 +3004,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -2799,7 +3019,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>6.0</v>
@@ -2811,7 +3031,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -2823,7 +3043,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1">
         <v>1.0</v>
@@ -2832,10 +3052,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>6.0</v>
@@ -2845,10 +3065,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
         <v>3.0</v>
@@ -2857,10 +3077,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
@@ -2869,10 +3089,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>7.0</v>
@@ -2881,10 +3101,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>2.0</v>
@@ -2893,10 +3113,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -2905,10 +3125,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>5.0</v>
@@ -2917,10 +3137,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>4.0</v>
@@ -2929,10 +3149,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1">
         <v>1.0</v>
@@ -2941,10 +3161,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>6.0</v>
@@ -2953,10 +3173,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>3.0</v>
@@ -2965,10 +3185,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1">
         <v>1.0</v>
@@ -2977,10 +3197,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
         <v>6.0</v>
@@ -2989,10 +3209,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>3.0</v>
@@ -3001,10 +3221,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -3013,34 +3233,34 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C28" s="1">
         <v>1.0</v>
@@ -3049,10 +3269,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1">
         <v>6.0</v>
@@ -3061,43 +3281,46 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
         <v>3.0</v>
       </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C31" s="1">
         <v>1.0</v>
       </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1">
         <v>6.0</v>
       </c>
+      <c r="E32" s="1"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1">
         <v>3.0</v>
@@ -3105,10 +3328,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C34" s="1">
         <v>1.0</v>
@@ -3116,32 +3339,32 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="C37" s="1">
         <v>1.0</v>
@@ -3149,10 +3372,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C38" s="1">
         <v>7.0</v>
@@ -3160,10 +3383,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C39" s="1">
         <v>2.0</v>
@@ -3171,10 +3394,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="C40" s="1">
         <v>1.0</v>
@@ -3182,21 +3405,21 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C42" s="1">
         <v>2.0</v>
@@ -3204,54 +3427,54 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="C43" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C45" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="C46" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C47" s="1">
         <v>5.0</v>
@@ -3259,10 +3482,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C48" s="1">
         <v>4.0</v>
@@ -3270,10 +3493,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C49" s="1">
         <v>1.0</v>
@@ -3281,32 +3504,32 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C50" s="1">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C51" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C52" s="1">
         <v>1.0</v>
@@ -3314,10 +3537,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C53" s="1">
         <v>8.0</v>
@@ -3325,10 +3548,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C54" s="1">
         <v>1.0</v>
@@ -3336,10 +3559,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="C55" s="1">
         <v>1.0</v>
@@ -3347,10 +3570,10 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C56" s="1">
         <v>8.0</v>
@@ -3358,10 +3581,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C57" s="1">
         <v>1.0</v>
@@ -3369,12 +3592,45 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="C58" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -3402,109 +3658,131 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C3" t="s">
         <v>192</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B5" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B6" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B7" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B8" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B10" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="1">
         <v>3.0</v>
       </c>
-      <c r="C10" t="s">
-        <v>218</v>
+      <c r="C11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3526,22 +3804,22 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3561,73 +3839,73 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -3636,51 +3914,51 @@
         <v>10.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -3689,51 +3967,51 @@
         <v>10.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
@@ -3742,51 +4020,51 @@
         <v>8.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -3795,51 +4073,51 @@
         <v>10.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -3848,34 +4126,34 @@
         <v>8.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update after code review: changed updateStats function to use lodash merge instead of Object.assign, and added player images.
</commit_message>
<xml_diff>
--- a/lib/seeds/Aeon's End Database.xlsx
+++ b/lib/seeds/Aeon's End Database.xlsx
@@ -16,18 +16,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="330">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
     <t>Image Name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amplify Vision</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
     <t>Ability</t>
   </si>
   <si>
     <t>Adelheim</t>
+  </si>
+  <si>
+    <t>Crystal</t>
   </si>
   <si>
     <t>Adelheim.jpg</t>
@@ -55,54 +85,15 @@
     <t>Dezmodia.jpg</t>
   </si>
   <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>Amethyst Shard</t>
+  </si>
+  <si>
     <t>Cost: 6 Charges.
 Activate during your main phase:
 Any player destroys an opened I or II breach and returns any spells to their hand. That player gains a Sigil breach and places it where the destroyed breach was. Then, that player may prep a spell from their hand to a breach.</t>
-  </si>
-  <si>
-    <t>Mage</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Amplify Vision</t>
-  </si>
-  <si>
-    <t>Spell</t>
-  </si>
-  <si>
-    <t>Market</t>
-  </si>
-  <si>
-    <t>AmplifyVision.jpg</t>
-  </si>
-  <si>
-    <t>Spark</t>
-  </si>
-  <si>
-    <t>Amethyst Shard</t>
-  </si>
-  <si>
-    <t>Buried Light</t>
   </si>
   <si>
     <t>Garu</t>
@@ -129,7 +120,7 @@
 Any ally draws one card and gains 2 life.</t>
   </si>
   <si>
-    <t>Oblivion Shard</t>
+    <t>Buried Light</t>
   </si>
   <si>
     <t>Jian</t>
@@ -144,22 +135,19 @@
 Then cast that prepped spell again.</t>
   </si>
   <si>
-    <t>Arcane Nexus</t>
-  </si>
-  <si>
-    <t>ArcaneNexus.jpg</t>
+    <t>Market</t>
   </si>
   <si>
     <t>Kadir</t>
   </si>
   <si>
+    <t>AmplifyVision.jpg</t>
+  </si>
+  <si>
     <t>Kadir.jpg</t>
   </si>
   <si>
-    <t>Aurora</t>
-  </si>
-  <si>
-    <t>Torch</t>
+    <t>Oblivion Shard</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -167,16 +155,10 @@
 That player may return up to three spells in their discard pile to their hand. That player may prep up to two spells to each of their opened breaches this turn.</t>
   </si>
   <si>
-    <t>Aurora.jpg</t>
-  </si>
-  <si>
     <t>Lash</t>
   </si>
   <si>
     <t>Lash.jpg</t>
-  </si>
-  <si>
-    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -184,16 +166,10 @@
 Shuffle any player's turn order card into the turn order deck. That player suffers 1 damage.</t>
   </si>
   <si>
-    <t>Gem</t>
-  </si>
-  <si>
     <t>Malastar</t>
   </si>
   <si>
     <t>Malastar.jpg</t>
-  </si>
-  <si>
-    <t>BanishingTopaz.jpg</t>
   </si>
   <si>
     <t>6 Charges.
@@ -201,22 +177,13 @@
 Gain a spell from any supply pile. You may prep that spell to any player's opened breach.</t>
   </si>
   <si>
-    <t>Blasting Staff</t>
-  </si>
-  <si>
     <t>Mazahaedron</t>
   </si>
   <si>
-    <t>Relic</t>
+    <t>Torch</t>
   </si>
   <si>
     <t>Mazahaedron.jpg</t>
-  </si>
-  <si>
-    <t>Shattered Geode</t>
-  </si>
-  <si>
-    <t>BlastingStaff.jpg</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -225,16 +192,10 @@
 Gravehold gains 4 life.</t>
   </si>
   <si>
-    <t>Blaze</t>
-  </si>
-  <si>
     <t>Mist (Dagger Captain)</t>
   </si>
   <si>
     <t>Mist.jpg</t>
-  </si>
-  <si>
-    <t>Blaze.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -242,7 +203,7 @@
 Any ally draws 4 cards.</t>
   </si>
   <si>
-    <t>Bloodstone Jewel</t>
+    <t>Arcane Nexus</t>
   </si>
   <si>
     <t>Mist (Voidwalker)</t>
@@ -251,7 +212,7 @@
     <t>MistWE.jpg</t>
   </si>
   <si>
-    <t>BloodstoneJewel.jpg</t>
+    <t>Shattered Geode</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -259,16 +220,19 @@
 Cast up to three different spells prepped by any number of players. For each spell cast this way, place that spell into any ally's hand.</t>
   </si>
   <si>
-    <t>Bottled Vortex</t>
+    <t>ArcaneNexus.jpg</t>
+  </si>
+  <si>
+    <t>Aurora</t>
   </si>
   <si>
     <t>Nym</t>
   </si>
   <si>
-    <t>Moonstone Shard</t>
-  </si>
-  <si>
     <t>Nym.jpg</t>
+  </si>
+  <si>
+    <t>Aurora.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -277,16 +241,22 @@
 If you discarded an attack card, discard an additional card.</t>
   </si>
   <si>
-    <t>BottledVortex.jpg</t>
+    <t>Moonstone Shard</t>
+  </si>
+  <si>
+    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Phaedraxa</t>
   </si>
   <si>
-    <t>Breach Ore</t>
-  </si>
-  <si>
     <t>Phaedraxa.jpg</t>
+  </si>
+  <si>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>BanishingTopaz.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -294,16 +264,16 @@
 Prevent any damage that the players or Gravehold would suffer during that turn.</t>
   </si>
   <si>
-    <t>BreachOre.jpg</t>
+    <t>Blasting Staff</t>
   </si>
   <si>
     <t>Quilius</t>
   </si>
   <si>
-    <t>Burning Opal</t>
-  </si>
-  <si>
     <t>Quilius.jpg</t>
+  </si>
+  <si>
+    <t>Relic</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -315,6 +285,15 @@
   </si>
   <si>
     <t>Reeve.jpg</t>
+  </si>
+  <si>
+    <t>BlastingStaff.jpg</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Emerald Shard</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -329,7 +308,7 @@
     <t>Ulgimor.jpg</t>
   </si>
   <si>
-    <t>Emerald Shard</t>
+    <t>Blaze.jpg</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -338,10 +317,16 @@
 If you are exhausted, any ally gains 5 life instead.</t>
   </si>
   <si>
+    <t>Bloodstone Jewel</t>
+  </si>
+  <si>
     <t>Xaxos</t>
   </si>
   <si>
     <t>Xaxos.jpg</t>
+  </si>
+  <si>
+    <t>BloodstoneJewel.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -350,7 +335,13 @@
 Reveal the turn order deck and return the revealed cards in any order.</t>
   </si>
   <si>
+    <t>Bottled Vortex</t>
+  </si>
+  <si>
     <t>Yan Magda</t>
+  </si>
+  <si>
+    <t>Quartz Shard</t>
   </si>
   <si>
     <t>YanMagda.jpg</t>
@@ -361,13 +352,16 @@
 Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
   </si>
   <si>
+    <t>BottledVortex.jpg</t>
+  </si>
+  <si>
     <t>Z'hana</t>
   </si>
   <si>
+    <t>Breach Ore</t>
+  </si>
+  <si>
     <t>Zhana.jpg</t>
-  </si>
-  <si>
-    <t>Quartz Shard</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -375,21 +369,30 @@
 Gravehold gains 7 life.</t>
   </si>
   <si>
+    <t>Immolate</t>
+  </si>
+  <si>
+    <t>BreachOre.jpg</t>
+  </si>
+  <si>
+    <t>Burning Opal</t>
+  </si>
+  <si>
     <t>BurningOpal.jpg</t>
   </si>
   <si>
     <t>Cairn Compass</t>
   </si>
   <si>
+    <t>Worldheart Shard</t>
+  </si>
+  <si>
     <t>CairnCompass.jpg</t>
   </si>
   <si>
     <t>Carbonize</t>
   </si>
   <si>
-    <t>Immolate</t>
-  </si>
-  <si>
     <t>Carbonize.jpg</t>
   </si>
   <si>
@@ -399,6 +402,9 @@
     <t>CelestialSpire.jpg</t>
   </si>
   <si>
+    <t>Garnet Shard</t>
+  </si>
+  <si>
     <t>Chaos Arc</t>
   </si>
   <si>
@@ -408,7 +414,7 @@
     <t>Clouded Sapphire</t>
   </si>
   <si>
-    <t>Worldheart Shard</t>
+    <t>Amethyst Paragon</t>
   </si>
   <si>
     <t>CloudedSapphire.jpg</t>
@@ -423,36 +429,39 @@
     <t>Conclave Scroll</t>
   </si>
   <si>
+    <t>Cinder</t>
+  </si>
+  <si>
     <t>ConclaveScroll.jpg</t>
   </si>
   <si>
     <t>Conjure The Lost</t>
   </si>
   <si>
-    <t>Garnet Shard</t>
-  </si>
-  <si>
     <t>ConjureTheLost.jpg</t>
   </si>
   <si>
     <t>Consuming Void</t>
   </si>
   <si>
+    <t>Tourmaline Shard</t>
+  </si>
+  <si>
     <t>ConsumingVoid.jpg</t>
   </si>
   <si>
     <t>Convection Field</t>
   </si>
   <si>
-    <t>Amethyst Paragon</t>
-  </si>
-  <si>
     <t>ConvectionField.jpg</t>
   </si>
   <si>
     <t>Crystallize</t>
   </si>
   <si>
+    <t>Extinguish</t>
+  </si>
+  <si>
     <t>Crystallize.jpg</t>
   </si>
   <si>
@@ -465,7 +474,7 @@
     <t>Devouring Shadow</t>
   </si>
   <si>
-    <t>Cinder</t>
+    <t>Obsidian Shard</t>
   </si>
   <si>
     <t>DevouringShadow.jpg</t>
@@ -480,7 +489,7 @@
     <t>Disintegrating Scythe</t>
   </si>
   <si>
-    <t>Tourmaline Shard</t>
+    <t>Coal Shard</t>
   </si>
   <si>
     <t>DisintegratingScythe.jpg</t>
@@ -495,12 +504,12 @@
     <t>Equilibrium</t>
   </si>
   <si>
+    <t>Flare</t>
+  </si>
+  <si>
     <t>Equilibrium.jpg</t>
   </si>
   <si>
-    <t>Extinguish</t>
-  </si>
-  <si>
     <t>Erratic Ingot</t>
   </si>
   <si>
@@ -510,7 +519,7 @@
     <t>Essence Theft</t>
   </si>
   <si>
-    <t>Obsidian Shard</t>
+    <t>Illuminate</t>
   </si>
   <si>
     <t>EssenceTheft.jpg</t>
@@ -522,12 +531,12 @@
     <t>FeralLightning.jpg</t>
   </si>
   <si>
+    <t>Eternal Ember</t>
+  </si>
+  <si>
     <t>Fiend Catcher</t>
   </si>
   <si>
-    <t>Coal Shard</t>
-  </si>
-  <si>
     <t>FiendCatcher.jpg</t>
   </si>
   <si>
@@ -537,9 +546,6 @@
     <t>FieryTorrent.jpg</t>
   </si>
   <si>
-    <t>Flare</t>
-  </si>
-  <si>
     <t>Flexing Dagger</t>
   </si>
   <si>
@@ -549,9 +555,6 @@
     <t>Focusing Orb</t>
   </si>
   <si>
-    <t>Illuminate</t>
-  </si>
-  <si>
     <t>FocusingOrb.jpg</t>
   </si>
   <si>
@@ -564,9 +567,6 @@
     <t>Ignite</t>
   </si>
   <si>
-    <t>Eternal Ember</t>
-  </si>
-  <si>
     <t>Ignite.jpg</t>
   </si>
   <si>
@@ -693,170 +693,158 @@
     <t>Searing Ruby</t>
   </si>
   <si>
+    <t>SearingRuby.jpg</t>
+  </si>
+  <si>
+    <t>Sifter's Pearl</t>
+  </si>
+  <si>
+    <t>SiftersPearl.jpg</t>
+  </si>
+  <si>
+    <t>Spectral Echo</t>
+  </si>
+  <si>
+    <t>SpectralEcho.jpg</t>
+  </si>
+  <si>
+    <t>Temporal Helix</t>
+  </si>
+  <si>
+    <t>TemporalHelix.jpg</t>
+  </si>
+  <si>
+    <t>Thoughtform Familiar</t>
+  </si>
+  <si>
+    <t>ThoughtformFamiliar.jpg</t>
+  </si>
+  <si>
+    <t>Transmogrifier</t>
+  </si>
+  <si>
+    <t>Transmogrifier.jpg</t>
+  </si>
+  <si>
+    <t>Unstable Prism</t>
+  </si>
+  <si>
     <t>Difficulty</t>
   </si>
   <si>
+    <t>UnstablePrism.jpg</t>
+  </si>
+  <si>
     <t>Blight Lord</t>
   </si>
   <si>
+    <t>V'riswood Amber</t>
+  </si>
+  <si>
     <t>BlightLord.jpg</t>
   </si>
   <si>
-    <t>SearingRuby.jpg</t>
+    <t>VriswoodAmber.jpg</t>
+  </si>
+  <si>
+    <t>Vim Dynamo</t>
   </si>
   <si>
     <t>Carapace Queen</t>
   </si>
   <si>
-    <t>Sifter's Pearl</t>
-  </si>
-  <si>
     <t>CarapaceQueen.jpg</t>
   </si>
   <si>
+    <t>VimDynamo.jpg</t>
+  </si>
+  <si>
     <t>Crooked Mask</t>
   </si>
   <si>
+    <t>Void Bond</t>
+  </si>
+  <si>
     <t>CrookedMask.jpg</t>
   </si>
   <si>
-    <t>SiftersPearl.jpg</t>
-  </si>
-  <si>
     <t>Gate Witch</t>
   </si>
   <si>
+    <t>VoidBond.jpg</t>
+  </si>
+  <si>
     <t>GateWitch.jpg</t>
   </si>
   <si>
+    <t>Volcanic Glass</t>
+  </si>
+  <si>
     <t>Hollow Crown</t>
   </si>
   <si>
-    <t>Spectral Echo</t>
-  </si>
-  <si>
     <t>HollowCrown.jpg</t>
   </si>
   <si>
+    <t>VolcanicGlass.jpg</t>
+  </si>
+  <si>
     <t>Horde Crone</t>
   </si>
   <si>
-    <t>SpectralEcho.jpg</t>
-  </si>
-  <si>
     <t>HordeCrone.jpg</t>
   </si>
   <si>
-    <t>Temporal Helix</t>
-  </si>
-  <si>
     <t>Magus Of Cloaks</t>
   </si>
   <si>
+    <t>Vortex Gauntlet</t>
+  </si>
+  <si>
     <t>MagusOfCloaks.jpg</t>
   </si>
   <si>
-    <t>TemporalHelix.jpg</t>
+    <t>VortexGauntlet.jpg</t>
   </si>
   <si>
     <t>Prince Of Gluttons</t>
   </si>
   <si>
+    <t>Wildfire Whip</t>
+  </si>
+  <si>
     <t>PrinceOfGluttons.jpg</t>
   </si>
   <si>
-    <t>Thoughtform Familiar</t>
-  </si>
-  <si>
     <t>RageBorne</t>
   </si>
   <si>
+    <t>WildfireWhip.jpg</t>
+  </si>
+  <si>
     <t>RageBorne.jpg</t>
   </si>
   <si>
-    <t>ThoughtformFamiliar.jpg</t>
-  </si>
-  <si>
     <t>Umbra Titan</t>
   </si>
   <si>
+    <t>Unique</t>
+  </si>
+  <si>
     <t>UmbraTitan.jpg</t>
   </si>
   <si>
-    <t>Transmogrifier</t>
+    <t>AmethystParagon.jpg</t>
   </si>
   <si>
     <t>Wayward One</t>
-  </si>
-  <si>
-    <t>WaywardOne.jpg</t>
-  </si>
-  <si>
-    <t>Transmogrifier.jpg</t>
-  </si>
-  <si>
-    <t>Unstable Prism</t>
-  </si>
-  <si>
-    <t>UnstablePrism.jpg</t>
-  </si>
-  <si>
-    <t>Miriam</t>
-  </si>
-  <si>
-    <t>V'riswood Amber</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Kermit</t>
-  </si>
-  <si>
-    <t>Homura</t>
-  </si>
-  <si>
-    <t>VriswoodAmber.jpg</t>
-  </si>
-  <si>
-    <t>Vim Dynamo</t>
-  </si>
-  <si>
-    <t>VimDynamo.jpg</t>
-  </si>
-  <si>
-    <t>Void Bond</t>
-  </si>
-  <si>
-    <t>VoidBond.jpg</t>
-  </si>
-  <si>
-    <t>Volcanic Glass</t>
-  </si>
-  <si>
-    <t>VolcanicGlass.jpg</t>
-  </si>
-  <si>
-    <t>Vortex Gauntlet</t>
-  </si>
-  <si>
-    <t>VortexGauntlet.jpg</t>
-  </si>
-  <si>
-    <t>Wildfire Whip</t>
-  </si>
-  <si>
-    <t>WildfireWhip.jpg</t>
-  </si>
-  <si>
-    <t>Unique</t>
-  </si>
-  <si>
-    <t>AmethystParagon.jpg</t>
   </si>
   <si>
     <t>Gain 1 Aether. 
 Any ally may prep a spell in hand to their opened or closed breach(es).</t>
+  </si>
+  <si>
+    <t>WaywardOne.jpg</t>
   </si>
   <si>
     <t>AmethystShard.jpg</t>
@@ -951,54 +939,18 @@
     <t>Gain 2 Aether that cannot be used to gain a relic or spell.</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Player 1</t>
-  </si>
-  <si>
     <t>ObsidianShard.jpg</t>
-  </si>
-  <si>
-    <t>Mage 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
   </si>
   <si>
     <t>Gain 1 Aether.
 You may suffer 1 damage. If you do, gain an additional 2 Aether.</t>
   </si>
   <si>
-    <t>Mage 2</t>
-  </si>
-  <si>
-    <t>Won</t>
-  </si>
-  <si>
-    <t>Nemesis</t>
-  </si>
-  <si>
-    <t>Market Card 1</t>
-  </si>
-  <si>
     <t>QuartzShard.jpg</t>
-  </si>
-  <si>
-    <t>Market Card 2</t>
-  </si>
-  <si>
-    <t>Market Card 3</t>
-  </si>
-  <si>
-    <t>Market Card 4</t>
   </si>
   <si>
     <t>Gain 1 Aether.
 Reveal the top card of the turn order deck. You may place that card on the bottom or the top of the turn order deck. If you revealed a player turn order card, gain an additional 1 Aether.</t>
-  </si>
-  <si>
-    <t>Market Card 5</t>
   </si>
   <si>
     <t>ShatteredGeode.jpg</t>
@@ -1038,6 +990,66 @@
   </si>
   <si>
     <t>Spark.jpg</t>
+  </si>
+  <si>
+    <t>Miriam</t>
+  </si>
+  <si>
+    <t>Miriam.jpg</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>James.jpg</t>
+  </si>
+  <si>
+    <t>Kermit</t>
+  </si>
+  <si>
+    <t>Kermit.png</t>
+  </si>
+  <si>
+    <t>Homura</t>
+  </si>
+  <si>
+    <t>Homura.jpg</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Mage 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Mage 2</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>Nemesis</t>
+  </si>
+  <si>
+    <t>Market Card 1</t>
+  </si>
+  <si>
+    <t>Market Card 2</t>
+  </si>
+  <si>
+    <t>Market Card 3</t>
+  </si>
+  <si>
+    <t>Market Card 4</t>
+  </si>
+  <si>
+    <t>Market Card 5</t>
   </si>
   <si>
     <t>Market Card 6</t>
@@ -1165,629 +1177,629 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1">
         <v>7.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1">
         <v>4.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1">
         <v>6.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1">
         <v>3.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B10" s="1">
         <v>4.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1">
         <v>5.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B12" s="1">
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B13" s="1">
         <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B14" s="1">
         <v>5.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1">
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B16" s="1">
         <v>6.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1">
         <v>5.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B18" s="1">
         <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B19" s="1">
         <v>6.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1">
         <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B21" s="1">
         <v>5.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B22" s="1">
         <v>8.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1">
         <v>5.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B24" s="1">
         <v>6.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B25" s="1">
         <v>4.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B26" s="1">
         <v>7.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B27" s="1">
         <v>3.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B28" s="1">
         <v>7.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B29" s="1">
         <v>5.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B31" s="1">
         <v>5.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B32" s="1">
         <v>3.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B33" s="1">
         <v>5.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1">
         <v>2.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B35" s="1">
         <v>4.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B36" s="1">
         <v>3.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B37" s="1">
         <v>4.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>167</v>
@@ -1801,10 +1813,10 @@
         <v>2.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>169</v>
@@ -1818,10 +1830,10 @@
         <v>4.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>171</v>
@@ -1835,10 +1847,10 @@
         <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>173</v>
@@ -1852,10 +1864,10 @@
         <v>4.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>175</v>
@@ -1869,10 +1881,10 @@
         <v>3.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>177</v>
@@ -1887,10 +1899,10 @@
         <v>5.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>179</v>
@@ -1904,10 +1916,10 @@
         <v>2.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>181</v>
@@ -1921,10 +1933,10 @@
         <v>8.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>183</v>
@@ -1938,10 +1950,10 @@
         <v>5.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>185</v>
@@ -1955,10 +1967,10 @@
         <v>6.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>187</v>
@@ -1972,10 +1984,10 @@
         <v>5.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>189</v>
@@ -1989,10 +2001,10 @@
         <v>3.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>191</v>
@@ -2006,10 +2018,10 @@
         <v>6.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>193</v>
@@ -2023,10 +2035,10 @@
         <v>4.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>195</v>
@@ -2040,10 +2052,10 @@
         <v>4.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>197</v>
@@ -2057,10 +2069,10 @@
         <v>8.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>199</v>
@@ -2074,10 +2086,10 @@
         <v>7.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>201</v>
@@ -2091,10 +2103,10 @@
         <v>7.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>203</v>
@@ -2108,10 +2120,10 @@
         <v>4.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>205</v>
@@ -2125,10 +2137,10 @@
         <v>6.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>207</v>
@@ -2142,651 +2154,651 @@
         <v>4.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B59" s="1">
         <v>3.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B60" s="1">
         <v>3.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="B61" s="1">
         <v>7.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="B62" s="1">
         <v>3.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="B63" s="1">
         <v>4.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="B64" s="1">
         <v>3.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="B65" s="1">
         <v>3.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B66" s="1">
         <v>4.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B67" s="1">
         <v>4.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B68" s="1">
         <v>3.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="B69" s="1">
         <v>6.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="B70" s="1">
         <v>6.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B71" s="1">
         <v>0.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B72" s="1">
         <v>0.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B73" s="1">
         <v>0.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B74" s="1">
         <v>0.0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B75" s="1">
         <v>0.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B76" s="1">
         <v>0.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B77" s="1">
         <v>0.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B78" s="1">
         <v>0.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B79" s="1">
         <v>0.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B80" s="1">
         <v>0.0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B81" s="1">
         <v>0.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B82" s="1">
         <v>0.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B83" s="1">
         <v>0.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B84" s="1">
         <v>0.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B85" s="1">
         <v>0.0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B86" s="1">
         <v>0.0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B87" s="1">
         <v>0.0</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B88" s="1">
         <v>0.0</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B89" s="1">
         <v>0.0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B90" s="1">
         <v>0.0</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B91" s="1">
         <v>0.0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B92" s="1">
         <v>0.0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2812,230 +2824,230 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3055,23 +3067,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>7.0</v>
@@ -3081,10 +3093,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -3094,10 +3106,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
@@ -3106,10 +3118,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>7.0</v>
@@ -3118,10 +3130,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -3130,10 +3142,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -3142,10 +3154,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1">
         <v>6.0</v>
@@ -3154,10 +3166,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -3166,10 +3178,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1">
         <v>1.0</v>
@@ -3178,10 +3190,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>6.0</v>
@@ -3191,10 +3203,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>3.0</v>
@@ -3203,10 +3215,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
@@ -3215,10 +3227,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <v>7.0</v>
@@ -3227,10 +3239,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
         <v>2.0</v>
@@ -3239,10 +3251,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -3251,10 +3263,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1">
         <v>5.0</v>
@@ -3263,10 +3275,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
         <v>4.0</v>
@@ -3275,10 +3287,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1">
         <v>1.0</v>
@@ -3287,10 +3299,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20" s="1">
         <v>6.0</v>
@@ -3299,10 +3311,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1">
         <v>3.0</v>
@@ -3311,10 +3323,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1">
         <v>1.0</v>
@@ -3323,10 +3335,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
         <v>6.0</v>
@@ -3335,10 +3347,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
         <v>3.0</v>
@@ -3347,10 +3359,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -3359,10 +3371,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1">
         <v>9.0</v>
@@ -3371,10 +3383,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1">
         <v>0.0</v>
@@ -3383,10 +3395,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1">
         <v>1.0</v>
@@ -3395,10 +3407,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1">
         <v>6.0</v>
@@ -3407,10 +3419,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" s="1">
         <v>3.0</v>
@@ -3419,10 +3431,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1">
         <v>1.0</v>
@@ -3431,10 +3443,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C32" s="1">
         <v>6.0</v>
@@ -3443,10 +3455,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1">
         <v>3.0</v>
@@ -3454,10 +3466,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C34" s="1">
         <v>1.0</v>
@@ -3465,10 +3477,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C35" s="1">
         <v>6.0</v>
@@ -3476,10 +3488,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C36" s="1">
         <v>3.0</v>
@@ -3487,10 +3499,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C37" s="1">
         <v>1.0</v>
@@ -3498,10 +3510,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1">
         <v>7.0</v>
@@ -3509,10 +3521,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C39" s="1">
         <v>2.0</v>
@@ -3520,10 +3532,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1">
         <v>1.0</v>
@@ -3531,10 +3543,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C41" s="1">
         <v>7.0</v>
@@ -3542,10 +3554,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C42" s="1">
         <v>2.0</v>
@@ -3553,10 +3565,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C43" s="1">
         <v>1.0</v>
@@ -3564,10 +3576,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C44" s="1">
         <v>6.0</v>
@@ -3575,10 +3587,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1">
         <v>2.0</v>
@@ -3586,10 +3598,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C46" s="1">
         <v>2.0</v>
@@ -3597,10 +3609,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1">
         <v>5.0</v>
@@ -3608,10 +3620,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C48" s="1">
         <v>4.0</v>
@@ -3619,10 +3631,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C49" s="1">
         <v>1.0</v>
@@ -3630,10 +3642,10 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C50" s="1">
         <v>5.0</v>
@@ -3641,10 +3653,10 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C51" s="1">
         <v>4.0</v>
@@ -3652,10 +3664,10 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C52" s="1">
         <v>1.0</v>
@@ -3663,10 +3675,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C53" s="1">
         <v>8.0</v>
@@ -3674,10 +3686,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C54" s="1">
         <v>1.0</v>
@@ -3685,10 +3697,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C55" s="1">
         <v>1.0</v>
@@ -3696,10 +3708,10 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C56" s="1">
         <v>8.0</v>
@@ -3707,10 +3719,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C57" s="1">
         <v>1.0</v>
@@ -3718,10 +3730,10 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C58" s="1">
         <v>1.0</v>
@@ -3729,10 +3741,10 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C59" s="1">
         <v>8.0</v>
@@ -3740,10 +3752,10 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C60" s="1">
         <v>1.0</v>
@@ -3751,10 +3763,10 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C61" s="1">
         <v>1.0</v>
@@ -3784,131 +3796,131 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="B3" s="1">
         <v>3.0</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="B5" s="1">
         <v>7.0</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="B6" s="1">
         <v>5.0</v>
       </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="B7" s="1">
         <v>6.0</v>
       </c>
       <c r="C7" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="B8" s="1">
         <v>7.0</v>
       </c>
       <c r="C8" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="B9" s="1">
         <v>5.0</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="B10" s="1">
         <v>2.0</v>
       </c>
       <c r="C10" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="B11" s="1">
         <v>3.0</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="B12" s="1">
         <v>7.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3927,25 +3939,40 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>245</v>
+        <v>301</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>247</v>
+        <v>303</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3965,73 +3992,73 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -4040,25 +4067,25 @@
         <v>10.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>204</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>180</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>190</v>
@@ -4067,24 +4094,24 @@
         <v>182</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -4093,25 +4120,25 @@
         <v>10.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>204</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>180</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>190</v>
@@ -4120,24 +4147,24 @@
         <v>182</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
@@ -4146,25 +4173,25 @@
         <v>8.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>204</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>180</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>190</v>
@@ -4173,24 +4200,24 @@
         <v>182</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -4199,51 +4226,51 @@
         <v>10.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>208</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -4252,34 +4279,34 @@
         <v>8.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>208</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>196</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add player component, update stats for mages, cards, nemeses, and pla… (#39)
* Add player component, update stats for mages, cards, nemeses, and players when the user saves a game, and minor changes to improve UI.

* Update cards.jsx

* Update players.jsx

* Update after code review: changed updateStats function to use lodash merge instead of Object.assign, and added player images.
</commit_message>
<xml_diff>
--- a/lib/seeds/Aeon's End Database.xlsx
+++ b/lib/seeds/Aeon's End Database.xlsx
@@ -16,18 +16,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="330">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
     <t>Image Name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amplify Vision</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
     <t>Ability</t>
   </si>
   <si>
     <t>Adelheim</t>
+  </si>
+  <si>
+    <t>Crystal</t>
   </si>
   <si>
     <t>Adelheim.jpg</t>
@@ -55,54 +85,15 @@
     <t>Dezmodia.jpg</t>
   </si>
   <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>Amethyst Shard</t>
+  </si>
+  <si>
     <t>Cost: 6 Charges.
 Activate during your main phase:
 Any player destroys an opened I or II breach and returns any spells to their hand. That player gains a Sigil breach and places it where the destroyed breach was. Then, that player may prep a spell from their hand to a breach.</t>
-  </si>
-  <si>
-    <t>Mage</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Card</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Amplify Vision</t>
-  </si>
-  <si>
-    <t>Spell</t>
-  </si>
-  <si>
-    <t>Market</t>
-  </si>
-  <si>
-    <t>AmplifyVision.jpg</t>
-  </si>
-  <si>
-    <t>Spark</t>
-  </si>
-  <si>
-    <t>Amethyst Shard</t>
-  </si>
-  <si>
-    <t>Buried Light</t>
   </si>
   <si>
     <t>Garu</t>
@@ -129,7 +120,7 @@
 Any ally draws one card and gains 2 life.</t>
   </si>
   <si>
-    <t>Oblivion Shard</t>
+    <t>Buried Light</t>
   </si>
   <si>
     <t>Jian</t>
@@ -144,22 +135,19 @@
 Then cast that prepped spell again.</t>
   </si>
   <si>
-    <t>Arcane Nexus</t>
-  </si>
-  <si>
-    <t>ArcaneNexus.jpg</t>
+    <t>Market</t>
   </si>
   <si>
     <t>Kadir</t>
   </si>
   <si>
+    <t>AmplifyVision.jpg</t>
+  </si>
+  <si>
     <t>Kadir.jpg</t>
   </si>
   <si>
-    <t>Aurora</t>
-  </si>
-  <si>
-    <t>Torch</t>
+    <t>Oblivion Shard</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -167,16 +155,10 @@
 That player may return up to three spells in their discard pile to their hand. That player may prep up to two spells to each of their opened breaches this turn.</t>
   </si>
   <si>
-    <t>Aurora.jpg</t>
-  </si>
-  <si>
     <t>Lash</t>
   </si>
   <si>
     <t>Lash.jpg</t>
-  </si>
-  <si>
-    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -184,16 +166,10 @@
 Shuffle any player's turn order card into the turn order deck. That player suffers 1 damage.</t>
   </si>
   <si>
-    <t>Gem</t>
-  </si>
-  <si>
     <t>Malastar</t>
   </si>
   <si>
     <t>Malastar.jpg</t>
-  </si>
-  <si>
-    <t>BanishingTopaz.jpg</t>
   </si>
   <si>
     <t>6 Charges.
@@ -201,22 +177,13 @@
 Gain a spell from any supply pile. You may prep that spell to any player's opened breach.</t>
   </si>
   <si>
-    <t>Blasting Staff</t>
-  </si>
-  <si>
     <t>Mazahaedron</t>
   </si>
   <si>
-    <t>Relic</t>
+    <t>Torch</t>
   </si>
   <si>
     <t>Mazahaedron.jpg</t>
-  </si>
-  <si>
-    <t>Shattered Geode</t>
-  </si>
-  <si>
-    <t>BlastingStaff.jpg</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -225,16 +192,10 @@
 Gravehold gains 4 life.</t>
   </si>
   <si>
-    <t>Blaze</t>
-  </si>
-  <si>
     <t>Mist (Dagger Captain)</t>
   </si>
   <si>
     <t>Mist.jpg</t>
-  </si>
-  <si>
-    <t>Blaze.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -242,7 +203,7 @@
 Any ally draws 4 cards.</t>
   </si>
   <si>
-    <t>Bloodstone Jewel</t>
+    <t>Arcane Nexus</t>
   </si>
   <si>
     <t>Mist (Voidwalker)</t>
@@ -251,7 +212,7 @@
     <t>MistWE.jpg</t>
   </si>
   <si>
-    <t>BloodstoneJewel.jpg</t>
+    <t>Shattered Geode</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -259,16 +220,19 @@
 Cast up to three different spells prepped by any number of players. For each spell cast this way, place that spell into any ally's hand.</t>
   </si>
   <si>
-    <t>Bottled Vortex</t>
+    <t>ArcaneNexus.jpg</t>
+  </si>
+  <si>
+    <t>Aurora</t>
   </si>
   <si>
     <t>Nym</t>
   </si>
   <si>
-    <t>Moonstone Shard</t>
-  </si>
-  <si>
     <t>Nym.jpg</t>
+  </si>
+  <si>
+    <t>Aurora.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -277,16 +241,22 @@
 If you discarded an attack card, discard an additional card.</t>
   </si>
   <si>
-    <t>BottledVortex.jpg</t>
+    <t>Moonstone Shard</t>
+  </si>
+  <si>
+    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Phaedraxa</t>
   </si>
   <si>
-    <t>Breach Ore</t>
-  </si>
-  <si>
     <t>Phaedraxa.jpg</t>
+  </si>
+  <si>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>BanishingTopaz.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -294,16 +264,16 @@
 Prevent any damage that the players or Gravehold would suffer during that turn.</t>
   </si>
   <si>
-    <t>BreachOre.jpg</t>
+    <t>Blasting Staff</t>
   </si>
   <si>
     <t>Quilius</t>
   </si>
   <si>
-    <t>Burning Opal</t>
-  </si>
-  <si>
     <t>Quilius.jpg</t>
+  </si>
+  <si>
+    <t>Relic</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -315,6 +285,15 @@
   </si>
   <si>
     <t>Reeve.jpg</t>
+  </si>
+  <si>
+    <t>BlastingStaff.jpg</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Emerald Shard</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -329,7 +308,7 @@
     <t>Ulgimor.jpg</t>
   </si>
   <si>
-    <t>Emerald Shard</t>
+    <t>Blaze.jpg</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -338,10 +317,16 @@
 If you are exhausted, any ally gains 5 life instead.</t>
   </si>
   <si>
+    <t>Bloodstone Jewel</t>
+  </si>
+  <si>
     <t>Xaxos</t>
   </si>
   <si>
     <t>Xaxos.jpg</t>
+  </si>
+  <si>
+    <t>BloodstoneJewel.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -350,7 +335,13 @@
 Reveal the turn order deck and return the revealed cards in any order.</t>
   </si>
   <si>
+    <t>Bottled Vortex</t>
+  </si>
+  <si>
     <t>Yan Magda</t>
+  </si>
+  <si>
+    <t>Quartz Shard</t>
   </si>
   <si>
     <t>YanMagda.jpg</t>
@@ -361,13 +352,16 @@
 Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
   </si>
   <si>
+    <t>BottledVortex.jpg</t>
+  </si>
+  <si>
     <t>Z'hana</t>
   </si>
   <si>
+    <t>Breach Ore</t>
+  </si>
+  <si>
     <t>Zhana.jpg</t>
-  </si>
-  <si>
-    <t>Quartz Shard</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -375,21 +369,30 @@
 Gravehold gains 7 life.</t>
   </si>
   <si>
+    <t>Immolate</t>
+  </si>
+  <si>
+    <t>BreachOre.jpg</t>
+  </si>
+  <si>
+    <t>Burning Opal</t>
+  </si>
+  <si>
     <t>BurningOpal.jpg</t>
   </si>
   <si>
     <t>Cairn Compass</t>
   </si>
   <si>
+    <t>Worldheart Shard</t>
+  </si>
+  <si>
     <t>CairnCompass.jpg</t>
   </si>
   <si>
     <t>Carbonize</t>
   </si>
   <si>
-    <t>Immolate</t>
-  </si>
-  <si>
     <t>Carbonize.jpg</t>
   </si>
   <si>
@@ -399,6 +402,9 @@
     <t>CelestialSpire.jpg</t>
   </si>
   <si>
+    <t>Garnet Shard</t>
+  </si>
+  <si>
     <t>Chaos Arc</t>
   </si>
   <si>
@@ -408,7 +414,7 @@
     <t>Clouded Sapphire</t>
   </si>
   <si>
-    <t>Worldheart Shard</t>
+    <t>Amethyst Paragon</t>
   </si>
   <si>
     <t>CloudedSapphire.jpg</t>
@@ -423,36 +429,39 @@
     <t>Conclave Scroll</t>
   </si>
   <si>
+    <t>Cinder</t>
+  </si>
+  <si>
     <t>ConclaveScroll.jpg</t>
   </si>
   <si>
     <t>Conjure The Lost</t>
   </si>
   <si>
-    <t>Garnet Shard</t>
-  </si>
-  <si>
     <t>ConjureTheLost.jpg</t>
   </si>
   <si>
     <t>Consuming Void</t>
   </si>
   <si>
+    <t>Tourmaline Shard</t>
+  </si>
+  <si>
     <t>ConsumingVoid.jpg</t>
   </si>
   <si>
     <t>Convection Field</t>
   </si>
   <si>
-    <t>Amethyst Paragon</t>
-  </si>
-  <si>
     <t>ConvectionField.jpg</t>
   </si>
   <si>
     <t>Crystallize</t>
   </si>
   <si>
+    <t>Extinguish</t>
+  </si>
+  <si>
     <t>Crystallize.jpg</t>
   </si>
   <si>
@@ -465,7 +474,7 @@
     <t>Devouring Shadow</t>
   </si>
   <si>
-    <t>Cinder</t>
+    <t>Obsidian Shard</t>
   </si>
   <si>
     <t>DevouringShadow.jpg</t>
@@ -480,7 +489,7 @@
     <t>Disintegrating Scythe</t>
   </si>
   <si>
-    <t>Tourmaline Shard</t>
+    <t>Coal Shard</t>
   </si>
   <si>
     <t>DisintegratingScythe.jpg</t>
@@ -495,12 +504,12 @@
     <t>Equilibrium</t>
   </si>
   <si>
+    <t>Flare</t>
+  </si>
+  <si>
     <t>Equilibrium.jpg</t>
   </si>
   <si>
-    <t>Extinguish</t>
-  </si>
-  <si>
     <t>Erratic Ingot</t>
   </si>
   <si>
@@ -510,7 +519,7 @@
     <t>Essence Theft</t>
   </si>
   <si>
-    <t>Obsidian Shard</t>
+    <t>Illuminate</t>
   </si>
   <si>
     <t>EssenceTheft.jpg</t>
@@ -522,12 +531,12 @@
     <t>FeralLightning.jpg</t>
   </si>
   <si>
+    <t>Eternal Ember</t>
+  </si>
+  <si>
     <t>Fiend Catcher</t>
   </si>
   <si>
-    <t>Coal Shard</t>
-  </si>
-  <si>
     <t>FiendCatcher.jpg</t>
   </si>
   <si>
@@ -537,9 +546,6 @@
     <t>FieryTorrent.jpg</t>
   </si>
   <si>
-    <t>Flare</t>
-  </si>
-  <si>
     <t>Flexing Dagger</t>
   </si>
   <si>
@@ -549,9 +555,6 @@
     <t>Focusing Orb</t>
   </si>
   <si>
-    <t>Illuminate</t>
-  </si>
-  <si>
     <t>FocusingOrb.jpg</t>
   </si>
   <si>
@@ -564,9 +567,6 @@
     <t>Ignite</t>
   </si>
   <si>
-    <t>Eternal Ember</t>
-  </si>
-  <si>
     <t>Ignite.jpg</t>
   </si>
   <si>
@@ -693,170 +693,158 @@
     <t>Searing Ruby</t>
   </si>
   <si>
+    <t>SearingRuby.jpg</t>
+  </si>
+  <si>
+    <t>Sifter's Pearl</t>
+  </si>
+  <si>
+    <t>SiftersPearl.jpg</t>
+  </si>
+  <si>
+    <t>Spectral Echo</t>
+  </si>
+  <si>
+    <t>SpectralEcho.jpg</t>
+  </si>
+  <si>
+    <t>Temporal Helix</t>
+  </si>
+  <si>
+    <t>TemporalHelix.jpg</t>
+  </si>
+  <si>
+    <t>Thoughtform Familiar</t>
+  </si>
+  <si>
+    <t>ThoughtformFamiliar.jpg</t>
+  </si>
+  <si>
+    <t>Transmogrifier</t>
+  </si>
+  <si>
+    <t>Transmogrifier.jpg</t>
+  </si>
+  <si>
+    <t>Unstable Prism</t>
+  </si>
+  <si>
     <t>Difficulty</t>
   </si>
   <si>
+    <t>UnstablePrism.jpg</t>
+  </si>
+  <si>
     <t>Blight Lord</t>
   </si>
   <si>
+    <t>V'riswood Amber</t>
+  </si>
+  <si>
     <t>BlightLord.jpg</t>
   </si>
   <si>
-    <t>SearingRuby.jpg</t>
+    <t>VriswoodAmber.jpg</t>
+  </si>
+  <si>
+    <t>Vim Dynamo</t>
   </si>
   <si>
     <t>Carapace Queen</t>
   </si>
   <si>
-    <t>Sifter's Pearl</t>
-  </si>
-  <si>
     <t>CarapaceQueen.jpg</t>
   </si>
   <si>
+    <t>VimDynamo.jpg</t>
+  </si>
+  <si>
     <t>Crooked Mask</t>
   </si>
   <si>
+    <t>Void Bond</t>
+  </si>
+  <si>
     <t>CrookedMask.jpg</t>
   </si>
   <si>
-    <t>SiftersPearl.jpg</t>
-  </si>
-  <si>
     <t>Gate Witch</t>
   </si>
   <si>
+    <t>VoidBond.jpg</t>
+  </si>
+  <si>
     <t>GateWitch.jpg</t>
   </si>
   <si>
+    <t>Volcanic Glass</t>
+  </si>
+  <si>
     <t>Hollow Crown</t>
   </si>
   <si>
-    <t>Spectral Echo</t>
-  </si>
-  <si>
     <t>HollowCrown.jpg</t>
   </si>
   <si>
+    <t>VolcanicGlass.jpg</t>
+  </si>
+  <si>
     <t>Horde Crone</t>
   </si>
   <si>
-    <t>SpectralEcho.jpg</t>
-  </si>
-  <si>
     <t>HordeCrone.jpg</t>
   </si>
   <si>
-    <t>Temporal Helix</t>
-  </si>
-  <si>
     <t>Magus Of Cloaks</t>
   </si>
   <si>
+    <t>Vortex Gauntlet</t>
+  </si>
+  <si>
     <t>MagusOfCloaks.jpg</t>
   </si>
   <si>
-    <t>TemporalHelix.jpg</t>
+    <t>VortexGauntlet.jpg</t>
   </si>
   <si>
     <t>Prince Of Gluttons</t>
   </si>
   <si>
+    <t>Wildfire Whip</t>
+  </si>
+  <si>
     <t>PrinceOfGluttons.jpg</t>
   </si>
   <si>
-    <t>Thoughtform Familiar</t>
-  </si>
-  <si>
     <t>RageBorne</t>
   </si>
   <si>
+    <t>WildfireWhip.jpg</t>
+  </si>
+  <si>
     <t>RageBorne.jpg</t>
   </si>
   <si>
-    <t>ThoughtformFamiliar.jpg</t>
-  </si>
-  <si>
     <t>Umbra Titan</t>
   </si>
   <si>
+    <t>Unique</t>
+  </si>
+  <si>
     <t>UmbraTitan.jpg</t>
   </si>
   <si>
-    <t>Transmogrifier</t>
+    <t>AmethystParagon.jpg</t>
   </si>
   <si>
     <t>Wayward One</t>
-  </si>
-  <si>
-    <t>WaywardOne.jpg</t>
-  </si>
-  <si>
-    <t>Transmogrifier.jpg</t>
-  </si>
-  <si>
-    <t>Unstable Prism</t>
-  </si>
-  <si>
-    <t>UnstablePrism.jpg</t>
-  </si>
-  <si>
-    <t>Miriam</t>
-  </si>
-  <si>
-    <t>V'riswood Amber</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Kermit</t>
-  </si>
-  <si>
-    <t>Homura</t>
-  </si>
-  <si>
-    <t>VriswoodAmber.jpg</t>
-  </si>
-  <si>
-    <t>Vim Dynamo</t>
-  </si>
-  <si>
-    <t>VimDynamo.jpg</t>
-  </si>
-  <si>
-    <t>Void Bond</t>
-  </si>
-  <si>
-    <t>VoidBond.jpg</t>
-  </si>
-  <si>
-    <t>Volcanic Glass</t>
-  </si>
-  <si>
-    <t>VolcanicGlass.jpg</t>
-  </si>
-  <si>
-    <t>Vortex Gauntlet</t>
-  </si>
-  <si>
-    <t>VortexGauntlet.jpg</t>
-  </si>
-  <si>
-    <t>Wildfire Whip</t>
-  </si>
-  <si>
-    <t>WildfireWhip.jpg</t>
-  </si>
-  <si>
-    <t>Unique</t>
-  </si>
-  <si>
-    <t>AmethystParagon.jpg</t>
   </si>
   <si>
     <t>Gain 1 Aether. 
 Any ally may prep a spell in hand to their opened or closed breach(es).</t>
+  </si>
+  <si>
+    <t>WaywardOne.jpg</t>
   </si>
   <si>
     <t>AmethystShard.jpg</t>
@@ -951,54 +939,18 @@
     <t>Gain 2 Aether that cannot be used to gain a relic or spell.</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Player 1</t>
-  </si>
-  <si>
     <t>ObsidianShard.jpg</t>
-  </si>
-  <si>
-    <t>Mage 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
   </si>
   <si>
     <t>Gain 1 Aether.
 You may suffer 1 damage. If you do, gain an additional 2 Aether.</t>
   </si>
   <si>
-    <t>Mage 2</t>
-  </si>
-  <si>
-    <t>Won</t>
-  </si>
-  <si>
-    <t>Nemesis</t>
-  </si>
-  <si>
-    <t>Market Card 1</t>
-  </si>
-  <si>
     <t>QuartzShard.jpg</t>
-  </si>
-  <si>
-    <t>Market Card 2</t>
-  </si>
-  <si>
-    <t>Market Card 3</t>
-  </si>
-  <si>
-    <t>Market Card 4</t>
   </si>
   <si>
     <t>Gain 1 Aether.
 Reveal the top card of the turn order deck. You may place that card on the bottom or the top of the turn order deck. If you revealed a player turn order card, gain an additional 1 Aether.</t>
-  </si>
-  <si>
-    <t>Market Card 5</t>
   </si>
   <si>
     <t>ShatteredGeode.jpg</t>
@@ -1038,6 +990,66 @@
   </si>
   <si>
     <t>Spark.jpg</t>
+  </si>
+  <si>
+    <t>Miriam</t>
+  </si>
+  <si>
+    <t>Miriam.jpg</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>James.jpg</t>
+  </si>
+  <si>
+    <t>Kermit</t>
+  </si>
+  <si>
+    <t>Kermit.png</t>
+  </si>
+  <si>
+    <t>Homura</t>
+  </si>
+  <si>
+    <t>Homura.jpg</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Mage 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Mage 2</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
+    <t>Nemesis</t>
+  </si>
+  <si>
+    <t>Market Card 1</t>
+  </si>
+  <si>
+    <t>Market Card 2</t>
+  </si>
+  <si>
+    <t>Market Card 3</t>
+  </si>
+  <si>
+    <t>Market Card 4</t>
+  </si>
+  <si>
+    <t>Market Card 5</t>
   </si>
   <si>
     <t>Market Card 6</t>
@@ -1165,629 +1177,629 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1">
         <v>7.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1">
         <v>4.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1">
         <v>6.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1">
         <v>3.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B10" s="1">
         <v>4.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1">
         <v>5.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B12" s="1">
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B13" s="1">
         <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B14" s="1">
         <v>5.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1">
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B16" s="1">
         <v>6.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1">
         <v>5.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B18" s="1">
         <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B19" s="1">
         <v>6.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1">
         <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B21" s="1">
         <v>5.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B22" s="1">
         <v>8.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1">
         <v>5.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B24" s="1">
         <v>6.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B25" s="1">
         <v>4.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B26" s="1">
         <v>7.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B27" s="1">
         <v>3.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B28" s="1">
         <v>7.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B29" s="1">
         <v>5.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B31" s="1">
         <v>5.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B32" s="1">
         <v>3.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B33" s="1">
         <v>5.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1">
         <v>2.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B35" s="1">
         <v>4.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B36" s="1">
         <v>3.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B37" s="1">
         <v>4.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>167</v>
@@ -1801,10 +1813,10 @@
         <v>2.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>169</v>
@@ -1818,10 +1830,10 @@
         <v>4.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>171</v>
@@ -1835,10 +1847,10 @@
         <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>173</v>
@@ -1852,10 +1864,10 @@
         <v>4.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>175</v>
@@ -1869,10 +1881,10 @@
         <v>3.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>177</v>
@@ -1887,10 +1899,10 @@
         <v>5.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>179</v>
@@ -1904,10 +1916,10 @@
         <v>2.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>181</v>
@@ -1921,10 +1933,10 @@
         <v>8.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>183</v>
@@ -1938,10 +1950,10 @@
         <v>5.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>185</v>
@@ -1955,10 +1967,10 @@
         <v>6.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>187</v>
@@ -1972,10 +1984,10 @@
         <v>5.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>189</v>
@@ -1989,10 +2001,10 @@
         <v>3.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>191</v>
@@ -2006,10 +2018,10 @@
         <v>6.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>193</v>
@@ -2023,10 +2035,10 @@
         <v>4.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>195</v>
@@ -2040,10 +2052,10 @@
         <v>4.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>197</v>
@@ -2057,10 +2069,10 @@
         <v>8.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>199</v>
@@ -2074,10 +2086,10 @@
         <v>7.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>201</v>
@@ -2091,10 +2103,10 @@
         <v>7.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>203</v>
@@ -2108,10 +2120,10 @@
         <v>4.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>205</v>
@@ -2125,10 +2137,10 @@
         <v>6.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>207</v>
@@ -2142,651 +2154,651 @@
         <v>4.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B59" s="1">
         <v>3.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B60" s="1">
         <v>3.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="B61" s="1">
         <v>7.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="B62" s="1">
         <v>3.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="B63" s="1">
         <v>4.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="B64" s="1">
         <v>3.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="B65" s="1">
         <v>3.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B66" s="1">
         <v>4.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B67" s="1">
         <v>4.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B68" s="1">
         <v>3.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="B69" s="1">
         <v>6.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="B70" s="1">
         <v>6.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B71" s="1">
         <v>0.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B72" s="1">
         <v>0.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B73" s="1">
         <v>0.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B74" s="1">
         <v>0.0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B75" s="1">
         <v>0.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B76" s="1">
         <v>0.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B77" s="1">
         <v>0.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B78" s="1">
         <v>0.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B79" s="1">
         <v>0.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B80" s="1">
         <v>0.0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B81" s="1">
         <v>0.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B82" s="1">
         <v>0.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B83" s="1">
         <v>0.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B84" s="1">
         <v>0.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B85" s="1">
         <v>0.0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B86" s="1">
         <v>0.0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B87" s="1">
         <v>0.0</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B88" s="1">
         <v>0.0</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B89" s="1">
         <v>0.0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B90" s="1">
         <v>0.0</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B91" s="1">
         <v>0.0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B92" s="1">
         <v>0.0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2812,230 +2824,230 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3055,23 +3067,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>7.0</v>
@@ -3081,10 +3093,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -3094,10 +3106,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
@@ -3106,10 +3118,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>7.0</v>
@@ -3118,10 +3130,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -3130,10 +3142,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -3142,10 +3154,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1">
         <v>6.0</v>
@@ -3154,10 +3166,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -3166,10 +3178,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1">
         <v>1.0</v>
@@ -3178,10 +3190,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>6.0</v>
@@ -3191,10 +3203,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>3.0</v>
@@ -3203,10 +3215,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
@@ -3215,10 +3227,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <v>7.0</v>
@@ -3227,10 +3239,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
         <v>2.0</v>
@@ -3239,10 +3251,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -3251,10 +3263,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1">
         <v>5.0</v>
@@ -3263,10 +3275,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1">
         <v>4.0</v>
@@ -3275,10 +3287,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1">
         <v>1.0</v>
@@ -3287,10 +3299,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20" s="1">
         <v>6.0</v>
@@ -3299,10 +3311,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1">
         <v>3.0</v>
@@ -3311,10 +3323,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1">
         <v>1.0</v>
@@ -3323,10 +3335,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
         <v>6.0</v>
@@ -3335,10 +3347,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
         <v>3.0</v>
@@ -3347,10 +3359,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -3359,10 +3371,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1">
         <v>9.0</v>
@@ -3371,10 +3383,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1">
         <v>0.0</v>
@@ -3383,10 +3395,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1">
         <v>1.0</v>
@@ -3395,10 +3407,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1">
         <v>6.0</v>
@@ -3407,10 +3419,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" s="1">
         <v>3.0</v>
@@ -3419,10 +3431,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1">
         <v>1.0</v>
@@ -3431,10 +3443,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C32" s="1">
         <v>6.0</v>
@@ -3443,10 +3455,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1">
         <v>3.0</v>
@@ -3454,10 +3466,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C34" s="1">
         <v>1.0</v>
@@ -3465,10 +3477,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C35" s="1">
         <v>6.0</v>
@@ -3476,10 +3488,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C36" s="1">
         <v>3.0</v>
@@ -3487,10 +3499,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C37" s="1">
         <v>1.0</v>
@@ -3498,10 +3510,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1">
         <v>7.0</v>
@@ -3509,10 +3521,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C39" s="1">
         <v>2.0</v>
@@ -3520,10 +3532,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1">
         <v>1.0</v>
@@ -3531,10 +3543,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C41" s="1">
         <v>7.0</v>
@@ -3542,10 +3554,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C42" s="1">
         <v>2.0</v>
@@ -3553,10 +3565,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C43" s="1">
         <v>1.0</v>
@@ -3564,10 +3576,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C44" s="1">
         <v>6.0</v>
@@ -3575,10 +3587,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1">
         <v>2.0</v>
@@ -3586,10 +3598,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C46" s="1">
         <v>2.0</v>
@@ -3597,10 +3609,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1">
         <v>5.0</v>
@@ -3608,10 +3620,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C48" s="1">
         <v>4.0</v>
@@ -3619,10 +3631,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C49" s="1">
         <v>1.0</v>
@@ -3630,10 +3642,10 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C50" s="1">
         <v>5.0</v>
@@ -3641,10 +3653,10 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C51" s="1">
         <v>4.0</v>
@@ -3652,10 +3664,10 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C52" s="1">
         <v>1.0</v>
@@ -3663,10 +3675,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C53" s="1">
         <v>8.0</v>
@@ -3674,10 +3686,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C54" s="1">
         <v>1.0</v>
@@ -3685,10 +3697,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C55" s="1">
         <v>1.0</v>
@@ -3696,10 +3708,10 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C56" s="1">
         <v>8.0</v>
@@ -3707,10 +3719,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C57" s="1">
         <v>1.0</v>
@@ -3718,10 +3730,10 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C58" s="1">
         <v>1.0</v>
@@ -3729,10 +3741,10 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C59" s="1">
         <v>8.0</v>
@@ -3740,10 +3752,10 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C60" s="1">
         <v>1.0</v>
@@ -3751,10 +3763,10 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C61" s="1">
         <v>1.0</v>
@@ -3784,131 +3796,131 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="B3" s="1">
         <v>3.0</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="B5" s="1">
         <v>7.0</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="B6" s="1">
         <v>5.0</v>
       </c>
       <c r="C6" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="B7" s="1">
         <v>6.0</v>
       </c>
       <c r="C7" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="B8" s="1">
         <v>7.0</v>
       </c>
       <c r="C8" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="B9" s="1">
         <v>5.0</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="B10" s="1">
         <v>2.0</v>
       </c>
       <c r="C10" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="B11" s="1">
         <v>3.0</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="B12" s="1">
         <v>7.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3927,25 +3939,40 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>245</v>
+        <v>301</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>247</v>
+        <v>303</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3965,73 +3992,73 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="R1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -4040,25 +4067,25 @@
         <v>10.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>204</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>180</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>190</v>
@@ -4067,24 +4094,24 @@
         <v>182</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -4093,25 +4120,25 @@
         <v>10.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>204</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>180</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>190</v>
@@ -4120,24 +4147,24 @@
         <v>182</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
@@ -4146,25 +4173,25 @@
         <v>8.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>204</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>180</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>190</v>
@@ -4173,24 +4200,24 @@
         <v>182</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -4199,51 +4226,51 @@
         <v>10.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>208</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>248</v>
+        <v>305</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -4252,34 +4279,34 @@
         <v>8.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>208</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>196</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change market card titles to "market card 1", etc.
</commit_message>
<xml_diff>
--- a/lib/seeds/Aeon's End Database.xlsx
+++ b/lib/seeds/Aeon's End Database.xlsx
@@ -22,76 +22,31 @@
     <t>Mage</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Card</t>
   </si>
   <si>
     <t>Quantity</t>
   </si>
   <si>
+    <t>Cost</t>
+  </si>
+  <si>
     <t>Adelheim</t>
+  </si>
+  <si>
+    <t>Image Name</t>
+  </si>
+  <si>
+    <t>Ability</t>
   </si>
   <si>
     <t>Crystal</t>
   </si>
   <si>
-    <t>Spark</t>
-  </si>
-  <si>
-    <t>Amethyst Shard</t>
-  </si>
-  <si>
-    <t>Brama</t>
-  </si>
-  <si>
-    <t>Buried Light</t>
-  </si>
-  <si>
-    <t>Dezmodia</t>
-  </si>
-  <si>
-    <t>Oblivion Shard</t>
-  </si>
-  <si>
-    <t>Garu</t>
-  </si>
-  <si>
-    <t>Torch</t>
-  </si>
-  <si>
-    <t>Gex</t>
-  </si>
-  <si>
-    <t>Shattered Geode</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Image Name</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Ability</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Amplify Vision</t>
-  </si>
-  <si>
     <t>Adelheim.jpg</t>
-  </si>
-  <si>
-    <t>Spell</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -99,10 +54,16 @@
 When a nemesis attack or power card is drawn but before it is resolved, you may discard it. It has no effect.</t>
   </si>
   <si>
-    <t>Market</t>
+    <t>Type</t>
   </si>
   <si>
-    <t>AmplifyVision.jpg</t>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>Brama</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
   <si>
     <t>Brama.jpg</t>
@@ -113,12 +74,27 @@
 Any player gains 4 life.</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Dezmodia</t>
+  </si>
+  <si>
     <t>Dezmodia.jpg</t>
+  </si>
+  <si>
+    <t>Amethyst Shard</t>
+  </si>
+  <si>
+    <t>Amplify Vision</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
 Activate during your main phase:
 Any player destroys an opened I or II breach and returns any spells to their hand. That player gains a Sigil breach and places it where the destroyed breach was. Then, that player may prep a spell from their hand to a breach.</t>
+  </si>
+  <si>
+    <t>Garu</t>
   </si>
   <si>
     <t>Garu.jpg</t>
@@ -130,7 +106,22 @@
 Deal 2 damage plus 4 additional damage for each spell you discarded divided however you choose to the nemesis or any number of minions</t>
   </si>
   <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>AmplifyVision.jpg</t>
+  </si>
+  <si>
+    <t>Gex</t>
+  </si>
+  <si>
     <t>Gex.jpg</t>
+  </si>
+  <si>
+    <t>Buried Light</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -165,10 +156,10 @@
     <t>Lash</t>
   </si>
   <si>
-    <t>Lash.jpg</t>
+    <t>Oblivion Shard</t>
   </si>
   <si>
-    <t>Arcane Nexus</t>
+    <t>Lash.jpg</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -179,13 +170,10 @@
     <t>Malastar</t>
   </si>
   <si>
-    <t>ArcaneNexus.jpg</t>
+    <t>Arcane Nexus</t>
   </si>
   <si>
     <t>Malastar.jpg</t>
-  </si>
-  <si>
-    <t>Aurora</t>
   </si>
   <si>
     <t>6 Charges.
@@ -196,16 +184,16 @@
     <t>Mazahaedron</t>
   </si>
   <si>
-    <t>Aurora.jpg</t>
-  </si>
-  <si>
-    <t>Banishing Topaz</t>
+    <t>ArcaneNexus.jpg</t>
   </si>
   <si>
     <t>Mazahaedron.jpg</t>
   </si>
   <si>
-    <t>Gem</t>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Aurora</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -214,16 +202,13 @@
 Gravehold gains 4 life.</t>
   </si>
   <si>
-    <t>BanishingTopaz.jpg</t>
-  </si>
-  <si>
     <t>Mist (Dagger Captain)</t>
   </si>
   <si>
     <t>Mist.jpg</t>
   </si>
   <si>
-    <t>Blasting Staff</t>
+    <t>Aurora.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -231,7 +216,7 @@
 Any ally draws 4 cards.</t>
   </si>
   <si>
-    <t>Relic</t>
+    <t>Banishing Topaz</t>
   </si>
   <si>
     <t>Mist (Voidwalker)</t>
@@ -240,10 +225,7 @@
     <t>MistWE.jpg</t>
   </si>
   <si>
-    <t>BlastingStaff.jpg</t>
-  </si>
-  <si>
-    <t>Blaze</t>
+    <t>Gem</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -254,13 +236,13 @@
     <t>Nym</t>
   </si>
   <si>
+    <t>BanishingTopaz.jpg</t>
+  </si>
+  <si>
     <t>Nym.jpg</t>
   </si>
   <si>
-    <t>Blaze.jpg</t>
-  </si>
-  <si>
-    <t>Bloodstone Jewel</t>
+    <t>Shattered Geode</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -269,13 +251,19 @@
 If you discarded an attack card, discard an additional card.</t>
   </si>
   <si>
+    <t>Blasting Staff</t>
+  </si>
+  <si>
+    <t>Relic</t>
+  </si>
+  <si>
     <t>Phaedraxa</t>
   </si>
   <si>
     <t>Phaedraxa.jpg</t>
   </si>
   <si>
-    <t>BloodstoneJewel.jpg</t>
+    <t>BlastingStaff.jpg</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -283,7 +271,7 @@
 Prevent any damage that the players or Gravehold would suffer during that turn.</t>
   </si>
   <si>
-    <t>Bottled Vortex</t>
+    <t>Blaze</t>
   </si>
   <si>
     <t>Quilius</t>
@@ -297,19 +285,16 @@
 Deal 2 damage for each Trophy token you have.</t>
   </si>
   <si>
-    <t>BottledVortex.jpg</t>
+    <t>Blaze.jpg</t>
   </si>
   <si>
     <t>Reeve</t>
   </si>
   <si>
-    <t>Breach Ore</t>
-  </si>
-  <si>
     <t>Reeve.jpg</t>
   </si>
   <si>
-    <t>Moonstone Shard</t>
+    <t>Bloodstone Jewel</t>
   </si>
   <si>
     <t>Cost: 4 Charges.
@@ -318,16 +303,13 @@
 Deal 3 damage to a different minion.</t>
   </si>
   <si>
+    <t>Moonstone Shard</t>
+  </si>
+  <si>
     <t>Ulgimor</t>
   </si>
   <si>
-    <t>BreachOre.jpg</t>
-  </si>
-  <si>
     <t>Ulgimor.jpg</t>
-  </si>
-  <si>
-    <t>Burning Opal</t>
   </si>
   <si>
     <t>Cost: 6 Charges.
@@ -339,10 +321,13 @@
     <t>Xaxos</t>
   </si>
   <si>
+    <t>BloodstoneJewel.jpg</t>
+  </si>
+  <si>
     <t>Xaxos.jpg</t>
   </si>
   <si>
-    <t>BurningOpal.jpg</t>
+    <t>Bottled Vortex</t>
   </si>
   <si>
     <t>Cost: 5 Charges.
@@ -351,7 +336,50 @@
 Reveal the turn order deck and return the revealed cards in any order.</t>
   </si>
   <si>
+    <t>Yan Magda</t>
+  </si>
+  <si>
+    <t>YanMagda.jpg</t>
+  </si>
+  <si>
+    <t>BottledVortex.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
+  </si>
+  <si>
+    <t>Z'hana</t>
+  </si>
+  <si>
+    <t>Breach Ore</t>
+  </si>
+  <si>
+    <t>Emerald Shard</t>
+  </si>
+  <si>
+    <t>Zhana.jpg</t>
+  </si>
+  <si>
+    <t>Cost: 5 Charges.
+Activate during your main phase:
+Gravehold gains 7 life.</t>
+  </si>
+  <si>
+    <t>BreachOre.jpg</t>
+  </si>
+  <si>
+    <t>Burning Opal</t>
+  </si>
+  <si>
+    <t>BurningOpal.jpg</t>
+  </si>
+  <si>
     <t>Cairn Compass</t>
+  </si>
+  <si>
+    <t>Quartz Shard</t>
   </si>
   <si>
     <t>CairnCompass.jpg</t>
@@ -366,56 +394,37 @@
     <t>Celestial Spire</t>
   </si>
   <si>
+    <t>Immolate</t>
+  </si>
+  <si>
     <t>CelestialSpire.jpg</t>
   </si>
   <si>
     <t>Chaos Arc</t>
   </si>
   <si>
-    <t>Yan Magda</t>
-  </si>
-  <si>
-    <t>Emerald Shard</t>
-  </si>
-  <si>
     <t>ChaosArc.jpg</t>
-  </si>
-  <si>
-    <t>YanMagda.jpg</t>
   </si>
   <si>
     <t>Clouded Sapphire</t>
   </si>
   <si>
-    <t>Cost: 5 Charges.
-Activate during your main phase:
-Gain a card from any supply pile. If you have four opened breaches, any ally gains a card from any supply pile and places it on top of their deck.</t>
+    <t>Worldheart Shard</t>
   </si>
   <si>
     <t>CloudedSapphire.jpg</t>
   </si>
   <si>
-    <t>Z'hana</t>
-  </si>
-  <si>
     <t>Combustion</t>
-  </si>
-  <si>
-    <t>Quartz Shard</t>
-  </si>
-  <si>
-    <t>Zhana.jpg</t>
-  </si>
-  <si>
-    <t>Cost: 5 Charges.
-Activate during your main phase:
-Gravehold gains 7 life.</t>
   </si>
   <si>
     <t>Combustion.jpg</t>
   </si>
   <si>
     <t>Conclave Scroll</t>
+  </si>
+  <si>
+    <t>Garnet Shard</t>
   </si>
   <si>
     <t>ConclaveScroll.jpg</t>
@@ -427,13 +436,13 @@
     <t>ConjureTheLost.jpg</t>
   </si>
   <si>
-    <t>Immolate</t>
-  </si>
-  <si>
     <t>Consuming Void</t>
   </si>
   <si>
     <t>ConsumingVoid.jpg</t>
+  </si>
+  <si>
+    <t>Amethyst Paragon</t>
   </si>
   <si>
     <t>Convection Field</t>
@@ -445,7 +454,7 @@
     <t>Crystallize</t>
   </si>
   <si>
-    <t>Worldheart Shard</t>
+    <t>Cinder</t>
   </si>
   <si>
     <t>Crystallize.jpg</t>
@@ -454,13 +463,13 @@
     <t>Dark Fire</t>
   </si>
   <si>
+    <t>Tourmaline Shard</t>
+  </si>
+  <si>
     <t>DarkFire.jpg</t>
   </si>
   <si>
     <t>Devouring Shadow</t>
-  </si>
-  <si>
-    <t>Garnet Shard</t>
   </si>
   <si>
     <t>DevouringShadow.jpg</t>
@@ -469,16 +478,19 @@
     <t>Diamond Cluster</t>
   </si>
   <si>
+    <t>Extinguish</t>
+  </si>
+  <si>
     <t>DiamondCluster.jpg</t>
   </si>
   <si>
     <t>Disintegrating Scythe</t>
   </si>
   <si>
-    <t>Amethyst Paragon</t>
+    <t>DisintegratingScythe.jpg</t>
   </si>
   <si>
-    <t>DisintegratingScythe.jpg</t>
+    <t>Obsidian Shard</t>
   </si>
   <si>
     <t>Dread Diamond</t>
@@ -490,10 +502,10 @@
     <t>Equilibrium</t>
   </si>
   <si>
-    <t>Cinder</t>
+    <t>Equilibrium.jpg</t>
   </si>
   <si>
-    <t>Equilibrium.jpg</t>
+    <t>Coal Shard</t>
   </si>
   <si>
     <t>Erratic Ingot</t>
@@ -505,10 +517,10 @@
     <t>Essence Theft</t>
   </si>
   <si>
-    <t>Tourmaline Shard</t>
+    <t>EssenceTheft.jpg</t>
   </si>
   <si>
-    <t>EssenceTheft.jpg</t>
+    <t>Flare</t>
   </si>
   <si>
     <t>Feral Lightning</t>
@@ -520,10 +532,10 @@
     <t>Fiend Catcher</t>
   </si>
   <si>
-    <t>Extinguish</t>
+    <t>FiendCatcher.jpg</t>
   </si>
   <si>
-    <t>FiendCatcher.jpg</t>
+    <t>Illuminate</t>
   </si>
   <si>
     <t>Fiery Torrent</t>
@@ -535,52 +547,112 @@
     <t>Flexing Dagger</t>
   </si>
   <si>
-    <t>Obsidian Shard</t>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Eternal Ember</t>
+  </si>
+  <si>
+    <t>Blight Lord</t>
+  </si>
+  <si>
+    <t>BlightLord.jpg</t>
   </si>
   <si>
     <t>FlexingDagger.jpg</t>
   </si>
   <si>
+    <t>Carapace Queen</t>
+  </si>
+  <si>
     <t>Focusing Orb</t>
+  </si>
+  <si>
+    <t>CarapaceQueen.jpg</t>
+  </si>
+  <si>
+    <t>Crooked Mask</t>
+  </si>
+  <si>
+    <t>CrookedMask.jpg</t>
   </si>
   <si>
     <t>FocusingOrb.jpg</t>
   </si>
   <si>
+    <t>Gate Witch</t>
+  </si>
+  <si>
     <t>Frozen Magmite</t>
   </si>
   <si>
-    <t>Coal Shard</t>
+    <t>GateWitch.jpg</t>
+  </si>
+  <si>
+    <t>Hollow Crown</t>
+  </si>
+  <si>
+    <t>HollowCrown.jpg</t>
   </si>
   <si>
     <t>FrozenMagmite.jpg</t>
   </si>
   <si>
+    <t>Horde Crone</t>
+  </si>
+  <si>
     <t>Ignite</t>
+  </si>
+  <si>
+    <t>HordeCrone.jpg</t>
+  </si>
+  <si>
+    <t>Magus Of Cloaks</t>
+  </si>
+  <si>
+    <t>MagusOfCloaks.jpg</t>
   </si>
   <si>
     <t>Ignite.jpg</t>
   </si>
   <si>
+    <t>Prince Of Gluttons</t>
+  </si>
+  <si>
+    <t>PrinceOfGluttons.jpg</t>
+  </si>
+  <si>
     <t>Jade</t>
+  </si>
+  <si>
+    <t>RageBorne</t>
+  </si>
+  <si>
+    <t>RageBorne.jpg</t>
   </si>
   <si>
     <t>Jade.jpg</t>
   </si>
   <si>
+    <t>Umbra Titan</t>
+  </si>
+  <si>
+    <t>UmbraTitan.jpg</t>
+  </si>
+  <si>
     <t>Jagged Lightning</t>
   </si>
   <si>
-    <t>Flare</t>
+    <t>Wayward One</t>
+  </si>
+  <si>
+    <t>WaywardOne.jpg</t>
   </si>
   <si>
     <t>JaggedLightning.jpg</t>
   </si>
   <si>
     <t>Kindle</t>
-  </si>
-  <si>
-    <t>Illuminate</t>
   </si>
   <si>
     <t>Kindle.jpg</t>
@@ -593,9 +665,6 @@
   </si>
   <si>
     <t>Leeching Agate</t>
-  </si>
-  <si>
-    <t>Eternal Ember</t>
   </si>
   <si>
     <t>LeechingAgate.jpg</t>
@@ -697,19 +766,43 @@
     <t>SearingRuby.jpg</t>
   </si>
   <si>
+    <t>Miriam</t>
+  </si>
+  <si>
     <t>Sifter's Pearl</t>
+  </si>
+  <si>
+    <t>Miriam.jpg</t>
+  </si>
+  <si>
+    <t>James</t>
   </si>
   <si>
     <t>SiftersPearl.jpg</t>
   </si>
   <si>
+    <t>James.jpg</t>
+  </si>
+  <si>
     <t>Spectral Echo</t>
+  </si>
+  <si>
+    <t>Kermit</t>
+  </si>
+  <si>
+    <t>Kermit.png</t>
   </si>
   <si>
     <t>SpectralEcho.jpg</t>
   </si>
   <si>
+    <t>Homura</t>
+  </si>
+  <si>
     <t>Temporal Helix</t>
+  </si>
+  <si>
+    <t>Homura.jpg</t>
   </si>
   <si>
     <t>TemporalHelix.jpg</t>
@@ -760,13 +853,37 @@
     <t>Vortex Gauntlet</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>VortexGauntlet.jpg</t>
+  </si>
+  <si>
+    <t>Player 1</t>
   </si>
   <si>
     <t>Wildfire Whip</t>
   </si>
   <si>
+    <t>Mage 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Mage 2</t>
+  </si>
+  <si>
+    <t>Won</t>
+  </si>
+  <si>
     <t>WildfireWhip.jpg</t>
+  </si>
+  <si>
+    <t>Nemesis</t>
+  </si>
+  <si>
+    <t>Market Card 1</t>
   </si>
   <si>
     <t>Unique</t>
@@ -800,32 +917,14 @@
 Cast: Gain 2 Aether.</t>
   </si>
   <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
-    <t>Blight Lord</t>
-  </si>
-  <si>
     <t>CoalShard.jpg</t>
-  </si>
-  <si>
-    <t>BlightLord.jpg</t>
   </si>
   <si>
     <t>If you have 2 life or less, destroy this.
 Otherwise, gain 3 Aether, gain 1 charge, and suffer 2 damage.</t>
   </si>
   <si>
-    <t>Carapace Queen</t>
-  </si>
-  <si>
-    <t>CarapaceQueen.jpg</t>
-  </si>
-  <si>
     <t>EmeraldShard.jpg</t>
-  </si>
-  <si>
-    <t>Crooked Mask</t>
   </si>
   <si>
     <t>Gain 1 Aether 
@@ -833,30 +932,12 @@
 Any player gains 1 life.</t>
   </si>
   <si>
-    <t>CrookedMask.jpg</t>
-  </si>
-  <si>
-    <t>Gate Witch</t>
-  </si>
-  <si>
-    <t>GateWitch.jpg</t>
-  </si>
-  <si>
     <t>EternalEmber.jpg</t>
-  </si>
-  <si>
-    <t>Hollow Crown</t>
   </si>
   <si>
     <t>Cast: Deal 1 damage.
 OR
 Cast: Cast one of your prepped spells without discarding it.</t>
-  </si>
-  <si>
-    <t>HollowCrown.jpg</t>
-  </si>
-  <si>
-    <t>Horde Crone</t>
   </si>
   <si>
     <t>Extinguish.jpg</t>
@@ -866,52 +947,37 @@
 If this damage causes a minion from the nemesis deck to be discarded, Quilius gains a Trophy token.</t>
   </si>
   <si>
-    <t>HordeCrone.jpg</t>
+    <t>Market Card 2</t>
   </si>
   <si>
-    <t>Magus Of Cloaks</t>
-  </si>
-  <si>
-    <t>Miriam</t>
-  </si>
-  <si>
-    <t>MagusOfCloaks.jpg</t>
-  </si>
-  <si>
-    <t>Miriam.jpg</t>
+    <t>Market Card 3</t>
   </si>
   <si>
     <t>Flare.jpg</t>
   </si>
   <si>
-    <t>Prince Of Gluttons</t>
-  </si>
-  <si>
-    <t>James</t>
+    <t>Market Card 4</t>
   </si>
   <si>
     <t>Cast: Reveal the top card of the turn order deck, and then place it back on top of the turn order deck. If you revealed a player turn order card, deal 3 damage. Otherwise deal 1 damage.</t>
   </si>
   <si>
-    <t>James.jpg</t>
+    <t>Market Card 5</t>
   </si>
   <si>
-    <t>PrinceOfGluttons.jpg</t>
+    <t>Market Card 6</t>
   </si>
   <si>
-    <t>Kermit</t>
+    <t>Market Card 7</t>
   </si>
   <si>
-    <t>Kermit.png</t>
+    <t>Market Card 8</t>
   </si>
   <si>
-    <t>RageBorne</t>
+    <t>Market Card 9</t>
   </si>
   <si>
     <t>GarnetShard.jpg</t>
-  </si>
-  <si>
-    <t>Homura</t>
   </si>
   <si>
     <t>Gain 1 Aether.
@@ -919,29 +985,11 @@
 Cast any player's prepped spell.</t>
   </si>
   <si>
-    <t>Homura.jpg</t>
-  </si>
-  <si>
-    <t>RageBorne.jpg</t>
-  </si>
-  <si>
-    <t>Umbra Titan</t>
-  </si>
-  <si>
-    <t>UmbraTitan.jpg</t>
-  </si>
-  <si>
     <t>Illuminate.jpg</t>
   </si>
   <si>
     <t>While prepped, when you focus or open one of your breaches during your turn, deal 1 damage.
 Cast: Deal 1 damage.</t>
-  </si>
-  <si>
-    <t>Wayward One</t>
-  </si>
-  <si>
-    <t>WaywardOne.jpg</t>
   </si>
   <si>
     <t>Immolate.jpg</t>
@@ -962,6 +1010,9 @@
   </si>
   <si>
     <t>Gain 2 Aether that cannot be used to gain a relic or spell.</t>
+  </si>
+  <si>
+    <t>2017/11/12 5:30PM PST</t>
   </si>
   <si>
     <t>ObsidianShard.jpg</t>
@@ -996,6 +1047,9 @@
     <t>TourmalineShard.jpg</t>
   </si>
   <si>
+    <t>2017/11/12 7:00PM PST</t>
+  </si>
+  <si>
     <t>Gain 1 Aether.
 Any ally may suffer 1 damage. If they do, they destroy a card in hand.</t>
   </si>
@@ -1008,6 +1062,9 @@
 Gain 2 Aether that can only be used to gain a card. Place the next card you gain this turn on top of any ally's discard pile.</t>
   </si>
   <si>
+    <t>2017/11/12 9:00PM PST</t>
+  </si>
+  <si>
     <t>Common</t>
   </si>
   <si>
@@ -1017,70 +1074,13 @@
     <t>Spark.jpg</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Player 1</t>
-  </si>
-  <si>
-    <t>Mage 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
-  </si>
-  <si>
-    <t>Mage 2</t>
-  </si>
-  <si>
-    <t>Won</t>
-  </si>
-  <si>
-    <t>Nemesis</t>
-  </si>
-  <si>
-    <t>Market Card Gem 1</t>
-  </si>
-  <si>
-    <t>Market Card Gem 2</t>
-  </si>
-  <si>
-    <t>Market Card Gem 3</t>
-  </si>
-  <si>
-    <t>Market Card Relic 1</t>
-  </si>
-  <si>
-    <t>Market Card Relic 2</t>
-  </si>
-  <si>
-    <t>Market Card Spell 1</t>
-  </si>
-  <si>
-    <t>Market Card Spell 2</t>
-  </si>
-  <si>
-    <t>Market Card Spell 3</t>
-  </si>
-  <si>
-    <t>Market Card Spell 4</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>2017/11/12 5:30PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/12 7:00PM PST</t>
-  </si>
-  <si>
-    <t>2017/11/12 9:00PM PST</t>
+    <t>2017/11/10 7:00PM PST</t>
   </si>
   <si>
     <t>Fri, 11/17/2017, 10:21 PM</t>
-  </si>
-  <si>
-    <t>2017/11/10 7:00PM PST</t>
   </si>
   <si>
     <t>2017/11/10 9:00PM PST</t>
@@ -1154,11 +1154,11 @@
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1220,39 +1220,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -1263,1588 +1263,1588 @@
         <v>7.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1">
         <v>4.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B8" s="1">
         <v>6.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1">
         <v>3.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="B10" s="1">
         <v>4.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1">
         <v>5.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B12" s="1">
         <v>4.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B13" s="1">
         <v>4.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B14" s="1">
         <v>5.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B15" s="1">
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B16" s="1">
         <v>6.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B17" s="1">
         <v>5.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1">
         <v>3.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B19" s="1">
         <v>6.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B20" s="1">
         <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B21" s="1">
         <v>5.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B22" s="1">
         <v>8.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B23" s="1">
         <v>5.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B24" s="1">
         <v>6.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B25" s="1">
         <v>4.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B26" s="1">
         <v>7.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1">
         <v>3.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B28" s="1">
         <v>7.0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B29" s="1">
         <v>5.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B30" s="1">
         <v>5.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B31" s="1">
         <v>5.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B32" s="1">
         <v>3.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B33" s="1">
         <v>5.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B34" s="1">
         <v>2.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B35" s="1">
         <v>4.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B36" s="1">
         <v>3.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="B37" s="1">
         <v>4.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="B38" s="1">
         <v>2.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B39" s="1">
         <v>4.0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="B40" s="1">
         <v>4.0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="B41" s="1">
         <v>4.0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="B42" s="1">
         <v>3.0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="B43" s="1">
         <v>5.0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="B44" s="1">
         <v>2.0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="B45" s="1">
         <v>8.0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="B46" s="1">
         <v>5.0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="B47" s="1">
         <v>6.0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>187</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="B48" s="1">
         <v>5.0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>189</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="B49" s="1">
         <v>3.0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="B50" s="1">
         <v>6.0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>193</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="B51" s="1">
         <v>4.0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="B52" s="1">
         <v>4.0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="B53" s="1">
         <v>8.0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="B54" s="1">
         <v>7.0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="B55" s="1">
         <v>7.0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="B56" s="1">
         <v>4.0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="B57" s="1">
         <v>6.0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="B58" s="1">
         <v>4.0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="B59" s="1">
         <v>3.0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="B60" s="1">
         <v>3.0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
       <c r="B61" s="1">
         <v>7.0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="B62" s="1">
         <v>3.0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>217</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="B63" s="1">
         <v>4.0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>219</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="B64" s="1">
         <v>3.0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="B65" s="1">
         <v>3.0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>223</v>
+        <v>254</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="B66" s="1">
         <v>4.0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="B67" s="1">
         <v>4.0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>227</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>228</v>
+        <v>259</v>
       </c>
       <c r="B68" s="1">
         <v>3.0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>229</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="B69" s="1">
         <v>6.0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="B70" s="1">
         <v>6.0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B71" s="1">
         <v>0.0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>236</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B72" s="1">
         <v>0.0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>237</v>
+        <v>276</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B73" s="1">
         <v>0.0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>239</v>
+        <v>278</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>240</v>
+        <v>279</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B74" s="1">
         <v>0.0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>241</v>
+        <v>280</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>242</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B75" s="1">
         <v>0.0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>245</v>
+        <v>282</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>247</v>
+        <v>283</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B76" s="1">
         <v>0.0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>250</v>
+        <v>284</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>252</v>
+        <v>285</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="B77" s="1">
         <v>0.0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>256</v>
+        <v>286</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B78" s="1">
         <v>0.0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>262</v>
+        <v>289</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B79" s="1">
         <v>0.0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B80" s="1">
         <v>0.0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B81" s="1">
         <v>0.0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B82" s="1">
         <v>0.0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1">
         <v>0.0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B84" s="1">
         <v>0.0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B85" s="1">
         <v>0.0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B86" s="1">
         <v>0.0</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="B87" s="1">
         <v>0.0</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B88" s="1">
         <v>0.0</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B89" s="1">
         <v>0.0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B90" s="1">
         <v>0.0</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B91" s="1">
         <v>0.0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B92" s="1">
         <v>0.0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -2867,233 +2867,233 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3116,20 +3116,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>7.0</v>
@@ -3139,10 +3139,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -3152,10 +3152,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
@@ -3164,10 +3164,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>7.0</v>
@@ -3176,10 +3176,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
         <v>6.0</v>
@@ -3212,10 +3212,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>3.0</v>
@@ -3224,10 +3224,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1">
         <v>1.0</v>
@@ -3236,10 +3236,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>6.0</v>
@@ -3249,10 +3249,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
         <v>3.0</v>
@@ -3261,10 +3261,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
@@ -3273,10 +3273,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1">
         <v>7.0</v>
@@ -3285,10 +3285,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
         <v>2.0</v>
@@ -3297,10 +3297,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -3309,10 +3309,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1">
         <v>5.0</v>
@@ -3321,10 +3321,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
         <v>4.0</v>
@@ -3333,10 +3333,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1">
         <v>1.0</v>
@@ -3345,10 +3345,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1">
         <v>6.0</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1">
         <v>3.0</v>
@@ -3369,10 +3369,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1">
         <v>1.0</v>
@@ -3381,10 +3381,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1">
         <v>6.0</v>
@@ -3393,10 +3393,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
         <v>3.0</v>
@@ -3405,10 +3405,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -3417,10 +3417,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1">
         <v>9.0</v>
@@ -3429,10 +3429,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1">
         <v>0.0</v>
@@ -3441,10 +3441,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C28" s="1">
         <v>1.0</v>
@@ -3453,10 +3453,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1">
         <v>6.0</v>
@@ -3465,10 +3465,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C30" s="1">
         <v>3.0</v>
@@ -3477,10 +3477,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C31" s="1">
         <v>1.0</v>
@@ -3489,10 +3489,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1">
         <v>6.0</v>
@@ -3501,10 +3501,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C33" s="1">
         <v>3.0</v>
@@ -3512,10 +3512,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C34" s="1">
         <v>1.0</v>
@@ -3523,10 +3523,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C35" s="1">
         <v>6.0</v>
@@ -3534,10 +3534,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C36" s="1">
         <v>3.0</v>
@@ -3545,10 +3545,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C37" s="1">
         <v>1.0</v>
@@ -3556,10 +3556,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C38" s="1">
         <v>7.0</v>
@@ -3567,10 +3567,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C39" s="1">
         <v>2.0</v>
@@ -3578,10 +3578,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C40" s="1">
         <v>1.0</v>
@@ -3589,10 +3589,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C41" s="1">
         <v>7.0</v>
@@ -3600,10 +3600,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C42" s="1">
         <v>2.0</v>
@@ -3611,10 +3611,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C43" s="1">
         <v>1.0</v>
@@ -3622,10 +3622,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C44" s="1">
         <v>6.0</v>
@@ -3633,10 +3633,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C45" s="1">
         <v>2.0</v>
@@ -3644,10 +3644,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C46" s="1">
         <v>2.0</v>
@@ -3655,10 +3655,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C47" s="1">
         <v>5.0</v>
@@ -3666,10 +3666,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C48" s="1">
         <v>4.0</v>
@@ -3677,10 +3677,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C49" s="1">
         <v>1.0</v>
@@ -3688,10 +3688,10 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C50" s="1">
         <v>5.0</v>
@@ -3699,10 +3699,10 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C51" s="1">
         <v>4.0</v>
@@ -3710,10 +3710,10 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C52" s="1">
         <v>1.0</v>
@@ -3721,10 +3721,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C53" s="1">
         <v>8.0</v>
@@ -3732,10 +3732,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C54" s="1">
         <v>1.0</v>
@@ -3743,10 +3743,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C55" s="1">
         <v>1.0</v>
@@ -3754,10 +3754,10 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C56" s="1">
         <v>8.0</v>
@@ -3765,10 +3765,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C57" s="1">
         <v>1.0</v>
@@ -3776,10 +3776,10 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C58" s="1">
         <v>1.0</v>
@@ -3787,10 +3787,10 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C59" s="1">
         <v>8.0</v>
@@ -3798,10 +3798,10 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C60" s="1">
         <v>1.0</v>
@@ -3809,10 +3809,10 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C61" s="1">
         <v>1.0</v>
@@ -3839,134 +3839,134 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>160</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>244</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>246</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>248</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1">
         <v>3.0</v>
       </c>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>251</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
       </c>
       <c r="C4" t="s">
-        <v>253</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>254</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1">
         <v>7.0</v>
       </c>
       <c r="C5" t="s">
-        <v>255</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="B6" s="1">
         <v>5.0</v>
       </c>
       <c r="C6" t="s">
-        <v>259</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>260</v>
+        <v>177</v>
       </c>
       <c r="B7" s="1">
         <v>6.0</v>
       </c>
       <c r="C7" t="s">
-        <v>263</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>264</v>
+        <v>180</v>
       </c>
       <c r="B8" s="1">
         <v>7.0</v>
       </c>
       <c r="C8" t="s">
-        <v>266</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>269</v>
+        <v>183</v>
       </c>
       <c r="B9" s="1">
         <v>5.0</v>
       </c>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>276</v>
+        <v>186</v>
       </c>
       <c r="B10" s="1">
         <v>2.0</v>
       </c>
       <c r="C10" t="s">
-        <v>281</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>282</v>
+        <v>189</v>
       </c>
       <c r="B11" s="1">
         <v>3.0</v>
       </c>
       <c r="C11" t="s">
-        <v>283</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>286</v>
+        <v>192</v>
       </c>
       <c r="B12" s="1">
         <v>7.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>287</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3983,42 +3983,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4038,73 +4038,73 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>309</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>310</v>
+        <v>264</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>311</v>
+        <v>266</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>312</v>
+        <v>267</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>313</v>
+        <v>268</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>314</v>
+        <v>269</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>243</v>
+        <v>160</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>315</v>
+        <v>271</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>316</v>
+        <v>272</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="R1" s="5"/>
+        <v>299</v>
+      </c>
+      <c r="R1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -4113,31 +4113,31 @@
         <v>10.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>44</v>
@@ -4145,19 +4145,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -4166,31 +4166,31 @@
         <v>10.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>44</v>
@@ -4198,19 +4198,19 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>1</v>
@@ -4219,31 +4219,31 @@
         <v>8.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>44</v>
@@ -4251,19 +4251,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F5" s="1" t="b">
         <v>0</v>
@@ -4272,34 +4272,34 @@
         <v>10.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>248</v>
+        <v>165</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6">
@@ -4307,16 +4307,16 @@
         <v>331</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1" t="b">
         <v>1</v>
@@ -4325,34 +4325,34 @@
         <v>8.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>248</v>
+        <v>165</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -4372,58 +4372,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>309</v>
+        <v>262</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>314</v>
+        <v>269</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>315</v>
+        <v>160</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>271</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>310</v>
+        <v>264</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>311</v>
+        <v>266</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>312</v>
+        <v>267</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>313</v>
+        <v>268</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>316</v>
+        <v>272</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B2" s="7" t="b">
         <v>1</v>
@@ -4450,46 +4450,46 @@
         <v>9.0</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>248</v>
+        <v>165</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>332</v>

</xml_diff>